<commit_message>
* add display excel test cases * add formula test cases
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="12" r:id="rId1"/>
@@ -1298,7 +1298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="401">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2500,19 +2500,7 @@
     <t>1001</t>
   </si>
   <si>
-    <t>DATEVALUE("2008/1/1")</t>
-  </si>
-  <si>
-    <t>SERIESSUM(B105,0,2,B106:B109)</t>
-  </si>
-  <si>
-    <t>AVERAGEIF(B12:E12,"&lt;23000")</t>
-  </si>
-  <si>
-    <t>AVERAGEIFS(B15:E15,B15:E15,"&lt;&gt;未完成",B15:E15,"&gt;80")</t>
-  </si>
-  <si>
-    <t>BAHTTEXT(1234)</t>
+    <t>END OF FORMULA</t>
   </si>
 </sst>
 </file>
@@ -2666,7 +2654,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2709,6 +2697,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2717,55 +2706,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3580,10 +3521,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3602,15 +3543,16 @@
       <c r="A2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" t="s">
-        <v>404</v>
+      <c r="B2" t="str">
+        <f>BAHTTEXT(1234)</f>
+        <v>หนึ่งพันสองร้อยสามสิบสี่บาทถ้วน</v>
       </c>
       <c r="C2" t="s">
         <v>391</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2=C2,"T","WARN")</f>
-        <v>WARN</v>
+        <v>T</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
@@ -3726,9 +3668,14 @@
         <v>T</v>
       </c>
     </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>400</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3741,8 +3688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I415"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3766,17 +3713,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -3822,7 +3769,7 @@
         <f>ACOS(-0.5)</f>
         <v>2.0943951023931957</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="38">
         <v>2.0943951023931957</v>
       </c>
       <c r="D7" t="str">
@@ -3845,6 +3792,10 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9" t="str">
+        <f>IF(B9=C9,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="1"/>
@@ -3857,7 +3808,7 @@
         <f>ASIN(-0.5)</f>
         <v>-0.52359877559829893</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="11">
         <v>-0.52359877559829893</v>
       </c>
       <c r="D11" t="str">
@@ -3876,7 +3827,7 @@
         <f>ASINH(-2.5)</f>
         <v>-1.6472311463710965</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="25">
         <v>-1.6472311463710965</v>
       </c>
       <c r="D13" t="str">
@@ -3895,7 +3846,7 @@
         <f>ATAN(1)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="25">
         <v>0.78539816339744828</v>
       </c>
       <c r="D15" t="str">
@@ -3915,7 +3866,6 @@
         <v>0.78539816339744828</v>
       </c>
       <c r="C17" s="33">
-        <f>ATAN2(1, 1)</f>
         <v>0.78539816339744828</v>
       </c>
       <c r="D17" t="str">
@@ -3930,11 +3880,11 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="33">
         <f>ATANH(0.76159416)</f>
         <v>1.0000000096297197</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="25">
         <v>1.0000000096297197</v>
       </c>
       <c r="D19" t="str">
@@ -3991,7 +3941,7 @@
         <f>COS(1.047)</f>
         <v>0.50017107459707011</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="25">
         <v>0.50017107459707011</v>
       </c>
       <c r="D25" t="str">
@@ -4006,11 +3956,11 @@
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="33">
         <f>COSH(4)</f>
         <v>27.308232836016487</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="25">
         <v>27.308232836016487</v>
       </c>
       <c r="D27" t="str">
@@ -4063,11 +4013,11 @@
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="25">
         <f>EXP(1)</f>
         <v>2.7182818284590451</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="25">
         <v>2.7182818284590451</v>
       </c>
       <c r="D33" t="str">
@@ -4200,7 +4150,7 @@
         <f>LN(86)</f>
         <v>4.4543472962535073</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="11">
         <v>4.4543472962535073</v>
       </c>
       <c r="D47" t="str">
@@ -4458,13 +4408,13 @@
       <c r="C73">
         <v>9</v>
       </c>
+      <c r="D73" t="str">
+        <f>IF(B74=C74,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="15.75">
       <c r="A74" s="1"/>
-      <c r="D74" t="str">
-        <f>IF(B74=C74,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="75" spans="1:4" ht="15.75">
       <c r="A75" s="1" t="s">
@@ -4496,6 +4446,10 @@
       <c r="C77">
         <v>3</v>
       </c>
+      <c r="D77" t="str">
+        <f>IF(B77=C77,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="15.75">
       <c r="A78" s="1"/>
@@ -4508,7 +4462,7 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="11">
         <v>3.1415926535897931</v>
       </c>
       <c r="D79" t="str">
@@ -4602,7 +4556,7 @@
         <f>RADIANS(270)</f>
         <v>4.7123889803846897</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="11">
         <v>4.7123889803846897</v>
       </c>
       <c r="D90" t="str">
@@ -4619,7 +4573,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>83.5908967757737</v>
+        <v>74.806499213694892</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -4637,7 +4591,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -4729,15 +4683,16 @@
       <c r="A104" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="C104">
+      <c r="B104" s="8">
+        <f>SERIESSUM(B105,0,2,B106:B109)</f>
+        <v>0.70710321482284566</v>
+      </c>
+      <c r="C104" s="11">
         <v>0.70710321482284566</v>
       </c>
       <c r="D104" t="str">
         <f>IF(B104=C104,"T","WARN")</f>
-        <v>WARN</v>
+        <v>T</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75">
@@ -4823,7 +4778,7 @@
         <f>SINH(1)</f>
         <v>1.1752011936438014</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="11">
         <v>1.1752011936438014</v>
       </c>
       <c r="D115" t="str">
@@ -4861,7 +4816,7 @@
         <f>SQRTPI(1)</f>
         <v>1.7724538509055159</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="11">
         <v>1.7724538509055159</v>
       </c>
       <c r="D119" t="str">
@@ -5500,6 +5455,14 @@
       </c>
       <c r="C186" t="e">
         <v>#NAME?</v>
+      </c>
+      <c r="D186" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="415" spans="1:1">
@@ -5514,53 +5477,8 @@
   <mergeCells count="1">
     <mergeCell ref="A2:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31">
-    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33 D35 D37 D39 D41 D43 D45 D47">
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53 D51 D49">
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59 D63 D71 D74:D75">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59 D63 D71 D74:D75 D79 D81 D83 D88:D90">
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94">
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D117 D119 D121 D127 D129">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D135 D145 D150 D153">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D162 D171 D180">
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D182 D184 D186">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+  <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5576,8 +5494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5763,6 +5681,11 @@
     <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="1"/>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>400</v>
+      </c>
+    </row>
     <row r="248" spans="1:1">
       <c r="A248" s="3" t="s">
         <v>0</v>
@@ -5770,7 +5693,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5781,10 +5704,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D455"/>
+  <dimension ref="A1:D226"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6514,6 +6437,11 @@
       <c r="A76" s="1"/>
       <c r="C76" s="21"/>
     </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>400</v>
+      </c>
+    </row>
     <row r="81" spans="1:2">
       <c r="B81" s="11"/>
     </row>
@@ -6963,18 +6891,13 @@
     </row>
     <row r="226" spans="1:1" ht="15.75">
       <c r="A226" s="1"/>
-    </row>
-    <row r="455" spans="1:1">
-      <c r="A455" s="3" t="s">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <sortState ref="A5:A26">
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D75">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6988,8 +6911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J451"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7407,8 +7330,10 @@
     <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75">
-      <c r="A46" s="1"/>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="1"/>
@@ -7963,17 +7888,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7986,8 +7911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D458"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8049,15 +7974,16 @@
       <c r="A6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B6" t="s">
-        <v>400</v>
+      <c r="B6">
+        <f>DATEVALUE("2008/1/1")</f>
+        <v>39448</v>
       </c>
       <c r="C6">
         <v>39448</v>
       </c>
       <c r="D6" t="str">
         <f>IF(B6=C6,"T","WARN")</f>
-        <v>WARN</v>
+        <v>T</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
@@ -8195,7 +8121,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41394.677521990743</v>
+        <v>41396.762319212961</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -8264,7 +8190,7 @@
       </c>
       <c r="B29" s="22">
         <f ca="1">TODAY()</f>
-        <v>41394</v>
+        <v>41396</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -8346,8 +8272,10 @@
     <row r="38" spans="1:4" ht="15.75">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75">
-      <c r="A39" s="1"/>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>400</v>
+      </c>
       <c r="C39" s="21"/>
     </row>
     <row r="40" spans="1:4" ht="15.75">
@@ -8940,22 +8868,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8969,8 +8897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I534"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10414,8 +10342,10 @@
     <row r="124" spans="1:7" ht="15.75">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75">
-      <c r="A125" s="1"/>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="1"/>
@@ -10978,32 +10908,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11017,8 +10947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11163,15 +11093,16 @@
       <c r="A11" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B11" t="s">
-        <v>402</v>
+      <c r="B11">
+        <f>AVERAGEIF(B12:E12,"&lt;23000")</f>
+        <v>14000</v>
       </c>
       <c r="C11">
         <v>14000</v>
       </c>
       <c r="D11" t="str">
         <f>IF(B11=C11,"T","WARN")</f>
-        <v>WARN</v>
+        <v>T</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75">
@@ -11198,15 +11129,16 @@
       <c r="A14" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B14" t="s">
-        <v>403</v>
+      <c r="B14">
+        <f>AVERAGEIFS(B15:E15,B15:E15,"&lt;&gt;未完成",B15:E15,"&gt;80")</f>
+        <v>87.5</v>
       </c>
       <c r="C14">
         <v>87.5</v>
       </c>
       <c r="D14" t="str">
         <f>IF(B14=C14,"T","WARN")</f>
-        <v>WARN</v>
+        <v>T</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75">
@@ -13854,8 +13786,10 @@
     <row r="201" spans="1:11" ht="15.75">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:11" ht="15.75">
-      <c r="A202" s="1"/>
+    <row r="202" spans="1:11">
+      <c r="A202" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="203" spans="1:11" ht="15.75">
       <c r="A203" s="1"/>
@@ -14444,67 +14378,67 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D14 D17 D19 D21 D23 D25 D27">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14518,8 +14452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15339,8 +15273,10 @@
       <c r="A78" s="1"/>
       <c r="B78" s="24"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75">
-      <c r="A79" s="1"/>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>400</v>
+      </c>
       <c r="B79" s="24"/>
     </row>
     <row r="80" spans="1:4" ht="15.75">
@@ -15939,37 +15875,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
* use hamcrest-library to compare double (isCloseTo()) * refine formula test to be more complete
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="12" r:id="rId1"/>
@@ -62,31 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C64" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Hawk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-empty text</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A75" authorId="0">
+    <comment ref="A73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1298,7 +1274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="400">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2471,9 +2447,6 @@
   </si>
   <si>
     <t>DateTime</t>
-  </si>
-  <si>
-    <t>หนึ่งพันสองร้อยสามสิบสี่บาทถ้วน</t>
   </si>
   <si>
     <t>EXCEL</t>
@@ -2507,7 +2480,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="8" formatCode="&quot;NT$&quot;#,##0.00;[Red]\-&quot;NT$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2516,7 +2489,6 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0_ ;[Red]\-0\ "/>
     <numFmt numFmtId="170" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -2654,7 +2626,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2691,7 +2663,6 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2706,67 +2677,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3523,8 +3434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3547,22 +3458,22 @@
         <f>BAHTTEXT(1234)</f>
         <v>หนึ่งพันสองร้อยสามสิบสี่บาทถ้วน</v>
       </c>
-      <c r="C2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D2" t="str">
+      <c r="C2" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="D2" t="e">
         <f>IF(B2=C2,"T","WARN")</f>
-        <v>T</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>125</v>
       </c>
       <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>388</v>
       </c>
       <c r="B4" s="11"/>
@@ -3649,12 +3560,12 @@
     </row>
     <row r="22" spans="1:4" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B23" t="e">
         <f ca="1">abc()</f>
@@ -3670,12 +3581,12 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3688,8 +3599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3713,17 +3624,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -3769,7 +3680,7 @@
         <f>ACOS(-0.5)</f>
         <v>2.0943951023931957</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="37">
         <v>2.0943951023931957</v>
       </c>
       <c r="D7" t="str">
@@ -3937,7 +3848,7 @@
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="33">
         <f>COS(1.047)</f>
         <v>0.50017107459707011</v>
       </c>
@@ -4161,7 +4072,7 @@
     <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75">
+    <row r="49" spans="1:5" ht="15.75">
       <c r="A49" s="1" t="s">
         <v>25</v>
       </c>
@@ -4177,10 +4088,10 @@
         <v>T</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75">
+    <row r="50" spans="1:5" ht="15.75">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75">
+    <row r="51" spans="1:5" ht="15.75">
       <c r="A51" s="1" t="s">
         <v>26</v>
       </c>
@@ -4196,15 +4107,15 @@
         <v>T</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75">
+    <row r="52" spans="1:5" ht="15.75">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75">
+    <row r="53" spans="1:5" ht="15.75">
       <c r="A53" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B53">
-        <f>MDETERM(A54:D57)</f>
+        <f>MDETERM(B54:E57)</f>
         <v>87.999999999999972</v>
       </c>
       <c r="C53">
@@ -4215,38 +4126,35 @@
         <v>T</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54">
+    <row r="54" spans="1:5">
+      <c r="B54">
         <v>1</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>3</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>8</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55">
+    <row r="55" spans="1:5">
+      <c r="B55">
         <v>1</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>3</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>6</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56">
-        <v>1</v>
-      </c>
+    <row r="56" spans="1:5">
       <c r="B56">
         <v>1</v>
       </c>
@@ -4254,27 +4162,30 @@
         <v>1</v>
       </c>
       <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57">
+    <row r="57" spans="1:5">
+      <c r="B57">
         <v>7</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>3</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>10</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75">
+    <row r="58" spans="1:5" ht="15.75">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75">
+    <row r="59" spans="1:5" ht="15.75">
       <c r="A59" s="1" t="s">
         <v>28</v>
       </c>
@@ -4290,7 +4201,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75">
+    <row r="60" spans="1:5" ht="15.75">
       <c r="A60" s="1"/>
       <c r="B60">
         <v>4</v>
@@ -4299,7 +4210,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75">
+    <row r="61" spans="1:5" ht="15.75">
       <c r="A61" s="1"/>
       <c r="B61">
         <v>2</v>
@@ -4308,10 +4219,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75">
+    <row r="62" spans="1:5" ht="15.75">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75">
+    <row r="63" spans="1:5" ht="15.75">
       <c r="A63" s="1" t="s">
         <v>29</v>
       </c>
@@ -4327,7 +4238,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75">
+    <row r="64" spans="1:5" ht="15.75">
       <c r="A64" s="1"/>
       <c r="B64" t="s">
         <v>66</v>
@@ -4573,13 +4484,13 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>74.806499213694892</v>
+        <v>46.676197475810355</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
       </c>
       <c r="D92" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75">
@@ -4591,13 +4502,13 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
       </c>
       <c r="D94" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75">
@@ -5457,12 +5368,12 @@
         <v>#NAME?</v>
       </c>
       <c r="D186" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="415" spans="1:1">
@@ -5478,7 +5389,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5494,8 +5405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I248"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5683,7 +5594,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="248" spans="1:1">
@@ -5693,7 +5604,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5704,10 +5615,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D226"/>
+  <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5743,7 +5654,7 @@
         <v>EXCEL</v>
       </c>
       <c r="C3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D3" t="str">
         <f>IF(B3=C3,"T","WARN")</f>
@@ -5852,7 +5763,7 @@
         <v>NT$1,234.57</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D14" t="str">
         <f>IF(B14=C14,"T","WARN")</f>
@@ -5946,7 +5857,7 @@
         <v>1,234.6</v>
       </c>
       <c r="C24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D24" t="str">
         <f>IF(B24=C24,"T","WARN")</f>
@@ -6326,47 +6237,47 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75">
-      <c r="A64" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B64" s="5" t="str">
-        <f>T(B65)</f>
-        <v/>
-      </c>
-      <c r="D64" t="str">
-        <f>IF(B64=C64,"T","WARN")</f>
-        <v>T</v>
-      </c>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:4" ht="15.75">
-      <c r="A65" s="1"/>
-      <c r="B65">
-        <v>19</v>
+      <c r="A65" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" t="str">
+        <f>"Date: " &amp; TEXT(B66,"yyyy-mm-dd")</f>
+        <v>Date: 2007-08-06</v>
+      </c>
+      <c r="C65" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" t="str">
+        <f>IF(B65=C65,"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="1"/>
+      <c r="B66">
+        <v>39300.625</v>
+      </c>
     </row>
     <row r="67" spans="1:4" ht="15.75">
-      <c r="A67" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" t="str">
-        <f>"Date: " &amp; TEXT(B68,"yyyy-mm-dd")</f>
-        <v>Date: 2007-08-06</v>
-      </c>
-      <c r="C67" t="s">
-        <v>138</v>
-      </c>
-      <c r="D67" t="str">
-        <f>IF(B67=C67,"T","WARN")</f>
-        <v>T</v>
-      </c>
+      <c r="A67" s="1"/>
     </row>
     <row r="68" spans="1:4" ht="15.75">
-      <c r="A68" s="1"/>
-      <c r="B68">
-        <v>39300.625</v>
+      <c r="A68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" t="str">
+        <f>TRIM(" revenue in quarter 1 ")</f>
+        <v>revenue in quarter 1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" t="str">
+        <f>IF(B68=C68,"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75">
@@ -6374,14 +6285,14 @@
     </row>
     <row r="70" spans="1:4" ht="15.75">
       <c r="A70" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B70" t="str">
-        <f>TRIM(" revenue in quarter 1 ")</f>
-        <v>revenue in quarter 1</v>
+        <f>UPPER(B71)</f>
+        <v>TOTAL</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D70" t="str">
         <f>IF(B70=C70,"T","WARN")</f>
@@ -6390,60 +6301,48 @@
     </row>
     <row r="71" spans="1:4" ht="15.75">
       <c r="A71" s="1"/>
+      <c r="B71" s="5" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="15.75">
-      <c r="A72" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" t="str">
-        <f>UPPER(B73)</f>
-        <v>TOTAL</v>
-      </c>
-      <c r="C72" t="s">
-        <v>141</v>
-      </c>
-      <c r="D72" t="str">
-        <f>IF(B72=C72,"T","WARN")</f>
-        <v>T</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="1:4" ht="15.75">
-      <c r="A73" s="1"/>
-      <c r="B73" s="5" t="s">
-        <v>140</v>
+      <c r="A73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73">
+        <f>VALUE("16:48:00")</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="C73">
+        <v>0.7</v>
+      </c>
+      <c r="D73" t="str">
+        <f>IF(B73=C73,"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75">
       <c r="A74" s="1"/>
-      <c r="B74" s="5"/>
-    </row>
-    <row r="75" spans="1:4" ht="15.75">
-      <c r="A75" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B75">
-        <f>VALUE("16:48:00")</f>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="C75">
-        <v>0.7</v>
-      </c>
-      <c r="D75" t="str">
-        <f>IF(B75=C75,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75">
-      <c r="A76" s="1"/>
-      <c r="C76" s="21"/>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="B81" s="11"/>
+      <c r="C74" s="21"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="B79" s="11"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.75">
+      <c r="A81" s="1"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" ht="15.75">
       <c r="A82" s="1"/>
@@ -6457,21 +6356,20 @@
     </row>
     <row r="85" spans="1:2" ht="15.75">
       <c r="A85" s="1"/>
-      <c r="B85" s="5"/>
+      <c r="B85" s="8"/>
     </row>
     <row r="86" spans="1:2" ht="15.75">
       <c r="A86" s="1"/>
     </row>
     <row r="87" spans="1:2" ht="15.75">
       <c r="A87" s="1"/>
-      <c r="B87" s="8"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" ht="15.75">
       <c r="A88" s="1"/>
     </row>
     <row r="89" spans="1:2" ht="15.75">
       <c r="A89" s="1"/>
-      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" ht="15.75">
       <c r="A90" s="1"/>
@@ -6479,11 +6377,11 @@
     <row r="91" spans="1:2" ht="15.75">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:2" ht="15.75">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.75">
-      <c r="A93" s="1"/>
+    <row r="96" spans="1:2" ht="15.75">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.75">
+      <c r="A97" s="1"/>
     </row>
     <row r="98" spans="1:2" ht="15.75">
       <c r="A98" s="1"/>
@@ -6520,6 +6418,7 @@
     </row>
     <row r="109" spans="1:2" ht="15.75">
       <c r="A109" s="1"/>
+      <c r="B109" s="5"/>
     </row>
     <row r="110" spans="1:2" ht="15.75">
       <c r="A110" s="1"/>
@@ -6547,14 +6446,14 @@
     </row>
     <row r="117" spans="1:2" ht="15.75">
       <c r="A117" s="1"/>
-      <c r="B117" s="5"/>
+      <c r="B117" s="8"/>
     </row>
     <row r="118" spans="1:2" ht="15.75">
       <c r="A118" s="1"/>
     </row>
     <row r="119" spans="1:2" ht="15.75">
       <c r="A119" s="1"/>
-      <c r="B119" s="8"/>
+      <c r="B119" s="5"/>
     </row>
     <row r="120" spans="1:2" ht="15.75">
       <c r="A120" s="1"/>
@@ -6568,7 +6467,6 @@
     </row>
     <row r="123" spans="1:2" ht="15.75">
       <c r="A123" s="1"/>
-      <c r="B123" s="5"/>
     </row>
     <row r="124" spans="1:2" ht="15.75">
       <c r="A124" s="1"/>
@@ -6578,33 +6476,34 @@
     </row>
     <row r="126" spans="1:2" ht="15.75">
       <c r="A126" s="1"/>
+      <c r="B126" s="5"/>
     </row>
     <row r="127" spans="1:2" ht="15.75">
       <c r="A127" s="1"/>
     </row>
     <row r="128" spans="1:2" ht="15.75">
       <c r="A128" s="1"/>
-      <c r="B128" s="5"/>
+      <c r="B128" s="11"/>
     </row>
     <row r="129" spans="1:2" ht="15.75">
       <c r="A129" s="1"/>
     </row>
     <row r="130" spans="1:2" ht="15.75">
       <c r="A130" s="1"/>
-      <c r="B130" s="11"/>
+      <c r="B130" s="9"/>
     </row>
     <row r="131" spans="1:2" ht="15.75">
       <c r="A131" s="1"/>
     </row>
     <row r="132" spans="1:2" ht="15.75">
       <c r="A132" s="1"/>
-      <c r="B132" s="9"/>
     </row>
     <row r="133" spans="1:2" ht="15.75">
       <c r="A133" s="1"/>
     </row>
     <row r="134" spans="1:2" ht="15.75">
       <c r="A134" s="1"/>
+      <c r="B134" s="5"/>
     </row>
     <row r="135" spans="1:2" ht="15.75">
       <c r="A135" s="1"/>
@@ -6618,7 +6517,6 @@
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="1"/>
-      <c r="B138" s="5"/>
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="1"/>
@@ -6631,13 +6529,13 @@
     </row>
     <row r="142" spans="1:2" ht="15.75">
       <c r="A142" s="1"/>
+      <c r="B142" s="8"/>
     </row>
     <row r="143" spans="1:2" ht="15.75">
       <c r="A143" s="1"/>
     </row>
     <row r="144" spans="1:2" ht="15.75">
       <c r="A144" s="1"/>
-      <c r="B144" s="8"/>
     </row>
     <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="1"/>
@@ -6659,34 +6557,34 @@
     </row>
     <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
+      <c r="B151" s="12"/>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
     </row>
     <row r="153" spans="1:2" ht="15.75">
       <c r="A153" s="1"/>
-      <c r="B153" s="12"/>
+      <c r="B153" s="8"/>
     </row>
     <row r="154" spans="1:2" ht="15.75">
       <c r="A154" s="1"/>
     </row>
     <row r="155" spans="1:2" ht="15.75">
       <c r="A155" s="1"/>
-      <c r="B155" s="8"/>
+      <c r="B155" s="5"/>
     </row>
     <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="1"/>
     </row>
     <row r="157" spans="1:2" ht="15.75">
       <c r="A157" s="1"/>
-      <c r="B157" s="5"/>
+      <c r="B157" s="11"/>
     </row>
     <row r="158" spans="1:2" ht="15.75">
       <c r="A158" s="1"/>
     </row>
     <row r="159" spans="1:2" ht="15.75">
       <c r="A159" s="1"/>
-      <c r="B159" s="11"/>
     </row>
     <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="1"/>
@@ -6774,67 +6672,67 @@
     </row>
     <row r="188" spans="1:2" ht="15.75">
       <c r="A188" s="1"/>
+      <c r="B188" s="5"/>
     </row>
     <row r="189" spans="1:2" ht="15.75">
       <c r="A189" s="1"/>
     </row>
     <row r="190" spans="1:2" ht="15.75">
       <c r="A190" s="1"/>
-      <c r="B190" s="5"/>
     </row>
     <row r="191" spans="1:2" ht="15.75">
       <c r="A191" s="1"/>
+      <c r="B191" s="5"/>
     </row>
     <row r="192" spans="1:2" ht="15.75">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:2" ht="15.75">
+    <row r="193" spans="1:1" ht="15.75">
       <c r="A193" s="1"/>
-      <c r="B193" s="5"/>
-    </row>
-    <row r="194" spans="1:2" ht="15.75">
+    </row>
+    <row r="194" spans="1:1" ht="15.75">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:2" ht="15.75">
+    <row r="195" spans="1:1" ht="15.75">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:2" ht="15.75">
+    <row r="196" spans="1:1" ht="15.75">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:2" ht="15.75">
+    <row r="197" spans="1:1" ht="15.75">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:2" ht="15.75">
+    <row r="198" spans="1:1" ht="15.75">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:2" ht="15.75">
+    <row r="199" spans="1:1" ht="15.75">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:2" ht="15.75">
+    <row r="200" spans="1:1" ht="15.75">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" spans="1:2" ht="15.75">
+    <row r="201" spans="1:1" ht="15.75">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:2" ht="15.75">
+    <row r="202" spans="1:1" ht="15.75">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" spans="1:2" ht="15.75">
+    <row r="203" spans="1:1" ht="15.75">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" spans="1:2" ht="15.75">
+    <row r="204" spans="1:1" ht="15.75">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" spans="1:2" ht="15.75">
+    <row r="205" spans="1:1" ht="15.75">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" spans="1:2" ht="15.75">
+    <row r="206" spans="1:1" ht="15.75">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" spans="1:2" ht="15.75">
+    <row r="207" spans="1:1" ht="15.75">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" spans="1:2" ht="15.75">
+    <row r="208" spans="1:1" ht="15.75">
       <c r="A208" s="1"/>
     </row>
     <row r="209" spans="1:2" ht="15.75">
@@ -6866,6 +6764,7 @@
     </row>
     <row r="218" spans="1:2" ht="15.75">
       <c r="A218" s="1"/>
+      <c r="B218" s="11"/>
     </row>
     <row r="219" spans="1:2" ht="15.75">
       <c r="A219" s="1"/>
@@ -6876,28 +6775,21 @@
     </row>
     <row r="221" spans="1:2" ht="15.75">
       <c r="A221" s="1"/>
+      <c r="B221" s="11"/>
     </row>
     <row r="222" spans="1:2" ht="15.75">
       <c r="A222" s="1"/>
-      <c r="B222" s="11"/>
-    </row>
-    <row r="223" spans="1:2" ht="15.75">
-      <c r="A223" s="1"/>
-      <c r="B223" s="11"/>
+      <c r="B222" s="5"/>
     </row>
     <row r="224" spans="1:2" ht="15.75">
       <c r="A224" s="1"/>
-      <c r="B224" s="5"/>
-    </row>
-    <row r="226" spans="1:1" ht="15.75">
-      <c r="A226" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A5:A26">
     <sortCondition ref="A5"/>
   </sortState>
-  <conditionalFormatting sqref="D3:D75">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+  <conditionalFormatting sqref="D3:D73">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6990,7 +6882,7 @@
         <v>12.0</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D8" t="str">
         <f ca="1">IF(B8=C8,"T","WARN")</f>
@@ -7299,7 +7191,7 @@
         <v>#N/A</v>
       </c>
       <c r="D41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75">
@@ -7332,7 +7224,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75">
@@ -7888,17 +7780,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8121,7 +8013,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41396.762319212961</v>
+        <v>41397.626794791664</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -8190,7 +8082,7 @@
       </c>
       <c r="B29" s="22">
         <f ca="1">TODAY()</f>
-        <v>41396</v>
+        <v>41397</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -8274,7 +8166,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C39" s="21"/>
     </row>
@@ -8868,22 +8760,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8897,8 +8789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I534"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10140,7 +10032,7 @@
       <c r="A107" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B107" s="26">
+      <c r="B107" s="27">
         <f>SYD(30000,7500,10,1)</f>
         <v>4090.909090909091</v>
       </c>
@@ -10344,7 +10236,7 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75">
@@ -10908,32 +10800,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10947,8 +10839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10967,7 +10859,7 @@
       <c r="A1" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -11205,7 +11097,7 @@
         <f>BINOMDIST(6,10,0.5,FALSE)</f>
         <v>0.20507812500000006</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="25">
         <v>0.20507812500000006</v>
       </c>
       <c r="D21" t="str">
@@ -11225,7 +11117,7 @@
         <f>CHIDIST(18.307,10)</f>
         <v>5.0000589099658876E-2</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="25">
         <v>5.0000589099658876E-2</v>
       </c>
       <c r="D23" t="str">
@@ -11244,7 +11136,7 @@
         <f>CHIINV(0.05,10)</f>
         <v>18.307038053808746</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="25">
         <v>18.307038053808746</v>
       </c>
       <c r="D25" t="str">
@@ -11264,7 +11156,7 @@
         <f>CHITEST(B28:C30,B31:C33)</f>
         <v>3.081920170211661E-4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="32">
         <v>3.081920170211661E-4</v>
       </c>
       <c r="D27" t="str">
@@ -11337,7 +11229,7 @@
         <f>CONFIDENCE(0.05,2.5,50)</f>
         <v>0.69295191217483887</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="25">
         <v>0.69295191217483887</v>
       </c>
       <c r="D35" t="str">
@@ -11353,11 +11245,11 @@
       <c r="A37" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B37" s="34">
+      <c r="B37" s="11">
         <f>CORREL(B38:F38,B39:F39)</f>
         <v>0.99705448550158138</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="11">
         <v>0.99705448550158138</v>
       </c>
       <c r="D37" t="str">
@@ -11655,7 +11547,7 @@
         <f>EXPONDIST(0.2,10, TRUE)</f>
         <v>0.8646647167633873</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="25">
         <v>0.8646647167633873</v>
       </c>
       <c r="D57" t="str">
@@ -11674,7 +11566,7 @@
         <f>FDIST(15.2068,6,4)</f>
         <v>1.0000079377937579E-2</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="25">
         <v>1.0000079377937579E-2</v>
       </c>
       <c r="D59" t="str">
@@ -11693,7 +11585,7 @@
         <f>FINV(0.01,6,4)</f>
         <v>15.20686486148989</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="25">
         <v>15.20686486148989</v>
       </c>
       <c r="D61" t="str">
@@ -11712,7 +11604,7 @@
         <f>FISHER(0.75)</f>
         <v>0.97295507452765662</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="25">
         <v>0.97295507452765662</v>
       </c>
       <c r="D63" t="str">
@@ -11731,7 +11623,7 @@
         <f>FISHERINV(0.972955)</f>
         <v>0.74999996739414843</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="25">
         <v>0.74999996739414843</v>
       </c>
       <c r="D65" t="str">
@@ -11860,7 +11752,7 @@
         <f>FTEST(B74:F74,B75:F75)</f>
         <v>0.64831784680276039</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="25">
         <v>0.64831784680276039</v>
       </c>
       <c r="D73" t="str">
@@ -11912,7 +11804,7 @@
         <f>GAMMADIST(10, 9,2, FALSE)</f>
         <v>3.2639019680753736E-2</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="25">
         <v>3.2639019680753736E-2</v>
       </c>
       <c r="D76" t="str">
@@ -11950,7 +11842,7 @@
         <f>GAMMALN(4)</f>
         <v>1.7917594690821024</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="25">
         <v>1.7917594690821024</v>
       </c>
       <c r="D80" t="str">
@@ -11969,7 +11861,7 @@
         <f>GEOMEAN(B83:H83)</f>
         <v>5.4769869696569611</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="25">
         <v>5.4769869696569611</v>
       </c>
       <c r="D82" t="str">
@@ -12012,7 +11904,7 @@
         <f>GROWTH(B87:G87,B86:G86,H86:I86)</f>
         <v>320196.71836347238</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="25">
         <v>320196.71836347238</v>
       </c>
       <c r="D85" t="str">
@@ -12079,7 +11971,7 @@
         <f>HARMEAN(B90:H90)</f>
         <v>5.0283759620617277</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="25">
         <v>5.0283759620617277</v>
       </c>
       <c r="D89" t="str">
@@ -12122,7 +12014,7 @@
         <f>HYPGEOMDIST(1,4,8,20)</f>
         <v>0.36326109391124872</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="25">
         <v>0.36326109391124872</v>
       </c>
       <c r="D92" t="str">
@@ -12141,7 +12033,7 @@
         <f>INTERCEPT(B95:F95,B96:F96)</f>
         <v>4.8387096774192173E-2</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="25">
         <v>4.8387096774192173E-2</v>
       </c>
       <c r="D94" t="str">
@@ -12354,7 +12246,7 @@
         <f>LOGNORMDIST(4,3.5,1.2)</f>
         <v>3.9083555706800555E-2</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="25">
         <v>3.9083555706800555E-2</v>
       </c>
       <c r="D108" t="str">
@@ -12580,7 +12472,7 @@
         <f>NEGBINOMDIST(10,5,0.25)</f>
         <v>5.5048660375177888E-2</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="25">
         <v>5.5048660375177888E-2</v>
       </c>
       <c r="D123" t="str">
@@ -12599,7 +12491,7 @@
         <f>NORMDIST(42,40,1.5,TRUE)</f>
         <v>0.90878878027413212</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="25">
         <v>0.90878878027413212</v>
       </c>
       <c r="D125" t="str">
@@ -12614,11 +12506,11 @@
       <c r="A127" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B127" s="12">
+      <c r="B127" s="25">
         <f>NORMINV(0.908789,40,1.5)</f>
         <v>42.00000200956616</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="25">
         <v>42.00000200956616</v>
       </c>
       <c r="D127" t="str">
@@ -12637,7 +12529,7 @@
         <f>NORMSDIST(1.333333)</f>
         <v>0.90878872560409529</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="25">
         <v>0.90878872560409529</v>
       </c>
       <c r="D129" t="str">
@@ -12656,7 +12548,7 @@
         <f>NORMSINV(0.908789)</f>
         <v>1.3333346730441065</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="25">
         <v>1.3333346730441065</v>
       </c>
       <c r="D131" t="str">
@@ -12758,7 +12650,7 @@
         <f>PERCENTRANK(B139:K139,2)</f>
         <v>0.33300000000000002</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="25">
         <v>0.33300000000000002</v>
       </c>
       <c r="D138" t="str">
@@ -12826,7 +12718,7 @@
         <f>POISSON(2,5,TRUE)</f>
         <v>0.12465201948308466</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="25">
         <v>0.12465201948308466</v>
       </c>
       <c r="D142" t="str">
@@ -12966,7 +12858,7 @@
         <f>RSQ(B152:H152,B153:H153)</f>
         <v>5.7950191570881222E-2</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="25">
         <v>5.7950191570881222E-2</v>
       </c>
       <c r="D151" t="str">
@@ -13030,7 +12922,7 @@
         <f>SKEW(B155:K155)</f>
         <v>0.35954307140679742</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="25">
         <v>0.35954307140679742</v>
       </c>
       <c r="D154" t="str">
@@ -13079,7 +12971,7 @@
         <f>SLOPE(B157:H157,B158:H158)</f>
         <v>0.30555555555555558</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="25">
         <v>0.30555555555555558</v>
       </c>
       <c r="D156" t="str">
@@ -13192,7 +13084,7 @@
         <f>STANDARDIZE(42,40,1.5)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="C162">
+      <c r="C162" s="25">
         <v>1.3333333333333333</v>
       </c>
       <c r="D162" t="str">
@@ -13211,7 +13103,7 @@
         <f>STDEV(B165:K165)</f>
         <v>27.463915719840482</v>
       </c>
-      <c r="C164">
+      <c r="C164" s="25">
         <v>27.463915719840482</v>
       </c>
       <c r="D164" t="str">
@@ -13260,7 +13152,7 @@
         <f>STDEVA(B165:K165)</f>
         <v>27.463915719840482</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="25">
         <v>27.463915719840482</v>
       </c>
       <c r="D166" t="str">
@@ -13279,7 +13171,7 @@
         <f>STDEVP(B165:K165)</f>
         <v>26.054558142482477</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="25">
         <v>26.054558142482477</v>
       </c>
       <c r="D168" t="str">
@@ -13298,7 +13190,7 @@
         <f>STDEVPA(B165:K165)</f>
         <v>26.054558142482477</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="25">
         <v>26.054558142482477</v>
       </c>
       <c r="D170" t="str">
@@ -13788,7 +13680,7 @@
     </row>
     <row r="202" spans="1:11">
       <c r="A202" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="203" spans="1:11" ht="15.75">
@@ -14378,67 +14270,67 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D14 D17 D19 D21 D23 D25 D27">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14452,8 +14344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14613,7 +14505,7 @@
         <f>BIN2OCT(1001,3)</f>
         <v>011</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="35" t="s">
         <v>368</v>
       </c>
       <c r="D15" t="str">
@@ -14630,11 +14522,11 @@
       <c r="A17" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B17" s="24" t="str">
+      <c r="B17" s="12" t="str">
         <f>COMPLEX(3,4)</f>
         <v>3+4i</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="12" t="s">
         <v>369</v>
       </c>
       <c r="D17" t="str">
@@ -14656,7 +14548,7 @@
         <v>1001</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D19" t="str">
         <f>IF(B19=C19,"T","WARN")</f>
@@ -14676,7 +14568,7 @@
         <f>DEC2HEX(100,4)</f>
         <v>0064</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="35" t="s">
         <v>371</v>
       </c>
       <c r="D21" t="str">
@@ -14697,7 +14589,7 @@
         <f>DEC2OCT(58,3)</f>
         <v>072</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="35" t="s">
         <v>372</v>
       </c>
       <c r="D23" t="str">
@@ -14802,7 +14694,7 @@
         <f>HEX2BIN("F",8)</f>
         <v>00001111</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="35" t="s">
         <v>373</v>
       </c>
       <c r="D33" t="str">
@@ -14844,7 +14736,7 @@
         <f>HEX2OCT("F",3)</f>
         <v>017</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="35" t="s">
         <v>374</v>
       </c>
       <c r="D37" t="str">
@@ -15219,7 +15111,7 @@
         <f>OCT2BIN(3, 3)</f>
         <v>011</v>
       </c>
-      <c r="C73" s="36" t="s">
+      <c r="C73" s="35" t="s">
         <v>368</v>
       </c>
       <c r="D73" t="str">
@@ -15261,7 +15153,7 @@
         <f>OCT2HEX(100, 4)</f>
         <v>0040</v>
       </c>
-      <c r="C77" s="36" t="s">
+      <c r="C77" s="35" t="s">
         <v>387</v>
       </c>
       <c r="D77" t="str">
@@ -15275,7 +15167,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B79" s="24"/>
     </row>
@@ -15875,37 +15767,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update formula test case * use another way to determine end of formulas * add more test case * add custom formula
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,35 +4,106 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110"/>
   </bookViews>
   <sheets>
-    <sheet name="temp" sheetId="12" r:id="rId1"/>
-    <sheet name="formula-math" sheetId="2" r:id="rId2"/>
-    <sheet name="formula-logical" sheetId="4" r:id="rId3"/>
-    <sheet name="formula-text" sheetId="5" r:id="rId4"/>
-    <sheet name="formula-info" sheetId="6" r:id="rId5"/>
-    <sheet name="formula-datetime" sheetId="7" r:id="rId6"/>
-    <sheet name="formula-financial" sheetId="8" r:id="rId7"/>
-    <sheet name="formula-statistical" sheetId="9" r:id="rId8"/>
-    <sheet name="formula-engineering" sheetId="10" r:id="rId9"/>
-    <sheet name="formula-notsupported" sheetId="11" r:id="rId10"/>
+    <sheet name="first" sheetId="15" r:id="rId1"/>
+    <sheet name="temp" sheetId="14" r:id="rId2"/>
+    <sheet name="formula-math" sheetId="2" r:id="rId3"/>
+    <sheet name="formula-logical" sheetId="4" r:id="rId4"/>
+    <sheet name="formula-text" sheetId="5" r:id="rId5"/>
+    <sheet name="formula-info" sheetId="6" r:id="rId6"/>
+    <sheet name="formula-datetime" sheetId="7" r:id="rId7"/>
+    <sheet name="formula-financial" sheetId="8" r:id="rId8"/>
+    <sheet name="formula-statistical" sheetId="9" r:id="rId9"/>
+    <sheet name="formula-engineering" sheetId="10" r:id="rId10"/>
+    <sheet name="formula-notsupported" sheetId="11" r:id="rId11"/>
+    <sheet name="formula-custom" sheetId="13" r:id="rId12"/>
+    <sheet name="error" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-datetime'!$A$10:$C$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'formula-engineering'!$A$10:$C$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'formula-info'!$A$10:$C$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'formula-logical'!$A$8:$C$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'formula-math'!$A$9:$C$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-statistical'!$A$11:$C$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'formula-text'!$A$5:$C$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'formula-engineering'!$A$10:$C$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$10:$C$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'formula-logical'!$A$8:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'formula-math'!$A$9:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'formula-statistical'!$A$11:$C$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'formula-text'!$A$5:$C$35</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Hawk</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hawk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not in doc</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Hawk</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hawk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not in doc</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hawk</author>
@@ -91,7 +162,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hawk</author>
@@ -173,7 +244,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hawk</author>
@@ -399,7 +470,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hawk</author>
@@ -1273,8 +1344,42 @@
 </comments>
 </file>
 
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Hawk</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hawk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not in doc</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="402">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2474,6 +2579,12 @@
   </si>
   <si>
     <t>END OF FORMULA</t>
+  </si>
+  <si>
+    <t>toTWD</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -2677,7 +2788,127 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3420,21 +3651,1573 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15.75">
+      <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="str">
+        <f>ASC("EXCEL")</f>
+        <v>EXCEL</v>
+      </c>
+      <c r="C2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(B2=C2,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="5" t="str">
+        <f>CHAR(65)</f>
+        <v>A</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(B4=C4,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="25">
+        <f>BETADIST(2,8,10,1,3)</f>
+        <v>0.68547058095349067</v>
+      </c>
+      <c r="C6">
+        <v>0.68547058095349067</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(B6=C6,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" s="12">
+        <f>BETAINV(0.6854,8,10,1,3)</f>
+        <v>1.9999523162841797</v>
+      </c>
+      <c r="C8">
+        <v>1.9999523162841797</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(B8=C8,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D4">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6 D8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D501"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="25.5" customHeight="1"/>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="25">
+        <f>BESSELI(1.5,1)</f>
+        <v>0.98166642847516605</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.98166642847516605</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(B3=C3,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="1"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="25">
+        <f>BESSELJ(1.9,2)</f>
+        <v>0.3299258286697852</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.3299258286697852</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(B5=C5,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="1"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" s="25">
+        <f>BESSELK(1.5,1)</f>
+        <v>0.27738780363225868</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0.27738780363225868</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(B7=C7,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75">
+      <c r="A9" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="25">
+        <f>BESSELY(2.5,1)</f>
+        <v>0.14591813750831284</v>
+      </c>
+      <c r="C9" s="25">
+        <v>0.14591813750831284</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(B9=C9,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75">
+      <c r="A10" s="1"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75">
+      <c r="A11" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="7">
+        <f>BIN2DEC(1100100)</f>
+        <v>100</v>
+      </c>
+      <c r="C11" s="7">
+        <v>100</v>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(B11=C11,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
+      <c r="A12" s="1"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75">
+      <c r="A13" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B13" s="24" t="str">
+        <f>BIN2HEX(11111011,4)</f>
+        <v>00FB</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="D13" t="str">
+        <f>IF(B13=C13,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75">
+      <c r="A14" s="1"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="A15" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="24" t="str">
+        <f>BIN2OCT(1001,3)</f>
+        <v>011</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="D15" t="str">
+        <f>IF(B15=C15,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
+      <c r="A16" s="1"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
+      <c r="A17" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17" s="12" t="str">
+        <f>COMPLEX(3,4)</f>
+        <v>3+4i</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="D17" t="str">
+        <f>IF(B17=C17,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="1"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
+      <c r="A19" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B19" s="24" t="str">
+        <f>DEC2BIN(9,4)</f>
+        <v>1001</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(B19=C19,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
+      <c r="A20" s="1"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
+      <c r="A21" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B21" s="24" t="str">
+        <f>DEC2HEX(100,4)</f>
+        <v>0064</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(B21=C21,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
+      <c r="A22" s="1"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B23" s="24" t="str">
+        <f>DEC2OCT(58,3)</f>
+        <v>072</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(B23=C23,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75">
+      <c r="A24" s="1"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
+      <c r="A25" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B25" s="7">
+        <f>DELTA(5,4)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="24">
+        <v>0</v>
+      </c>
+      <c r="D25" t="str">
+        <f>IF(B25=C25,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
+      <c r="A26" s="1"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75">
+      <c r="A27" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B27" s="33">
+        <f>ERF(0.745)</f>
+        <v>0.70792869314881979</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0.70792869314881979</v>
+      </c>
+      <c r="D27" t="str">
+        <f>IF(B27=C27,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75">
+      <c r="A28" s="1"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B29" s="25">
+        <f>ERFC(1)</f>
+        <v>0.15729926482544476</v>
+      </c>
+      <c r="C29" s="25">
+        <v>0.15729926482544476</v>
+      </c>
+      <c r="D29" t="str">
+        <f>IF(B29=C29,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75">
+      <c r="A30" s="1"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
+      <c r="A31" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B31" s="24">
+        <f>GESTEP(5,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="24">
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f>IF(B31=C31,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="1"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75">
+      <c r="A33" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B33" s="24" t="str">
+        <f>HEX2BIN("F",8)</f>
+        <v>00001111</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="D33" t="str">
+        <f>IF(B33=C33,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="1"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75">
+      <c r="A35" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B35" s="24">
+        <f>HEX2DEC("A5")</f>
+        <v>165</v>
+      </c>
+      <c r="C35" s="24">
+        <v>165</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(B35=C35,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
+      <c r="A36" s="1"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B37" s="24" t="str">
+        <f>HEX2OCT("F",3)</f>
+        <v>017</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>374</v>
+      </c>
+      <c r="D37" t="str">
+        <f>IF(B37=C37,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" s="1"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75">
+      <c r="A39" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" s="24">
+        <f>IMABS("5+12i")</f>
+        <v>13</v>
+      </c>
+      <c r="C39" s="24">
+        <v>13</v>
+      </c>
+      <c r="D39" t="str">
+        <f>IF(B39=C39,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75">
+      <c r="A40" s="1"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
+      <c r="A41" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B41" s="24">
+        <f>IMAGINARY("3+4i")</f>
+        <v>4</v>
+      </c>
+      <c r="C41" s="24">
+        <v>4</v>
+      </c>
+      <c r="D41" t="str">
+        <f>IF(B41=C41,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" s="1"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75">
+      <c r="A43" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B43" s="25">
+        <f>IMARGUMENT("3+4i")</f>
+        <v>0.92729521800161219</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0.92729521800161219</v>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(B43=C43,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="1"/>
+      <c r="C44" s="24"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75">
+      <c r="A45" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B45" t="str">
+        <f>IMCONJUGATE("3+4i")</f>
+        <v>3-4i</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="D45" t="str">
+        <f>IF(B45=C45,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75">
+      <c r="A46" s="1"/>
+      <c r="C46" s="24"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75">
+      <c r="A47" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B47" s="25" t="str">
+        <f>IMCOS("1+i")</f>
+        <v>0.833730025131149-0.988897705762865i</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="D47" t="str">
+        <f>IF(B47=C47,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75">
+      <c r="A48" s="1"/>
+      <c r="C48" s="24"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75">
+      <c r="A49" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B49" t="str">
+        <f>IMDIV("-238+240i","10+24i")</f>
+        <v>5+12i</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="D49" t="str">
+        <f>IF(B49=C49,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75">
+      <c r="A50" s="1"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75">
+      <c r="A51" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B51" s="24" t="str">
+        <f>IMEXP("1+i")</f>
+        <v>1.46869393991589+2.28735528717884i</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="D51" t="str">
+        <f>IF(B51=C51,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75">
+      <c r="A52" s="1"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75">
+      <c r="A53" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B53" s="24" t="str">
+        <f>IMLN("3+4i")</f>
+        <v>1.6094379124341+0.927295218001612i</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="D53" t="str">
+        <f>IF(B53=C53,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75">
+      <c r="A54" s="1"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75">
+      <c r="A55" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" s="24" t="str">
+        <f>IMLOG10("3+4i")</f>
+        <v>0.698970004336019+0.402719196273373i</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="D55" t="str">
+        <f>IF(B55=C55,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="1"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B57" s="24" t="str">
+        <f>IMLOG2("3+4i")</f>
+        <v>2.32192809506607+1.33780421255394i</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="D57" t="str">
+        <f>IF(B57=C57,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="1"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75">
+      <c r="A59" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B59" s="24" t="str">
+        <f>IMPOWER("2+3i", 3)</f>
+        <v>-46+9.00000000000001i</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="D59" t="str">
+        <f>IF(B59=C59,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75">
+      <c r="A60" s="1"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75">
+      <c r="A61" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B61" s="24" t="str">
+        <f>IMPRODUCT("3+4i","5-3i")</f>
+        <v>27+11i</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D61" t="str">
+        <f>IF(B61=C61,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75">
+      <c r="A62" s="1"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75">
+      <c r="A63" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B63" s="24">
+        <f>IMREAL("6-9i")</f>
+        <v>6</v>
+      </c>
+      <c r="C63" s="24">
+        <v>6</v>
+      </c>
+      <c r="D63" t="str">
+        <f>IF(B63=C63,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75">
+      <c r="A64" s="1"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75">
+      <c r="A65" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B65" s="24" t="str">
+        <f>IMSIN("3+4i")</f>
+        <v>3.85373803791938-27.0168132580039i</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="D65" t="str">
+        <f>IF(B65=C65,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75">
+      <c r="A66" s="1"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="24"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75">
+      <c r="A67" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B67" s="24" t="str">
+        <f>IMSQRT("1+i")</f>
+        <v>1.09868411346781+0.455089860562227i</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="D67" t="str">
+        <f>IF(B67=C67,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75">
+      <c r="A68" s="1"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="24"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75">
+      <c r="A69" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B69" s="24" t="str">
+        <f>IMSUB("13+4i","5+3i")</f>
+        <v>8+i</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>386</v>
+      </c>
+      <c r="D69" t="str">
+        <f>IF(B69=C69,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75">
+      <c r="A70" s="1"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="24"/>
+    </row>
+    <row r="71" spans="1:4" ht="15.75">
+      <c r="A71" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B71" s="24" t="str">
+        <f>IMSUM("3+4i","5-3i")</f>
+        <v>8+i</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>386</v>
+      </c>
+      <c r="D71" t="str">
+        <f>IF(B71=C71,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75">
+      <c r="A72" s="1"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="24"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75">
+      <c r="A73" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B73" s="24" t="str">
+        <f>OCT2BIN(3, 3)</f>
+        <v>011</v>
+      </c>
+      <c r="C73" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="D73" t="str">
+        <f>IF(B73=C73,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75">
+      <c r="A74" s="1"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="24"/>
+    </row>
+    <row r="75" spans="1:4" ht="15.75">
+      <c r="A75" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B75" s="24">
+        <f>OCT2DEC(54)</f>
+        <v>44</v>
+      </c>
+      <c r="C75" s="24">
+        <v>44</v>
+      </c>
+      <c r="D75" t="str">
+        <f>IF(B75=C75,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75">
+      <c r="A76" s="1"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="24"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75">
+      <c r="A77" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B77" s="24" t="str">
+        <f>OCT2HEX(100, 4)</f>
+        <v>0040</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>387</v>
+      </c>
+      <c r="D77" t="str">
+        <f>IF(B77=C77,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75">
+      <c r="A78" s="1"/>
+      <c r="B78" s="24"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>399</v>
+      </c>
+      <c r="B79" s="24"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75">
+      <c r="A80" s="1"/>
+      <c r="B80" s="24"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.75">
+      <c r="A81" s="1"/>
+      <c r="B81" s="24"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.75">
+      <c r="A82" s="1"/>
+      <c r="B82" s="24"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.75">
+      <c r="A83" s="1"/>
+      <c r="B83" s="24"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.75">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.75">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:2" ht="15.75">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.75">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.75">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.75">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.75">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.75">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.75">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.75">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.75">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.75">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" ht="15.75">
+      <c r="A99" s="1"/>
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.75">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.75">
+      <c r="A101" s="1"/>
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.75">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.75">
+      <c r="A103" s="1"/>
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="1:2" ht="15.75">
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.75">
+      <c r="A105" s="1"/>
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" spans="1:2" ht="15.75">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.75">
+      <c r="A107" s="1"/>
+      <c r="B107" s="8"/>
+    </row>
+    <row r="108" spans="1:2" ht="15.75">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.75">
+      <c r="A109" s="1"/>
+      <c r="B109" s="5"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.75">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.75">
+      <c r="A111" s="1"/>
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.75">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.75">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.75">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.75">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.75">
+      <c r="A116" s="1"/>
+      <c r="B116" s="5"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.75">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.75">
+      <c r="A118" s="1"/>
+      <c r="B118" s="11"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.75">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.75">
+      <c r="A120" s="1"/>
+      <c r="B120" s="9"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.75">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.75">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.75">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.75">
+      <c r="A124" s="1"/>
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.75">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.75">
+      <c r="A126" s="1"/>
+      <c r="B126" s="5"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.75">
+      <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.75">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:2" ht="15.75">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.75">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.75">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.75">
+      <c r="A132" s="1"/>
+      <c r="B132" s="8"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.75">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.75">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:2" ht="15.75">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:2" ht="15.75">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:2" ht="15.75">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.75">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:2" ht="15.75">
+      <c r="A139" s="1"/>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="B141" s="12"/>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="B143" s="8"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.75">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:2" ht="15.75">
+      <c r="A145" s="1"/>
+      <c r="B145" s="5"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.75">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.75">
+      <c r="A147" s="1"/>
+      <c r="B147" s="11"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.75">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.75">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:2" ht="15.75">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:2" ht="15.75">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:2" ht="15.75">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.75">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.75">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.75">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:2" ht="15.75">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.75">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:2" ht="15.75">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.75">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.75">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" spans="1:1" ht="15.75">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" ht="15.75">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" ht="15.75">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" spans="1:1" ht="15.75">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" ht="15.75">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" ht="15.75">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" ht="15.75">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" ht="15.75">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" ht="15.75">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:1" ht="15.75">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" ht="15.75">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:1" ht="15.75">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:1" ht="15.75">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:1" ht="15.75">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:1" ht="15.75">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:1" ht="15.75">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:2" ht="15.75">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:2" ht="15.75">
+      <c r="A178" s="1"/>
+      <c r="B178" s="5"/>
+    </row>
+    <row r="179" spans="1:2" ht="15.75">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:2" ht="15.75">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:2" ht="15.75">
+      <c r="A181" s="1"/>
+      <c r="B181" s="5"/>
+    </row>
+    <row r="182" spans="1:2" ht="15.75">
+      <c r="A182" s="1"/>
+    </row>
+    <row r="183" spans="1:2" ht="15.75">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:2" ht="15.75">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:2" ht="15.75">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:2" ht="15.75">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:2" ht="15.75">
+      <c r="A187" s="1"/>
+    </row>
+    <row r="188" spans="1:2" ht="15.75">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:2" ht="15.75">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" spans="1:2" ht="15.75">
+      <c r="A190" s="1"/>
+    </row>
+    <row r="191" spans="1:2" ht="15.75">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:2" ht="15.75">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" spans="1:2" ht="15.75">
+      <c r="A193" s="1"/>
+    </row>
+    <row r="194" spans="1:2" ht="15.75">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" spans="1:2" ht="15.75">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:2" ht="15.75">
+      <c r="A196" s="1"/>
+    </row>
+    <row r="197" spans="1:2" ht="15.75">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" spans="1:2" ht="15.75">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" spans="1:2" ht="15.75">
+      <c r="A199" s="1"/>
+    </row>
+    <row r="200" spans="1:2" ht="15.75">
+      <c r="A200" s="1"/>
+    </row>
+    <row r="201" spans="1:2" ht="15.75">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" spans="1:2" ht="15.75">
+      <c r="A202" s="1"/>
+    </row>
+    <row r="203" spans="1:2" ht="15.75">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" spans="1:2" ht="15.75">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:2" ht="15.75">
+      <c r="A205" s="1"/>
+    </row>
+    <row r="206" spans="1:2" ht="15.75">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207" spans="1:2" ht="15.75">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:2" ht="15.75">
+      <c r="A208" s="1"/>
+      <c r="B208" s="11"/>
+    </row>
+    <row r="209" spans="1:2" ht="15.75">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210" spans="1:2" ht="15.75">
+      <c r="A210" s="1"/>
+      <c r="B210" s="11"/>
+    </row>
+    <row r="211" spans="1:2" ht="15.75">
+      <c r="A211" s="1"/>
+      <c r="B211" s="11"/>
+    </row>
+    <row r="212" spans="1:2" ht="15.75">
+      <c r="A212" s="1"/>
+      <c r="B212" s="5"/>
+    </row>
+    <row r="213" spans="1:2" ht="15.75">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:2" ht="15.75">
+      <c r="A214" s="1"/>
+    </row>
+    <row r="215" spans="1:2" ht="15.75">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:2" ht="15.75">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:2" ht="15.75">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:2" ht="15.75">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="219" spans="1:2" ht="15.75">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="220" spans="1:2" ht="15.75">
+      <c r="A220" s="1"/>
+    </row>
+    <row r="221" spans="1:2" ht="15.75">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:2" ht="15.75">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="223" spans="1:2" ht="15.75">
+      <c r="A223" s="1"/>
+    </row>
+    <row r="224" spans="1:2" ht="15.75">
+      <c r="A224" s="1"/>
+    </row>
+    <row r="225" spans="1:1" ht="15.75">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:1" ht="15.75">
+      <c r="A226" s="1"/>
+    </row>
+    <row r="227" spans="1:1" ht="15.75">
+      <c r="A227" s="1"/>
+    </row>
+    <row r="228" spans="1:1" ht="15.75">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:1" ht="15.75">
+      <c r="A229" s="1"/>
+    </row>
+    <row r="230" spans="1:1" ht="15.75">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:1" ht="15.75">
+      <c r="A231" s="1"/>
+    </row>
+    <row r="232" spans="1:1" ht="15.75">
+      <c r="A232" s="1"/>
+    </row>
+    <row r="233" spans="1:1" ht="15.75">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:1" ht="15.75">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:1" ht="15.75">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:1" ht="15.75">
+      <c r="A236" s="1"/>
+    </row>
+    <row r="237" spans="1:1" ht="15.75">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:1" ht="15.75">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="239" spans="1:1" ht="15.75">
+      <c r="A239" s="1"/>
+    </row>
+    <row r="240" spans="1:1" ht="15.75">
+      <c r="A240" s="1"/>
+    </row>
+    <row r="241" spans="1:1" ht="15.75">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" ht="15.75">
+      <c r="A242" s="1"/>
+    </row>
+    <row r="243" spans="1:1" ht="15.75">
+      <c r="A243" s="1"/>
+    </row>
+    <row r="244" spans="1:1" ht="15.75">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="245" spans="1:1" ht="15.75">
+      <c r="A245" s="1"/>
+    </row>
+    <row r="246" spans="1:1" ht="15.75">
+      <c r="A246" s="1"/>
+    </row>
+    <row r="247" spans="1:1" ht="15.75">
+      <c r="A247" s="1"/>
+    </row>
+    <row r="248" spans="1:1" ht="15.75">
+      <c r="A248" s="1"/>
+    </row>
+    <row r="249" spans="1:1" ht="15.75">
+      <c r="A249" s="1"/>
+    </row>
+    <row r="250" spans="1:1" ht="15.75">
+      <c r="A250" s="1"/>
+    </row>
+    <row r="251" spans="1:1" ht="15.75">
+      <c r="A251" s="1"/>
+    </row>
+    <row r="252" spans="1:1" ht="15.75">
+      <c r="A252" s="1"/>
+    </row>
+    <row r="253" spans="1:1" ht="15.75">
+      <c r="A253" s="1"/>
+    </row>
+    <row r="254" spans="1:1" ht="15.75">
+      <c r="A254" s="1"/>
+    </row>
+    <row r="255" spans="1:1" ht="15.75">
+      <c r="A255" s="1"/>
+    </row>
+    <row r="256" spans="1:1" ht="15.75">
+      <c r="A256" s="1"/>
+    </row>
+    <row r="257" spans="1:1" ht="15.75">
+      <c r="A257" s="1"/>
+    </row>
+    <row r="258" spans="1:1" ht="15.75">
+      <c r="A258" s="1"/>
+    </row>
+    <row r="259" spans="1:1" ht="15.75">
+      <c r="A259" s="1"/>
+    </row>
+    <row r="260" spans="1:1" ht="15.75">
+      <c r="A260" s="1"/>
+    </row>
+    <row r="261" spans="1:1" ht="15.75">
+      <c r="A261" s="1"/>
+    </row>
+    <row r="262" spans="1:1" ht="15.75">
+      <c r="A262" s="1"/>
+    </row>
+    <row r="263" spans="1:1" ht="15.75">
+      <c r="A263" s="1"/>
+    </row>
+    <row r="264" spans="1:1" ht="15.75">
+      <c r="A264" s="1"/>
+    </row>
+    <row r="265" spans="1:1" ht="15.75">
+      <c r="A265" s="1"/>
+    </row>
+    <row r="266" spans="1:1" ht="15.75">
+      <c r="A266" s="1"/>
+    </row>
+    <row r="267" spans="1:1" ht="15.75">
+      <c r="A267" s="1"/>
+    </row>
+    <row r="268" spans="1:1" ht="15.75">
+      <c r="A268" s="1"/>
+    </row>
+    <row r="269" spans="1:1" ht="15.75">
+      <c r="A269" s="1"/>
+    </row>
+    <row r="270" spans="1:1" ht="15.75">
+      <c r="A270" s="1"/>
+    </row>
+    <row r="272" spans="1:1" ht="15.75">
+      <c r="A272" s="1"/>
+    </row>
+    <row r="501" spans="1:1">
+      <c r="A501" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="D3:D42">
+    <sortCondition ref="D3"/>
+  </sortState>
+  <conditionalFormatting sqref="D3 D5 D7 D9 D11">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3586,7 +5369,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3595,12 +5378,250 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" t="e">
+        <f ca="1">toTWD(B4,C4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3" t="e">
+        <f ca="1">IF(B3=C3,"T","WARN")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" t="str">
+        <f>ASC("EXCEL")</f>
+        <v>EXCEL</v>
+      </c>
+      <c r="C4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(B4=C4,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="5" t="str">
+        <f>CHAR(65)</f>
+        <v>A</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(B6=C6,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D4:D6">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="str">
+        <f>ASC("EXCEL")</f>
+        <v>EXCEL</v>
+      </c>
+      <c r="C3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(B3=C3,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f>CHAR(65)</f>
+        <v>A</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(B5=C5,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="25">
+        <f>BETADIST(2,8,10,1,3)</f>
+        <v>0.68547058095349067</v>
+      </c>
+      <c r="C7">
+        <v>0.68547058095349067</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(B7=C7,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75">
+      <c r="A9" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" s="12">
+        <f>BETAINV(0.6854,8,10,1,3)</f>
+        <v>1.9999523162841797</v>
+      </c>
+      <c r="C9">
+        <v>1.9999523162841797</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(B9=C9,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>399</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:D5">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 D9">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I415"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4484,7 +6505,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>46.676197475810355</v>
+        <v>31.358356266281451</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -4502,7 +6523,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -5389,7 +7410,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5401,12 +7422,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5604,7 +7625,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5613,12 +7634,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6789,7 +8810,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6799,12 +8820,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J451"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7780,17 +9801,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7799,7 +9820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D458"/>
   <sheetViews>
@@ -8013,7 +10034,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41397.626794791664</v>
+        <v>41400.624196296296</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -8082,7 +10103,7 @@
       </c>
       <c r="B29" s="22">
         <f ca="1">TODAY()</f>
-        <v>41397</v>
+        <v>41400</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -8760,22 +10781,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8785,7 +10806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I534"/>
   <sheetViews>
@@ -10800,32 +12821,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10835,12 +12856,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14270,67 +16291,67 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D14 D17 D19 D21 D23 D25 D27">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14338,1470 +16359,4 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D501"/>
-  <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="25.5" customHeight="1"/>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B3" s="25">
-        <f>BESSELI(1.5,1)</f>
-        <v>0.98166642847516605</v>
-      </c>
-      <c r="C3" s="25">
-        <v>0.98166642847516605</v>
-      </c>
-      <c r="D3" t="str">
-        <f>IF(B3=C3,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="1"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B5" s="25">
-        <f>BESSELJ(1.9,2)</f>
-        <v>0.3299258286697852</v>
-      </c>
-      <c r="C5" s="25">
-        <v>0.3299258286697852</v>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(B5=C5,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="1"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
-      <c r="A7" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B7" s="25">
-        <f>BESSELK(1.5,1)</f>
-        <v>0.27738780363225868</v>
-      </c>
-      <c r="C7" s="25">
-        <v>0.27738780363225868</v>
-      </c>
-      <c r="D7" t="str">
-        <f>IF(B7=C7,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
-      <c r="A8" s="1"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75">
-      <c r="A9" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B9" s="25">
-        <f>BESSELY(2.5,1)</f>
-        <v>0.14591813750831284</v>
-      </c>
-      <c r="C9" s="25">
-        <v>0.14591813750831284</v>
-      </c>
-      <c r="D9" t="str">
-        <f>IF(B9=C9,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75">
-      <c r="A10" s="1"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75">
-      <c r="A11" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B11" s="7">
-        <f>BIN2DEC(1100100)</f>
-        <v>100</v>
-      </c>
-      <c r="C11" s="7">
-        <v>100</v>
-      </c>
-      <c r="D11" t="str">
-        <f>IF(B11=C11,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75">
-      <c r="A12" s="1"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75">
-      <c r="A13" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B13" s="24" t="str">
-        <f>BIN2HEX(11111011,4)</f>
-        <v>00FB</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>367</v>
-      </c>
-      <c r="D13" t="str">
-        <f>IF(B13=C13,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
-      <c r="A14" s="1"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75">
-      <c r="A15" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B15" s="24" t="str">
-        <f>BIN2OCT(1001,3)</f>
-        <v>011</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>368</v>
-      </c>
-      <c r="D15" t="str">
-        <f>IF(B15=C15,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75">
-      <c r="A16" s="1"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
-      <c r="A17" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B17" s="12" t="str">
-        <f>COMPLEX(3,4)</f>
-        <v>3+4i</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="D17" t="str">
-        <f>IF(B17=C17,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="1"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75">
-      <c r="A19" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="B19" s="24" t="str">
-        <f>DEC2BIN(9,4)</f>
-        <v>1001</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(B19=C19,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75">
-      <c r="A20" s="1"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75">
-      <c r="A21" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B21" s="24" t="str">
-        <f>DEC2HEX(100,4)</f>
-        <v>0064</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>371</v>
-      </c>
-      <c r="D21" t="str">
-        <f>IF(B21=C21,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75">
-      <c r="A22" s="1"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75">
-      <c r="A23" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B23" s="24" t="str">
-        <f>DEC2OCT(58,3)</f>
-        <v>072</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>372</v>
-      </c>
-      <c r="D23" t="str">
-        <f>IF(B23=C23,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75">
-      <c r="A24" s="1"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75">
-      <c r="A25" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="B25" s="7">
-        <f>DELTA(5,4)</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="24">
-        <v>0</v>
-      </c>
-      <c r="D25" t="str">
-        <f>IF(B25=C25,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75">
-      <c r="A26" s="1"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75">
-      <c r="A27" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B27" s="33">
-        <f>ERF(0.745)</f>
-        <v>0.70792869314881979</v>
-      </c>
-      <c r="C27" s="25">
-        <v>0.70792869314881979</v>
-      </c>
-      <c r="D27" t="str">
-        <f>IF(B27=C27,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75">
-      <c r="A28" s="1"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75">
-      <c r="A29" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B29" s="25">
-        <f>ERFC(1)</f>
-        <v>0.15729926482544476</v>
-      </c>
-      <c r="C29" s="25">
-        <v>0.15729926482544476</v>
-      </c>
-      <c r="D29" t="str">
-        <f>IF(B29=C29,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="1"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75">
-      <c r="A31" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="B31" s="24">
-        <f>GESTEP(5,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C31" s="24">
-        <v>1</v>
-      </c>
-      <c r="D31" t="str">
-        <f>IF(B31=C31,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75">
-      <c r="A32" s="1"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75">
-      <c r="A33" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B33" s="24" t="str">
-        <f>HEX2BIN("F",8)</f>
-        <v>00001111</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>373</v>
-      </c>
-      <c r="D33" t="str">
-        <f>IF(B33=C33,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75">
-      <c r="A34" s="1"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75">
-      <c r="A35" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="B35" s="24">
-        <f>HEX2DEC("A5")</f>
-        <v>165</v>
-      </c>
-      <c r="C35" s="24">
-        <v>165</v>
-      </c>
-      <c r="D35" t="str">
-        <f>IF(B35=C35,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75">
-      <c r="A36" s="1"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75">
-      <c r="A37" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="B37" s="24" t="str">
-        <f>HEX2OCT("F",3)</f>
-        <v>017</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>374</v>
-      </c>
-      <c r="D37" t="str">
-        <f>IF(B37=C37,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75">
-      <c r="A38" s="1"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75">
-      <c r="A39" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B39" s="24">
-        <f>IMABS("5+12i")</f>
-        <v>13</v>
-      </c>
-      <c r="C39" s="24">
-        <v>13</v>
-      </c>
-      <c r="D39" t="str">
-        <f>IF(B39=C39,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75">
-      <c r="A40" s="1"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75">
-      <c r="A41" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B41" s="24">
-        <f>IMAGINARY("3+4i")</f>
-        <v>4</v>
-      </c>
-      <c r="C41" s="24">
-        <v>4</v>
-      </c>
-      <c r="D41" t="str">
-        <f>IF(B41=C41,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75">
-      <c r="A42" s="1"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75">
-      <c r="A43" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B43" s="25">
-        <f>IMARGUMENT("3+4i")</f>
-        <v>0.92729521800161219</v>
-      </c>
-      <c r="C43" s="25">
-        <v>0.92729521800161219</v>
-      </c>
-      <c r="D43" t="str">
-        <f>IF(B43=C43,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75">
-      <c r="A44" s="1"/>
-      <c r="C44" s="24"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75">
-      <c r="A45" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B45" t="str">
-        <f>IMCONJUGATE("3+4i")</f>
-        <v>3-4i</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>375</v>
-      </c>
-      <c r="D45" t="str">
-        <f>IF(B45=C45,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75">
-      <c r="A46" s="1"/>
-      <c r="C46" s="24"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75">
-      <c r="A47" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B47" s="25" t="str">
-        <f>IMCOS("1+i")</f>
-        <v>0.833730025131149-0.988897705762865i</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>376</v>
-      </c>
-      <c r="D47" t="str">
-        <f>IF(B47=C47,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75">
-      <c r="A48" s="1"/>
-      <c r="C48" s="24"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75">
-      <c r="A49" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="B49" t="str">
-        <f>IMDIV("-238+240i","10+24i")</f>
-        <v>5+12i</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>377</v>
-      </c>
-      <c r="D49" t="str">
-        <f>IF(B49=C49,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75">
-      <c r="A50" s="1"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75">
-      <c r="A51" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B51" s="24" t="str">
-        <f>IMEXP("1+i")</f>
-        <v>1.46869393991589+2.28735528717884i</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>378</v>
-      </c>
-      <c r="D51" t="str">
-        <f>IF(B51=C51,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75">
-      <c r="A52" s="1"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75">
-      <c r="A53" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="B53" s="24" t="str">
-        <f>IMLN("3+4i")</f>
-        <v>1.6094379124341+0.927295218001612i</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>379</v>
-      </c>
-      <c r="D53" t="str">
-        <f>IF(B53=C53,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75">
-      <c r="A54" s="1"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75">
-      <c r="A55" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B55" s="24" t="str">
-        <f>IMLOG10("3+4i")</f>
-        <v>0.698970004336019+0.402719196273373i</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>380</v>
-      </c>
-      <c r="D55" t="str">
-        <f>IF(B55=C55,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="1"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="B57" s="24" t="str">
-        <f>IMLOG2("3+4i")</f>
-        <v>2.32192809506607+1.33780421255394i</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>381</v>
-      </c>
-      <c r="D57" t="str">
-        <f>IF(B57=C57,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="1"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B59" s="24" t="str">
-        <f>IMPOWER("2+3i", 3)</f>
-        <v>-46+9.00000000000001i</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>382</v>
-      </c>
-      <c r="D59" t="str">
-        <f>IF(B59=C59,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75">
-      <c r="A60" s="1"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-    </row>
-    <row r="61" spans="1:4" ht="15.75">
-      <c r="A61" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B61" s="24" t="str">
-        <f>IMPRODUCT("3+4i","5-3i")</f>
-        <v>27+11i</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>383</v>
-      </c>
-      <c r="D61" t="str">
-        <f>IF(B61=C61,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15.75">
-      <c r="A62" s="1"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-    </row>
-    <row r="63" spans="1:4" ht="15.75">
-      <c r="A63" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B63" s="24">
-        <f>IMREAL("6-9i")</f>
-        <v>6</v>
-      </c>
-      <c r="C63" s="24">
-        <v>6</v>
-      </c>
-      <c r="D63" t="str">
-        <f>IF(B63=C63,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75">
-      <c r="A64" s="1"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-    </row>
-    <row r="65" spans="1:4" ht="15.75">
-      <c r="A65" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="B65" s="24" t="str">
-        <f>IMSIN("3+4i")</f>
-        <v>3.85373803791938-27.0168132580039i</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="D65" t="str">
-        <f>IF(B65=C65,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.75">
-      <c r="A66" s="1"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="24"/>
-    </row>
-    <row r="67" spans="1:4" ht="15.75">
-      <c r="A67" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="B67" s="24" t="str">
-        <f>IMSQRT("1+i")</f>
-        <v>1.09868411346781+0.455089860562227i</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>385</v>
-      </c>
-      <c r="D67" t="str">
-        <f>IF(B67=C67,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15.75">
-      <c r="A68" s="1"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="24"/>
-    </row>
-    <row r="69" spans="1:4" ht="15.75">
-      <c r="A69" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B69" s="24" t="str">
-        <f>IMSUB("13+4i","5+3i")</f>
-        <v>8+i</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>386</v>
-      </c>
-      <c r="D69" t="str">
-        <f>IF(B69=C69,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="15.75">
-      <c r="A70" s="1"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="24"/>
-    </row>
-    <row r="71" spans="1:4" ht="15.75">
-      <c r="A71" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B71" s="24" t="str">
-        <f>IMSUM("3+4i","5-3i")</f>
-        <v>8+i</v>
-      </c>
-      <c r="C71" s="24" t="s">
-        <v>386</v>
-      </c>
-      <c r="D71" t="str">
-        <f>IF(B71=C71,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75">
-      <c r="A72" s="1"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="24"/>
-    </row>
-    <row r="73" spans="1:4" ht="15.75">
-      <c r="A73" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="B73" s="24" t="str">
-        <f>OCT2BIN(3, 3)</f>
-        <v>011</v>
-      </c>
-      <c r="C73" s="35" t="s">
-        <v>368</v>
-      </c>
-      <c r="D73" t="str">
-        <f>IF(B73=C73,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="15.75">
-      <c r="A74" s="1"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="24"/>
-    </row>
-    <row r="75" spans="1:4" ht="15.75">
-      <c r="A75" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B75" s="24">
-        <f>OCT2DEC(54)</f>
-        <v>44</v>
-      </c>
-      <c r="C75" s="24">
-        <v>44</v>
-      </c>
-      <c r="D75" t="str">
-        <f>IF(B75=C75,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="15.75">
-      <c r="A76" s="1"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="24"/>
-    </row>
-    <row r="77" spans="1:4" ht="15.75">
-      <c r="A77" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B77" s="24" t="str">
-        <f>OCT2HEX(100, 4)</f>
-        <v>0040</v>
-      </c>
-      <c r="C77" s="35" t="s">
-        <v>387</v>
-      </c>
-      <c r="D77" t="str">
-        <f>IF(B77=C77,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="15.75">
-      <c r="A78" s="1"/>
-      <c r="B78" s="24"/>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" t="s">
-        <v>399</v>
-      </c>
-      <c r="B79" s="24"/>
-    </row>
-    <row r="80" spans="1:4" ht="15.75">
-      <c r="A80" s="1"/>
-      <c r="B80" s="24"/>
-    </row>
-    <row r="81" spans="1:2" ht="15.75">
-      <c r="A81" s="1"/>
-      <c r="B81" s="24"/>
-    </row>
-    <row r="82" spans="1:2" ht="15.75">
-      <c r="A82" s="1"/>
-      <c r="B82" s="24"/>
-    </row>
-    <row r="83" spans="1:2" ht="15.75">
-      <c r="A83" s="1"/>
-      <c r="B83" s="24"/>
-    </row>
-    <row r="84" spans="1:2" ht="15.75">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.75">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:2" ht="15.75">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:2" ht="15.75">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.75">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.75">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.75">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.75">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="95" spans="1:2" ht="15.75">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.75">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" ht="15.75">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" ht="15.75">
-      <c r="A98" s="1"/>
-    </row>
-    <row r="99" spans="1:2" ht="15.75">
-      <c r="A99" s="1"/>
-      <c r="B99" s="5"/>
-    </row>
-    <row r="100" spans="1:2" ht="15.75">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:2" ht="15.75">
-      <c r="A101" s="1"/>
-      <c r="B101" s="5"/>
-    </row>
-    <row r="102" spans="1:2" ht="15.75">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" ht="15.75">
-      <c r="A103" s="1"/>
-      <c r="B103" s="5"/>
-    </row>
-    <row r="104" spans="1:2" ht="15.75">
-      <c r="A104" s="1"/>
-    </row>
-    <row r="105" spans="1:2" ht="15.75">
-      <c r="A105" s="1"/>
-      <c r="B105" s="5"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.75">
-      <c r="A106" s="1"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.75">
-      <c r="A107" s="1"/>
-      <c r="B107" s="8"/>
-    </row>
-    <row r="108" spans="1:2" ht="15.75">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.75">
-      <c r="A109" s="1"/>
-      <c r="B109" s="5"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.75">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.75">
-      <c r="A111" s="1"/>
-      <c r="B111" s="5"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.75">
-      <c r="A112" s="1"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.75">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.75">
-      <c r="A114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.75">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:2" ht="15.75">
-      <c r="A116" s="1"/>
-      <c r="B116" s="5"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.75">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.75">
-      <c r="A118" s="1"/>
-      <c r="B118" s="11"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.75">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.75">
-      <c r="A120" s="1"/>
-      <c r="B120" s="9"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.75">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:2" ht="15.75">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:2" ht="15.75">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.75">
-      <c r="A124" s="1"/>
-      <c r="B124" s="5"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.75">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.75">
-      <c r="A126" s="1"/>
-      <c r="B126" s="5"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.75">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.75">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:2" ht="15.75">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.75">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:2" ht="15.75">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:2" ht="15.75">
-      <c r="A132" s="1"/>
-      <c r="B132" s="8"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.75">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.75">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:2" ht="15.75">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:2" ht="15.75">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:2" ht="15.75">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.75">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.75">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="B141" s="12"/>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="B143" s="8"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.75">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.75">
-      <c r="A145" s="1"/>
-      <c r="B145" s="5"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.75">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.75">
-      <c r="A147" s="1"/>
-      <c r="B147" s="11"/>
-    </row>
-    <row r="148" spans="1:2" ht="15.75">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="149" spans="1:2" ht="15.75">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.75">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:2" ht="15.75">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:2" ht="15.75">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:2" ht="15.75">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:2" ht="15.75">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:2" ht="15.75">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:2" ht="15.75">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:2" ht="15.75">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:2" ht="15.75">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:2" ht="15.75">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:2" ht="15.75">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" ht="15.75">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" ht="15.75">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" ht="15.75">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" ht="15.75">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" ht="15.75">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="166" spans="1:1" ht="15.75">
-      <c r="A166" s="1"/>
-    </row>
-    <row r="167" spans="1:1" ht="15.75">
-      <c r="A167" s="1"/>
-    </row>
-    <row r="168" spans="1:1" ht="15.75">
-      <c r="A168" s="1"/>
-    </row>
-    <row r="169" spans="1:1" ht="15.75">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="170" spans="1:1" ht="15.75">
-      <c r="A170" s="1"/>
-    </row>
-    <row r="171" spans="1:1" ht="15.75">
-      <c r="A171" s="1"/>
-    </row>
-    <row r="172" spans="1:1" ht="15.75">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:1" ht="15.75">
-      <c r="A173" s="1"/>
-    </row>
-    <row r="174" spans="1:1" ht="15.75">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="175" spans="1:1" ht="15.75">
-      <c r="A175" s="1"/>
-    </row>
-    <row r="176" spans="1:1" ht="15.75">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:2" ht="15.75">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:2" ht="15.75">
-      <c r="A178" s="1"/>
-      <c r="B178" s="5"/>
-    </row>
-    <row r="179" spans="1:2" ht="15.75">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:2" ht="15.75">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:2" ht="15.75">
-      <c r="A181" s="1"/>
-      <c r="B181" s="5"/>
-    </row>
-    <row r="182" spans="1:2" ht="15.75">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:2" ht="15.75">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:2" ht="15.75">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:2" ht="15.75">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:2" ht="15.75">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:2" ht="15.75">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:2" ht="15.75">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:2" ht="15.75">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:2" ht="15.75">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:2" ht="15.75">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:2" ht="15.75">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:2" ht="15.75">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:2" ht="15.75">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:2" ht="15.75">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:2" ht="15.75">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:2" ht="15.75">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:2" ht="15.75">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:2" ht="15.75">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:2" ht="15.75">
-      <c r="A200" s="1"/>
-    </row>
-    <row r="201" spans="1:2" ht="15.75">
-      <c r="A201" s="1"/>
-    </row>
-    <row r="202" spans="1:2" ht="15.75">
-      <c r="A202" s="1"/>
-    </row>
-    <row r="203" spans="1:2" ht="15.75">
-      <c r="A203" s="1"/>
-    </row>
-    <row r="204" spans="1:2" ht="15.75">
-      <c r="A204" s="1"/>
-    </row>
-    <row r="205" spans="1:2" ht="15.75">
-      <c r="A205" s="1"/>
-    </row>
-    <row r="206" spans="1:2" ht="15.75">
-      <c r="A206" s="1"/>
-    </row>
-    <row r="207" spans="1:2" ht="15.75">
-      <c r="A207" s="1"/>
-    </row>
-    <row r="208" spans="1:2" ht="15.75">
-      <c r="A208" s="1"/>
-      <c r="B208" s="11"/>
-    </row>
-    <row r="209" spans="1:2" ht="15.75">
-      <c r="A209" s="1"/>
-    </row>
-    <row r="210" spans="1:2" ht="15.75">
-      <c r="A210" s="1"/>
-      <c r="B210" s="11"/>
-    </row>
-    <row r="211" spans="1:2" ht="15.75">
-      <c r="A211" s="1"/>
-      <c r="B211" s="11"/>
-    </row>
-    <row r="212" spans="1:2" ht="15.75">
-      <c r="A212" s="1"/>
-      <c r="B212" s="5"/>
-    </row>
-    <row r="213" spans="1:2" ht="15.75">
-      <c r="A213" s="1"/>
-    </row>
-    <row r="214" spans="1:2" ht="15.75">
-      <c r="A214" s="1"/>
-    </row>
-    <row r="215" spans="1:2" ht="15.75">
-      <c r="A215" s="1"/>
-    </row>
-    <row r="216" spans="1:2" ht="15.75">
-      <c r="A216" s="1"/>
-    </row>
-    <row r="217" spans="1:2" ht="15.75">
-      <c r="A217" s="1"/>
-    </row>
-    <row r="218" spans="1:2" ht="15.75">
-      <c r="A218" s="1"/>
-    </row>
-    <row r="219" spans="1:2" ht="15.75">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="220" spans="1:2" ht="15.75">
-      <c r="A220" s="1"/>
-    </row>
-    <row r="221" spans="1:2" ht="15.75">
-      <c r="A221" s="1"/>
-    </row>
-    <row r="222" spans="1:2" ht="15.75">
-      <c r="A222" s="1"/>
-    </row>
-    <row r="223" spans="1:2" ht="15.75">
-      <c r="A223" s="1"/>
-    </row>
-    <row r="224" spans="1:2" ht="15.75">
-      <c r="A224" s="1"/>
-    </row>
-    <row r="225" spans="1:1" ht="15.75">
-      <c r="A225" s="1"/>
-    </row>
-    <row r="226" spans="1:1" ht="15.75">
-      <c r="A226" s="1"/>
-    </row>
-    <row r="227" spans="1:1" ht="15.75">
-      <c r="A227" s="1"/>
-    </row>
-    <row r="228" spans="1:1" ht="15.75">
-      <c r="A228" s="1"/>
-    </row>
-    <row r="229" spans="1:1" ht="15.75">
-      <c r="A229" s="1"/>
-    </row>
-    <row r="230" spans="1:1" ht="15.75">
-      <c r="A230" s="1"/>
-    </row>
-    <row r="231" spans="1:1" ht="15.75">
-      <c r="A231" s="1"/>
-    </row>
-    <row r="232" spans="1:1" ht="15.75">
-      <c r="A232" s="1"/>
-    </row>
-    <row r="233" spans="1:1" ht="15.75">
-      <c r="A233" s="1"/>
-    </row>
-    <row r="234" spans="1:1" ht="15.75">
-      <c r="A234" s="1"/>
-    </row>
-    <row r="235" spans="1:1" ht="15.75">
-      <c r="A235" s="1"/>
-    </row>
-    <row r="236" spans="1:1" ht="15.75">
-      <c r="A236" s="1"/>
-    </row>
-    <row r="237" spans="1:1" ht="15.75">
-      <c r="A237" s="1"/>
-    </row>
-    <row r="238" spans="1:1" ht="15.75">
-      <c r="A238" s="1"/>
-    </row>
-    <row r="239" spans="1:1" ht="15.75">
-      <c r="A239" s="1"/>
-    </row>
-    <row r="240" spans="1:1" ht="15.75">
-      <c r="A240" s="1"/>
-    </row>
-    <row r="241" spans="1:1" ht="15.75">
-      <c r="A241" s="1"/>
-    </row>
-    <row r="242" spans="1:1" ht="15.75">
-      <c r="A242" s="1"/>
-    </row>
-    <row r="243" spans="1:1" ht="15.75">
-      <c r="A243" s="1"/>
-    </row>
-    <row r="244" spans="1:1" ht="15.75">
-      <c r="A244" s="1"/>
-    </row>
-    <row r="245" spans="1:1" ht="15.75">
-      <c r="A245" s="1"/>
-    </row>
-    <row r="246" spans="1:1" ht="15.75">
-      <c r="A246" s="1"/>
-    </row>
-    <row r="247" spans="1:1" ht="15.75">
-      <c r="A247" s="1"/>
-    </row>
-    <row r="248" spans="1:1" ht="15.75">
-      <c r="A248" s="1"/>
-    </row>
-    <row r="249" spans="1:1" ht="15.75">
-      <c r="A249" s="1"/>
-    </row>
-    <row r="250" spans="1:1" ht="15.75">
-      <c r="A250" s="1"/>
-    </row>
-    <row r="251" spans="1:1" ht="15.75">
-      <c r="A251" s="1"/>
-    </row>
-    <row r="252" spans="1:1" ht="15.75">
-      <c r="A252" s="1"/>
-    </row>
-    <row r="253" spans="1:1" ht="15.75">
-      <c r="A253" s="1"/>
-    </row>
-    <row r="254" spans="1:1" ht="15.75">
-      <c r="A254" s="1"/>
-    </row>
-    <row r="255" spans="1:1" ht="15.75">
-      <c r="A255" s="1"/>
-    </row>
-    <row r="256" spans="1:1" ht="15.75">
-      <c r="A256" s="1"/>
-    </row>
-    <row r="257" spans="1:1" ht="15.75">
-      <c r="A257" s="1"/>
-    </row>
-    <row r="258" spans="1:1" ht="15.75">
-      <c r="A258" s="1"/>
-    </row>
-    <row r="259" spans="1:1" ht="15.75">
-      <c r="A259" s="1"/>
-    </row>
-    <row r="260" spans="1:1" ht="15.75">
-      <c r="A260" s="1"/>
-    </row>
-    <row r="261" spans="1:1" ht="15.75">
-      <c r="A261" s="1"/>
-    </row>
-    <row r="262" spans="1:1" ht="15.75">
-      <c r="A262" s="1"/>
-    </row>
-    <row r="263" spans="1:1" ht="15.75">
-      <c r="A263" s="1"/>
-    </row>
-    <row r="264" spans="1:1" ht="15.75">
-      <c r="A264" s="1"/>
-    </row>
-    <row r="265" spans="1:1" ht="15.75">
-      <c r="A265" s="1"/>
-    </row>
-    <row r="266" spans="1:1" ht="15.75">
-      <c r="A266" s="1"/>
-    </row>
-    <row r="267" spans="1:1" ht="15.75">
-      <c r="A267" s="1"/>
-    </row>
-    <row r="268" spans="1:1" ht="15.75">
-      <c r="A268" s="1"/>
-    </row>
-    <row r="269" spans="1:1" ht="15.75">
-      <c r="A269" s="1"/>
-    </row>
-    <row r="270" spans="1:1" ht="15.75">
-      <c r="A270" s="1"/>
-    </row>
-    <row r="272" spans="1:1" ht="15.75">
-      <c r="A272" s="1"/>
-    </row>
-    <row r="501" spans="1:1">
-      <c r="A501" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="D3:D42">
-    <sortCondition ref="D3"/>
-  </sortState>
-  <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
* add custom formula
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="15" r:id="rId1"/>
+    <sheet name="first-error" sheetId="12" r:id="rId1"/>
     <sheet name="temp" sheetId="14" r:id="rId2"/>
     <sheet name="formula-math" sheetId="2" r:id="rId3"/>
     <sheet name="formula-logical" sheetId="4" r:id="rId4"/>
@@ -19,7 +19,6 @@
     <sheet name="formula-engineering" sheetId="10" r:id="rId10"/>
     <sheet name="formula-notsupported" sheetId="11" r:id="rId11"/>
     <sheet name="formula-custom" sheetId="13" r:id="rId12"/>
-    <sheet name="error" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$35</definedName>
@@ -41,7 +40,7 @@
     <author>Hawk</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1344,42 +1343,8 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Hawk</author>
-  </authors>
-  <commentList>
-    <comment ref="A4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Hawk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-not in doc</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="403">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2578,13 +2543,16 @@
     <t>1001</t>
   </si>
   <si>
-    <t>END OF FORMULA</t>
-  </si>
-  <si>
     <t>toTWD</t>
   </si>
   <si>
     <t>Custom</t>
+  </si>
+  <si>
+    <t>หนึ่งพันสองร้อยสามสิบสี่บาทถ้วน</t>
+  </si>
+  <si>
+    <t>USD2NTD</t>
   </si>
 </sst>
 </file>
@@ -2788,7 +2756,55 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3651,94 +3667,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <f>ASC("EXCEL")</f>
         <v>EXCEL</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>391</v>
       </c>
-      <c r="D2" t="str">
-        <f>IF(B2=C2,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="1" t="s">
+      <c r="D3" t="str">
+        <f>IF(B3=C3,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="5" t="str">
+      <c r="B5" s="5" t="str">
         <f>CHAR(65)</f>
         <v>A</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="D4" t="str">
-        <f>IF(B4=C4,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="1" t="s">
+      <c r="D5" t="str">
+        <f>IF(B5=C5,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B7" s="25">
         <f>BETADIST(2,8,10,1,3)</f>
         <v>0.68547058095349067</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>0.68547058095349067</v>
       </c>
-      <c r="D6" t="str">
-        <f>IF(B6=C6,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
-      <c r="A7" s="1"/>
+      <c r="D7" t="str">
+        <f>IF(B7=C7,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75">
+      <c r="A9" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B9" s="12">
         <f>BETAINV(0.6854,8,10,1,3)</f>
         <v>1.9999523162841797</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1.9999523162841797</v>
       </c>
-      <c r="D8" t="str">
-        <f>IF(B8=C8,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>399</v>
+      <c r="D9" t="str">
+        <f>IF(B9=C9,"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="D3:D5">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6 D8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="D7 D9">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3751,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4573,9 +4587,6 @@
       <c r="B78" s="24"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" t="s">
-        <v>399</v>
-      </c>
       <c r="B79" s="24"/>
     </row>
     <row r="80" spans="1:4" ht="15.75">
@@ -5174,37 +5185,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5215,10 +5226,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5241,12 +5252,12 @@
         <f>BAHTTEXT(1234)</f>
         <v>หนึ่งพันสองร้อยสามสิบสี่บาทถ้วน</v>
       </c>
-      <c r="C2" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D2" t="e">
+      <c r="C2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" t="str">
         <f>IF(B2=C2,"T","WARN")</f>
-        <v>#NAME?</v>
+        <v>T</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
@@ -5270,106 +5281,122 @@
       <c r="A6" t="s">
         <v>179</v>
       </c>
+      <c r="B6">
+        <f>EDATE(B7,1)</f>
+        <v>39493</v>
+      </c>
+      <c r="C6">
+        <v>39493</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(B6=C6,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>180</v>
+      <c r="B7" s="21">
+        <v>39462</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18.75">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:4" ht="18.75">
+      <c r="A10" s="4" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18.75">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:4" ht="18.75">
+      <c r="A18" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18.75">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:4" ht="18.75">
+      <c r="A20" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18.75">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:4" ht="18.75">
+      <c r="A23" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>397</v>
       </c>
-      <c r="B23" t="e">
+      <c r="B24" t="e">
         <f ca="1">abc()</f>
         <v>#NAME?</v>
       </c>
-      <c r="C23" t="e">
+      <c r="C24" t="e">
         <v>#NAME?</v>
       </c>
-      <c r="D23" t="str">
-        <f ca="1">IF(ISERR(B23),"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>399</v>
+      <c r="D24" t="str">
+        <f ca="1">IF(ISERR(B24),"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5380,10 +5407,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5396,7 +5423,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -5412,7 +5439,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B3" t="e">
         <f ca="1">toTWD(B4,C4)</f>
@@ -5434,19 +5461,58 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B6" t="e">
+        <f ca="1">USD2NTD(B7,C7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6" t="e">
+        <f ca="1">IF(B6=C6,"T","WARN")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5454,73 +5520,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:D8"/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" t="str">
-        <f>ASC("EXCEL")</f>
-        <v>EXCEL</v>
-      </c>
-      <c r="C4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D4" t="str">
-        <f>IF(B4=C4,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="5" t="str">
-        <f>CHAR(65)</f>
-        <v>A</v>
-      </c>
-      <c r="C6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(B6=C6,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D4:D6">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5595,19 +5600,14 @@
         <v>T</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>399</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6505,7 +6505,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>31.358356266281451</v>
+        <v>67.566944258413514</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -6523,7 +6523,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -7390,11 +7390,6 @@
       </c>
       <c r="D186" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="415" spans="1:1">
@@ -7410,7 +7405,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7427,7 +7422,7 @@
   <dimension ref="A1:I248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7613,11 +7608,6 @@
     <row r="19" spans="1:4" ht="15.75">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>399</v>
-      </c>
-    </row>
     <row r="248" spans="1:1">
       <c r="A248" s="3" t="s">
         <v>0</v>
@@ -7625,7 +7615,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7638,8 +7628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D5"/>
+    <sheetView topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8350,11 +8340,6 @@
       <c r="A74" s="1"/>
       <c r="C74" s="21"/>
     </row>
-    <row r="75" spans="1:4">
-      <c r="A75" t="s">
-        <v>399</v>
-      </c>
-    </row>
     <row r="79" spans="1:4">
       <c r="B79" s="11"/>
     </row>
@@ -8810,7 +8795,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8824,8 +8809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J451"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9243,11 +9228,6 @@
     <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>399</v>
-      </c>
-    </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="1"/>
     </row>
@@ -9801,17 +9781,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10034,7 +10014,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41400.624196296296</v>
+        <v>41400.702402662035</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -10186,9 +10166,6 @@
       <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>399</v>
-      </c>
       <c r="C39" s="21"/>
     </row>
     <row r="40" spans="1:4" ht="15.75">
@@ -10781,22 +10758,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10811,7 +10788,7 @@
   <dimension ref="A1:I534"/>
   <sheetViews>
     <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="H121" sqref="H121"/>
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12255,11 +12232,6 @@
     <row r="124" spans="1:7" ht="15.75">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:7">
-      <c r="A125" t="s">
-        <v>399</v>
-      </c>
-    </row>
     <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="1"/>
     </row>
@@ -12821,32 +12793,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12860,8 +12832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E19"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15699,11 +15671,6 @@
     <row r="201" spans="1:11" ht="15.75">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:11">
-      <c r="A202" t="s">
-        <v>399</v>
-      </c>
-    </row>
     <row r="203" spans="1:11" ht="15.75">
       <c r="A203" s="1"/>
     </row>
@@ -16291,67 +16258,67 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D14 D17 D19 D21 D23 D25 D27">
-    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
* mark spreadsheet unsupported formulas * make unsupported formulas pass test verification
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -1344,7 +1344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="406">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2553,6 +2553,15 @@
   </si>
   <si>
     <t>USD2NTD</t>
+  </si>
+  <si>
+    <t>unsupported</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -2756,7 +2765,103 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3747,12 +3852,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5185,37 +5290,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5226,10 +5331,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5237,6 +5342,8 @@
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
@@ -5255,9 +5362,8 @@
       <c r="C2" t="s">
         <v>401</v>
       </c>
-      <c r="D2" t="str">
-        <f>IF(B2=C2,"T","WARN")</f>
-        <v>T</v>
+      <c r="D2" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
@@ -5288,9 +5394,8 @@
       <c r="C6">
         <v>39493</v>
       </c>
-      <c r="D6" t="str">
-        <f>IF(B6=C6,"T","WARN")</f>
-        <v>T</v>
+      <c r="D6" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5302,11 +5407,31 @@
       <c r="A8" t="s">
         <v>180</v>
       </c>
+      <c r="B8" s="21">
+        <f>EOMONTH(DATE(2008,1,1),1)</f>
+        <v>39507</v>
+      </c>
+      <c r="C8" s="21">
+        <v>39507</v>
+      </c>
+      <c r="D8" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>182</v>
       </c>
+      <c r="B9">
+        <f>WEEKNUM(DATE(2008,3,9),1)</f>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="4" t="s">
@@ -5317,86 +5442,270 @@
       <c r="A11" t="s">
         <v>228</v>
       </c>
+      <c r="B11" s="25">
+        <f>MDURATION(DATE(2008,1,1),DATE(2016,1,1),0.08, 0.09, 2,1)</f>
+        <v>5.7356698139188387</v>
+      </c>
+      <c r="C11" s="25">
+        <v>5.7356698139188387</v>
+      </c>
+      <c r="D11" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>232</v>
       </c>
+      <c r="B12" s="25">
+        <f>ODDFPRICE(DATE(2008,11,11), DATE(2021,3,1), DATE(2008,10,15), DATE(2009,3,1), 0.0785, 0.0625, 100,2,1)</f>
+        <v>113.59771747407883</v>
+      </c>
+      <c r="C12" s="25">
+        <v>113.59771747407883</v>
+      </c>
+      <c r="D12" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>233</v>
       </c>
+      <c r="B13" s="25">
+        <f>ODDFYIELD(DATE(2008,11,11), DATE(2021,3,1), DATE(2008,10,15), DATE(2009,3,1), 0.0575, 84.5, 100,2,0)</f>
+        <v>7.7245541597298878E-2</v>
+      </c>
+      <c r="C13" s="25">
+        <v>7.7245541597298878E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>234</v>
       </c>
+      <c r="B14" s="25">
+        <f>ODDLPRICE(DATE(2008,2,7), DATE(2008,6,15), DATE(2007,10,15), 0.0375, 0.0405, 100, 2,0)</f>
+        <v>99.87828601472134</v>
+      </c>
+      <c r="C14" s="25">
+        <v>99.87828601472134</v>
+      </c>
+      <c r="D14" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>235</v>
       </c>
+      <c r="B15" s="25">
+        <f>ODDLYIELD(DATE(2008,4,20), DATE(2008,6,15), DATE(2007,12,24), 0.0375, 99.875, 100, 2,0)</f>
+        <v>4.5192235629169158E-2</v>
+      </c>
+      <c r="C15" s="25">
+        <v>4.5192235629169158E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="B16" s="25">
+        <f>TBILLPRICE(DATE(2008,3,31), DATE(2008,6,1),0.09)</f>
+        <v>98.45</v>
+      </c>
+      <c r="C16" s="25">
+        <v>98.45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="25">
+        <f>XIRR(B18:F18,B19:F19,0.1)</f>
+        <v>0.3733625352382659</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0.3733625352382659</v>
+      </c>
+      <c r="D17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18">
+        <v>-10000</v>
+      </c>
+      <c r="C18">
+        <v>2750</v>
+      </c>
+      <c r="D18">
+        <v>4250</v>
+      </c>
+      <c r="E18">
+        <v>3250</v>
+      </c>
+      <c r="F18">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" s="21">
+        <v>39448</v>
+      </c>
+      <c r="C19" s="21">
+        <v>39508</v>
+      </c>
+      <c r="D19" s="21">
+        <v>39751</v>
+      </c>
+      <c r="E19" s="21">
+        <v>39859</v>
+      </c>
+      <c r="F19" s="21">
+        <v>39904</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18.75">
+      <c r="A20" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75">
-      <c r="A20" s="4" t="s">
+      <c r="B21">
+        <f>COUNTIFS(B22:E22,"Yes")</f>
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" t="s">
+        <v>404</v>
+      </c>
+      <c r="C22" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" t="s">
+        <v>404</v>
+      </c>
+      <c r="E22" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75">
+      <c r="A23" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="18.75">
-      <c r="A23" s="4" t="s">
+      <c r="B24" s="25">
+        <f>CONVERT(1, "lbm", "kg")</f>
+        <v>0.45359230974881148</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0.45359230974881148</v>
+      </c>
+      <c r="D24" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18.75">
+      <c r="A26" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
         <v>397</v>
       </c>
-      <c r="B24" t="e">
+      <c r="B27" t="e">
         <f ca="1">abc()</f>
         <v>#NAME?</v>
       </c>
-      <c r="C24" t="e">
+      <c r="C27" t="e">
         <v>#NAME?</v>
       </c>
-      <c r="D24" t="str">
-        <f ca="1">IF(ISERR(B24),"T","WARN")</f>
-        <v>T</v>
+      <c r="D27" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D19 E18:F19">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D22 E22">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5409,7 +5718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -5487,27 +5796,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5602,12 +5911,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5620,8 +5929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I415"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="A188" sqref="A188"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6505,7 +6814,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>67.566944258413514</v>
+        <v>68.68161127813606</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -6523,7 +6832,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -6622,9 +6931,8 @@
       <c r="C104" s="11">
         <v>0.70710321482284566</v>
       </c>
-      <c r="D104" t="str">
-        <f>IF(B104=C104,"T","WARN")</f>
-        <v>T</v>
+      <c r="D104" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75">
@@ -7405,7 +7713,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7615,7 +7923,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8795,7 +9103,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9781,17 +10089,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10014,7 +10322,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41400.702402662035</v>
+        <v>41436.497227199077</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -10083,7 +10391,7 @@
       </c>
       <c r="B29" s="22">
         <f ca="1">TODAY()</f>
-        <v>41400</v>
+        <v>41436</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -10758,22 +11066,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10787,7 +11095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I534"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
@@ -12793,32 +13101,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12832,8 +13140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12985,9 +13293,8 @@
       <c r="C11">
         <v>14000</v>
       </c>
-      <c r="D11" t="str">
-        <f>IF(B11=C11,"T","WARN")</f>
-        <v>T</v>
+      <c r="D11" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75">
@@ -13021,9 +13328,8 @@
       <c r="C14">
         <v>87.5</v>
       </c>
-      <c r="D14" t="str">
-        <f>IF(B14=C14,"T","WARN")</f>
-        <v>T</v>
+      <c r="D14" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75">
@@ -16257,68 +16563,68 @@
   <sortState ref="D3:D50">
     <sortCondition ref="D50"/>
   </sortState>
-  <conditionalFormatting sqref="D3 D6 D8 D11 D14 D17 D19 D21 D23 D25 D27">
-    <cfRule type="cellIs" dxfId="30" priority="13" operator="equal">
+  <conditionalFormatting sqref="D3 D6 D8 D11 D17 D19 D21 D23 D25 D27 D14">
+    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="29" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
correct test case for SECOND(), use a cell reference instead of date string like help
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -2714,7 +2714,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2760,24 +2760,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3852,12 +3841,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5290,37 +5279,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5650,62 +5639,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D19 E18:F19">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D22 E22">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5796,32 +5785,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5911,12 +5900,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6814,7 +6803,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>68.68161127813606</v>
+        <v>89.10715326644312</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -6832,7 +6821,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -7713,7 +7702,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="54" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7923,7 +7912,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9103,7 +9092,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10089,17 +10078,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10112,8 +10101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D458"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10322,7 +10311,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41436.497227199077</v>
+        <v>41442.687667592596</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -10333,11 +10322,11 @@
         <v>173</v>
       </c>
       <c r="B23">
-        <f>SECOND("4:48 PM")</f>
-        <v>0</v>
+        <f>SECOND(B24)</f>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D23" t="str">
         <f>IF(B23=C23,"T","WARN")</f>
@@ -10346,6 +10335,9 @@
     </row>
     <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="1"/>
+      <c r="B24" s="39">
+        <v>0.70020833333333332</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="1" t="s">
@@ -10391,7 +10383,7 @@
       </c>
       <c r="B29" s="22">
         <f ca="1">TODAY()</f>
-        <v>41436</v>
+        <v>41442</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -11066,22 +11058,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13101,32 +13093,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13140,7 +13132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -16564,67 +16556,67 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D17 D19 D21 D23 D25 D27 D14">
-    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="37" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix test cases. use a cell reference for HOUR() and MINUTE() according to Excel's help
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -2757,10 +2757,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5943,17 +5943,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>89.10715326644312</v>
+        <v>60.275584961328079</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -6821,7 +6821,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -10101,8 +10101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D458"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10234,11 +10234,11 @@
         <v>169</v>
       </c>
       <c r="B13">
-        <f>HOUR("15:30")</f>
-        <v>15</v>
+        <f>HOUR(B14)</f>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D13" t="str">
         <f>IF(B13=C13,"T","WARN")</f>
@@ -10247,13 +10247,16 @@
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="1"/>
+      <c r="B14" s="38">
+        <v>0.14618055555555556</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
       <c r="B15">
-        <f>MINUTE("4:48:00 PM")</f>
+        <f>MINUTE(B16)</f>
         <v>48</v>
       </c>
       <c r="C15">
@@ -10266,6 +10269,9 @@
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="1"/>
+      <c r="B16" s="38">
+        <v>0.70000000000000007</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="1" t="s">
@@ -10311,7 +10317,7 @@
       </c>
       <c r="B21" s="23">
         <f ca="1">NOW()</f>
-        <v>41442.687667592596</v>
+        <v>41442.714560185188</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -10335,7 +10341,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="1"/>
-      <c r="B24" s="39">
+      <c r="B24" s="38">
         <v>0.70020833333333332</v>
       </c>
     </row>
@@ -10412,11 +10418,11 @@
       <c r="A33" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33" s="21">
         <f>WORKDAY(DATE(2013,4,1),5)</f>
         <v>41372</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="21">
         <v>41372</v>
       </c>
       <c r="D33" t="str">

</xml_diff>

<commit_message>
* add more test case for NETWORKDAYS and WORKDAY
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="formula-custom" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'formula-engineering'!$A$10:$C$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$10:$C$49</definedName>
@@ -191,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0">
+    <comment ref="A41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0">
+    <comment ref="A58" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1344,7 +1344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="416">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2562,6 +2562,36 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>start date is holiday</t>
+  </si>
+  <si>
+    <t>end date is holiday</t>
+  </si>
+  <si>
+    <t>negative workday, end date is holiday</t>
+  </si>
+  <si>
+    <t>boundary</t>
+  </si>
+  <si>
+    <t>specified holiday</t>
+  </si>
+  <si>
+    <t>all holidays</t>
+  </si>
+  <si>
+    <t>specified holidays</t>
+  </si>
+  <si>
+    <t>Formula Count</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>invalid, different spec</t>
   </si>
 </sst>
 </file>
@@ -2766,7 +2796,91 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -3841,12 +3955,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3859,8 +3973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5279,37 +5393,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5322,8 +5436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="B24:C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5639,62 +5753,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D19 E18:F19">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D22 E22">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5785,32 +5899,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5900,12 +6014,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6803,7 +6917,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>60.275584961328079</v>
+        <v>95.202640772771232</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -6821,7 +6935,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -7702,7 +7816,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="53" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7912,7 +8026,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9092,7 +9206,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10078,17 +10192,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5 D8 D10:D12 D15 D18 D21 D23 D26 D29 D31">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10099,15 +10213,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D458"/>
+  <dimension ref="A1:D479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
@@ -10310,266 +10424,492 @@
     </row>
     <row r="20" spans="1:4" ht="15.75">
       <c r="A20" s="1"/>
+      <c r="B20">
+        <f>NETWORKDAYS(DATE(2008,10,1), DATE(2009,3,1))</f>
+        <v>108</v>
+      </c>
+      <c r="C20">
+        <v>108</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" ref="D20:D25" si="0">IF(B20=C20,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B21">
+        <f>NETWORKDAYS(DATE(2013,6,1), DATE(2013,6,9))</f>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
+      <c r="A22" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B22">
+        <f>NETWORKDAYS(DATE(2013,6,1), DATE(2013,6,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" s="1"/>
+      <c r="B23">
+        <f>NETWORKDAYS(DATE(2013,6,1), DATE(2013,6,2))</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75">
+      <c r="A24" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B24">
+        <f>NETWORKDAYS(DATE(2008,10,1), DATE(2009,3,1), DATE(2008,11,26))</f>
+        <v>107</v>
+      </c>
+      <c r="C24">
+        <v>107</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
+      <c r="A25" s="1"/>
+      <c r="B25">
+        <f>NETWORKDAYS(DATE(2013,6,1), DATE(2013,6,4), DATE(2013,6,3))</f>
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
+      <c r="A26" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B26">
+        <f>NETWORKDAYS(DATE(2013,6,2), DATE(2013,6,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C26" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="D26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B29" s="23">
         <f ca="1">NOW()</f>
-        <v>41442.714560185188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75">
-      <c r="A23" s="1" t="s">
+        <v>41443.609986805553</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
+      <c r="A31" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B23">
-        <f>SECOND(B24)</f>
+      <c r="B31">
+        <f>SECOND(B32)</f>
         <v>18</v>
       </c>
-      <c r="C23">
+      <c r="C31">
         <v>18</v>
       </c>
-      <c r="D23" t="str">
-        <f>IF(B23=C23,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75">
-      <c r="A24" s="1"/>
-      <c r="B24" s="38">
+      <c r="D31" t="str">
+        <f>IF(B31=C31,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="1"/>
+      <c r="B32" s="38">
         <v>0.70020833333333332</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75">
-      <c r="A25" s="1" t="s">
+    <row r="33" spans="1:4" ht="15.75">
+      <c r="A33" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B33" s="18">
         <f>TIME(12,0,0)</f>
         <v>0.5</v>
       </c>
-      <c r="C25">
+      <c r="C33">
         <v>0.5</v>
       </c>
-      <c r="D25" t="str">
-        <f>IF(B25=C25,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75">
-      <c r="A27" s="1" t="s">
+      <c r="D33" t="str">
+        <f>IF(B33=C33,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75">
+      <c r="A35" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B35" s="5">
         <f>TIMEVALUE("2:24 AM")</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="C27">
+      <c r="C35">
         <v>0.1</v>
       </c>
-      <c r="D27" t="str">
-        <f>IF(B27=C27,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75">
-      <c r="A29" s="1" t="s">
+      <c r="D35" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B37" s="22">
         <f ca="1">TODAY()</f>
-        <v>41442</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75">
-      <c r="A31" s="1" t="s">
+        <v>41443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75">
+      <c r="A39" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B31">
+      <c r="B39">
         <f>WEEKDAY(DATE(2008,2,14))</f>
         <v>5</v>
       </c>
-      <c r="C31">
+      <c r="C39">
         <v>5</v>
       </c>
-      <c r="D31" t="str">
-        <f>IF(B31=C31,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75">
-      <c r="A33" s="1" t="s">
+      <c r="D39" t="str">
+        <f>IF(B39=C39,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
+      <c r="A41" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B41" s="21">
+        <f>WORKDAY(DATE(2013,4,1),4)</f>
+        <v>41369</v>
+      </c>
+      <c r="C41" s="21">
+        <v>41369</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" ref="D41:D44" si="1">IF(B41=C41,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" s="1"/>
+      <c r="B42" s="21">
+        <f>WORKDAY(DATE(2008,10,1),151)</f>
+        <v>39933</v>
+      </c>
+      <c r="C42" s="21">
+        <v>39933</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75">
+      <c r="A43" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B43" s="21">
+        <f>WORKDAY(DATE(2013,6,1),1)</f>
+        <v>41428</v>
+      </c>
+      <c r="C43" s="21">
+        <v>41428</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="1"/>
+      <c r="B44" s="21">
+        <f>WORKDAY(DATE(2013,6,1), -1)</f>
+        <v>41425</v>
+      </c>
+      <c r="C44" s="21">
+        <v>41425</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75">
+      <c r="A45" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B45" s="21">
         <f>WORKDAY(DATE(2013,4,1),5)</f>
         <v>41372</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C45" s="21">
         <v>41372</v>
       </c>
-      <c r="D33" t="str">
-        <f>IF(B33=C33,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75">
-      <c r="A35" s="1" t="s">
+      <c r="D45" t="str">
+        <f>IF(B45=C45,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75">
+      <c r="A46" s="1"/>
+      <c r="B46" s="21">
+        <f>WORKDAY(DATE(2013,4,5),1)</f>
+        <v>41372</v>
+      </c>
+      <c r="C46" s="21">
+        <v>41372</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" ref="D46:D53" si="2">IF(B46=C46,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75">
+      <c r="A47" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B47" s="21">
+        <f>WORKDAY(DATE(2013,4,1),-1)</f>
+        <v>41362</v>
+      </c>
+      <c r="C47" s="21">
+        <v>41362</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75">
+      <c r="A48" s="1"/>
+      <c r="B48" s="21">
+        <f>WORKDAY(DATE(2013,6,7),-5)</f>
+        <v>41425</v>
+      </c>
+      <c r="C48" s="21">
+        <v>41425</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75">
+      <c r="A49" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B49" s="21">
+        <f>WORKDAY(DATE(2013,4,1),0)</f>
+        <v>41365</v>
+      </c>
+      <c r="C49" s="21">
+        <v>41365</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75">
+      <c r="A50" s="1"/>
+      <c r="B50" s="21">
+        <f>WORKDAY(DATE(2013,6,1),0)</f>
+        <v>41426</v>
+      </c>
+      <c r="C50" s="21">
+        <v>41426</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75">
+      <c r="A51" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B51" s="21">
+        <f>WORKDAY(DATE(2013,4,1),3, DATE(2013,4,2))</f>
+        <v>41369</v>
+      </c>
+      <c r="C51" s="21">
+        <v>41369</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75">
+      <c r="A52" s="1"/>
+      <c r="B52" s="21">
+        <f>WORKDAY(DATE(2013,4,7), -3,DATE(2013,4,2))</f>
+        <v>41367</v>
+      </c>
+      <c r="C52" s="21">
+        <v>41367</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75">
+      <c r="A53" s="1"/>
+      <c r="B53" s="21">
+        <f>WORKDAY(DATE(2013,4,3), -1,DATE(2013,4,2))</f>
+        <v>41365</v>
+      </c>
+      <c r="C53" s="21">
+        <v>41365</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B35">
+      <c r="B56">
         <f>YEAR(DATE(2008,1,1))</f>
         <v>2008</v>
       </c>
-      <c r="C35">
+      <c r="C56">
         <v>2008</v>
       </c>
-      <c r="D35" t="str">
-        <f>IF(B35=C35,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75">
-      <c r="A37" s="1" t="s">
+      <c r="D56" t="str">
+        <f>IF(B56=C56,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B58" s="25">
         <f>YEARFRAC(DATE(2012,1,1),DATE(2012,7,30))</f>
         <v>0.5805555555555556</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C58" s="25">
         <v>0.5805555555555556</v>
       </c>
-      <c r="D37" t="str">
-        <f>IF(B37=C37,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="C39" s="21"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.75">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.75">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.75">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.75">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.75">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.75">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.75">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.75">
+      <c r="D58" t="str">
+        <f>IF(B58=C58,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75">
       <c r="A59" s="1"/>
-      <c r="B59" s="5"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.75">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:2" ht="15.75">
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C60" s="24">
+        <v>33</v>
+      </c>
+      <c r="D60" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75">
       <c r="A61" s="1"/>
-      <c r="B61" s="5"/>
-    </row>
-    <row r="62" spans="1:2" ht="15.75">
+    </row>
+    <row r="62" spans="1:4" ht="15.75">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:2" ht="15.75">
-      <c r="A63" s="1"/>
-      <c r="B63" s="5"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.75">
+    <row r="63" spans="1:4">
+      <c r="D63" s="21"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:2" ht="15.75">
       <c r="A65" s="1"/>
-      <c r="B65" s="5"/>
     </row>
     <row r="66" spans="1:2" ht="15.75">
       <c r="A66" s="1"/>
     </row>
     <row r="67" spans="1:2" ht="15.75">
       <c r="A67" s="1"/>
-      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2" ht="15.75">
       <c r="A68" s="1"/>
     </row>
     <row r="69" spans="1:2" ht="15.75">
       <c r="A69" s="1"/>
-      <c r="B69" s="8"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.75">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:2" ht="15.75">
-      <c r="A71" s="1"/>
-      <c r="B71" s="5"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.75">
-      <c r="A72" s="1"/>
     </row>
     <row r="73" spans="1:2" ht="15.75">
       <c r="A73" s="1"/>
@@ -10594,149 +10934,150 @@
     </row>
     <row r="80" spans="1:2" ht="15.75">
       <c r="A80" s="1"/>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" ht="15.75">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:2" ht="15.75">
       <c r="A82" s="1"/>
+      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" ht="15.75">
       <c r="A83" s="1"/>
     </row>
     <row r="84" spans="1:2" ht="15.75">
       <c r="A84" s="1"/>
+      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" ht="15.75">
       <c r="A85" s="1"/>
     </row>
     <row r="86" spans="1:2" ht="15.75">
       <c r="A86" s="1"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" ht="15.75">
       <c r="A87" s="1"/>
     </row>
     <row r="88" spans="1:2" ht="15.75">
       <c r="A88" s="1"/>
+      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" ht="15.75">
       <c r="A89" s="1"/>
     </row>
     <row r="90" spans="1:2" ht="15.75">
       <c r="A90" s="1"/>
+      <c r="B90" s="8"/>
     </row>
     <row r="91" spans="1:2" ht="15.75">
       <c r="A91" s="1"/>
     </row>
     <row r="92" spans="1:2" ht="15.75">
       <c r="A92" s="1"/>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" ht="15.75">
       <c r="A93" s="1"/>
-      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" ht="15.75">
       <c r="A94" s="1"/>
     </row>
     <row r="95" spans="1:2" ht="15.75">
       <c r="A95" s="1"/>
-      <c r="B95" s="5"/>
     </row>
     <row r="96" spans="1:2" ht="15.75">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:2">
-      <c r="B97" s="5"/>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="B99" s="5"/>
-    </row>
-    <row r="101" spans="1:2" ht="15.75">
+    <row r="97" spans="1:1" ht="15.75">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" ht="15.75">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" ht="15.75">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" ht="15.75">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" ht="15.75">
       <c r="A101" s="1"/>
-      <c r="B101" s="8"/>
-    </row>
-    <row r="102" spans="1:2" ht="15.75">
+    </row>
+    <row r="102" spans="1:1" ht="15.75">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:2" ht="15.75">
+    <row r="103" spans="1:1" ht="15.75">
       <c r="A103" s="1"/>
-      <c r="B103" s="5"/>
-    </row>
-    <row r="104" spans="1:2" ht="15.75">
+    </row>
+    <row r="104" spans="1:1" ht="15.75">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:2" ht="15.75">
+    <row r="105" spans="1:1" ht="15.75">
       <c r="A105" s="1"/>
-      <c r="B105" s="5"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.75">
+    </row>
+    <row r="106" spans="1:1" ht="15.75">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:2" ht="15.75">
+    <row r="107" spans="1:1" ht="15.75">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:2" ht="15.75">
+    <row r="108" spans="1:1" ht="15.75">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:2" ht="15.75">
+    <row r="109" spans="1:1" ht="15.75">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:2" ht="15.75">
+    <row r="110" spans="1:1" ht="15.75">
       <c r="A110" s="1"/>
-      <c r="B110" s="5"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.75">
+    </row>
+    <row r="111" spans="1:1" ht="15.75">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:2" ht="15.75">
+    <row r="112" spans="1:1" ht="15.75">
       <c r="A112" s="1"/>
-      <c r="B112" s="11"/>
     </row>
     <row r="113" spans="1:2" ht="15.75">
       <c r="A113" s="1"/>
     </row>
     <row r="114" spans="1:2" ht="15.75">
       <c r="A114" s="1"/>
-      <c r="B114" s="9"/>
+      <c r="B114" s="5"/>
     </row>
     <row r="115" spans="1:2" ht="15.75">
       <c r="A115" s="1"/>
     </row>
     <row r="116" spans="1:2" ht="15.75">
       <c r="A116" s="1"/>
+      <c r="B116" s="5"/>
     </row>
     <row r="117" spans="1:2" ht="15.75">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:2" ht="15.75">
-      <c r="A118" s="1"/>
+    <row r="118" spans="1:2">
       <c r="B118" s="5"/>
     </row>
-    <row r="119" spans="1:2" ht="15.75">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.75">
-      <c r="A120" s="1"/>
+    <row r="120" spans="1:2">
       <c r="B120" s="5"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.75">
-      <c r="A121" s="1"/>
     </row>
     <row r="122" spans="1:2" ht="15.75">
       <c r="A122" s="1"/>
+      <c r="B122" s="8"/>
     </row>
     <row r="123" spans="1:2" ht="15.75">
       <c r="A123" s="1"/>
     </row>
     <row r="124" spans="1:2" ht="15.75">
       <c r="A124" s="1"/>
+      <c r="B124" s="5"/>
     </row>
     <row r="125" spans="1:2" ht="15.75">
       <c r="A125" s="1"/>
     </row>
     <row r="126" spans="1:2" ht="15.75">
       <c r="A126" s="1"/>
-      <c r="B126" s="8"/>
+      <c r="B126" s="5"/>
     </row>
     <row r="127" spans="1:2" ht="15.75">
       <c r="A127" s="1"/>
@@ -10752,26 +11093,27 @@
     </row>
     <row r="131" spans="1:2" ht="15.75">
       <c r="A131" s="1"/>
+      <c r="B131" s="5"/>
     </row>
     <row r="132" spans="1:2" ht="15.75">
       <c r="A132" s="1"/>
     </row>
     <row r="133" spans="1:2" ht="15.75">
       <c r="A133" s="1"/>
+      <c r="B133" s="11"/>
     </row>
     <row r="134" spans="1:2" ht="15.75">
       <c r="A134" s="1"/>
     </row>
     <row r="135" spans="1:2" ht="15.75">
       <c r="A135" s="1"/>
-      <c r="B135" s="12"/>
+      <c r="B135" s="9"/>
     </row>
     <row r="136" spans="1:2" ht="15.75">
       <c r="A136" s="1"/>
     </row>
     <row r="137" spans="1:2" ht="15.75">
       <c r="A137" s="1"/>
-      <c r="B137" s="8"/>
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="1"/>
@@ -10785,7 +11127,7 @@
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="1"/>
-      <c r="B141" s="11"/>
+      <c r="B141" s="5"/>
     </row>
     <row r="142" spans="1:2" ht="15.75">
       <c r="A142" s="1"/>
@@ -10796,59 +11138,64 @@
     <row r="144" spans="1:2" ht="15.75">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" ht="15.75">
+    <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" ht="15.75">
+    <row r="146" spans="1:2" ht="15.75">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" ht="15.75">
+    <row r="147" spans="1:2" ht="15.75">
       <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" ht="15.75">
+      <c r="B147" s="8"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.75">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" ht="15.75">
+    <row r="149" spans="1:2" ht="15.75">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" ht="15.75">
+    <row r="150" spans="1:2" ht="15.75">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" ht="15.75">
+    <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" ht="15.75">
+    <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" ht="15.75">
+    <row r="153" spans="1:2" ht="15.75">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" ht="15.75">
+    <row r="154" spans="1:2" ht="15.75">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" ht="15.75">
+    <row r="155" spans="1:2" ht="15.75">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" ht="15.75">
+    <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:1" ht="15.75">
+      <c r="B156" s="12"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.75">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" ht="15.75">
+    <row r="158" spans="1:2" ht="15.75">
       <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:1" ht="15.75">
+      <c r="B158" s="8"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.75">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" ht="15.75">
+    <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="1"/>
+      <c r="B160" s="5"/>
     </row>
     <row r="161" spans="1:2" ht="15.75">
       <c r="A161" s="1"/>
     </row>
     <row r="162" spans="1:2" ht="15.75">
       <c r="A162" s="1"/>
+      <c r="B162" s="11"/>
     </row>
     <row r="163" spans="1:2" ht="15.75">
       <c r="A163" s="1"/>
@@ -10879,7 +11226,6 @@
     </row>
     <row r="172" spans="1:2" ht="15.75">
       <c r="A172" s="1"/>
-      <c r="B172" s="5"/>
     </row>
     <row r="173" spans="1:2" ht="15.75">
       <c r="A173" s="1"/>
@@ -10889,7 +11235,6 @@
     </row>
     <row r="175" spans="1:2" ht="15.75">
       <c r="A175" s="1"/>
-      <c r="B175" s="5"/>
     </row>
     <row r="176" spans="1:2" ht="15.75">
       <c r="A176" s="1"/>
@@ -10944,6 +11289,7 @@
     </row>
     <row r="193" spans="1:2" ht="15.75">
       <c r="A193" s="1"/>
+      <c r="B193" s="5"/>
     </row>
     <row r="194" spans="1:2" ht="15.75">
       <c r="A194" s="1"/>
@@ -10953,6 +11299,7 @@
     </row>
     <row r="196" spans="1:2" ht="15.75">
       <c r="A196" s="1"/>
+      <c r="B196" s="5"/>
     </row>
     <row r="197" spans="1:2" ht="15.75">
       <c r="A197" s="1"/>
@@ -10971,22 +11318,18 @@
     </row>
     <row r="202" spans="1:2" ht="15.75">
       <c r="A202" s="1"/>
-      <c r="B202" s="11"/>
     </row>
     <row r="203" spans="1:2" ht="15.75">
       <c r="A203" s="1"/>
     </row>
     <row r="204" spans="1:2" ht="15.75">
       <c r="A204" s="1"/>
-      <c r="B204" s="11"/>
     </row>
     <row r="205" spans="1:2" ht="15.75">
       <c r="A205" s="1"/>
-      <c r="B205" s="11"/>
     </row>
     <row r="206" spans="1:2" ht="15.75">
       <c r="A206" s="1"/>
-      <c r="B206" s="5"/>
     </row>
     <row r="207" spans="1:2" ht="15.75">
       <c r="A207" s="1"/>
@@ -10994,68 +11337,135 @@
     <row r="208" spans="1:2" ht="15.75">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" spans="1:1" ht="15.75">
+    <row r="209" spans="1:2" ht="15.75">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" spans="1:1" ht="15.75">
+    <row r="210" spans="1:2" ht="15.75">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" spans="1:1" ht="15.75">
+    <row r="211" spans="1:2" ht="15.75">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" spans="1:1" ht="15.75">
+    <row r="212" spans="1:2" ht="15.75">
       <c r="A212" s="1"/>
     </row>
-    <row r="213" spans="1:1" ht="15.75">
+    <row r="213" spans="1:2" ht="15.75">
       <c r="A213" s="1"/>
     </row>
-    <row r="214" spans="1:1" ht="15.75">
+    <row r="214" spans="1:2" ht="15.75">
       <c r="A214" s="1"/>
     </row>
-    <row r="215" spans="1:1" ht="15.75">
+    <row r="215" spans="1:2" ht="15.75">
       <c r="A215" s="1"/>
     </row>
-    <row r="216" spans="1:1" ht="15.75">
+    <row r="216" spans="1:2" ht="15.75">
       <c r="A216" s="1"/>
     </row>
-    <row r="217" spans="1:1" ht="15.75">
+    <row r="217" spans="1:2" ht="15.75">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" spans="1:1" ht="15.75">
+    <row r="218" spans="1:2" ht="15.75">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" spans="1:1" ht="15.75">
+    <row r="219" spans="1:2" ht="15.75">
       <c r="A219" s="1"/>
     </row>
-    <row r="220" spans="1:1" ht="15.75">
+    <row r="220" spans="1:2" ht="15.75">
       <c r="A220" s="1"/>
     </row>
-    <row r="221" spans="1:1" ht="15.75">
+    <row r="221" spans="1:2" ht="15.75">
       <c r="A221" s="1"/>
     </row>
-    <row r="222" spans="1:1" ht="15.75">
+    <row r="222" spans="1:2" ht="15.75">
       <c r="A222" s="1"/>
     </row>
-    <row r="223" spans="1:1" ht="15.75">
+    <row r="223" spans="1:2" ht="15.75">
       <c r="A223" s="1"/>
-    </row>
-    <row r="224" spans="1:1" ht="15.75">
+      <c r="B223" s="11"/>
+    </row>
+    <row r="224" spans="1:2" ht="15.75">
       <c r="A224" s="1"/>
     </row>
-    <row r="225" spans="1:1" ht="15.75">
+    <row r="225" spans="1:2" ht="15.75">
       <c r="A225" s="1"/>
-    </row>
-    <row r="226" spans="1:1" ht="15.75">
+      <c r="B225" s="11"/>
+    </row>
+    <row r="226" spans="1:2" ht="15.75">
       <c r="A226" s="1"/>
-    </row>
-    <row r="227" spans="1:1" ht="15.75">
+      <c r="B226" s="11"/>
+    </row>
+    <row r="227" spans="1:2" ht="15.75">
       <c r="A227" s="1"/>
-    </row>
-    <row r="229" spans="1:1" ht="15.75">
+      <c r="B227" s="5"/>
+    </row>
+    <row r="228" spans="1:2" ht="15.75">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:2" ht="15.75">
       <c r="A229" s="1"/>
     </row>
-    <row r="458" spans="1:1">
-      <c r="A458" s="3" t="s">
+    <row r="230" spans="1:2" ht="15.75">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:2" ht="15.75">
+      <c r="A231" s="1"/>
+    </row>
+    <row r="232" spans="1:2" ht="15.75">
+      <c r="A232" s="1"/>
+    </row>
+    <row r="233" spans="1:2" ht="15.75">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:2" ht="15.75">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:2" ht="15.75">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:2" ht="15.75">
+      <c r="A236" s="1"/>
+    </row>
+    <row r="237" spans="1:2" ht="15.75">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:2" ht="15.75">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="239" spans="1:2" ht="15.75">
+      <c r="A239" s="1"/>
+    </row>
+    <row r="240" spans="1:2" ht="15.75">
+      <c r="A240" s="1"/>
+    </row>
+    <row r="241" spans="1:1" ht="15.75">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" ht="15.75">
+      <c r="A242" s="1"/>
+    </row>
+    <row r="243" spans="1:1" ht="15.75">
+      <c r="A243" s="1"/>
+    </row>
+    <row r="244" spans="1:1" ht="15.75">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="245" spans="1:1" ht="15.75">
+      <c r="A245" s="1"/>
+    </row>
+    <row r="246" spans="1:1" ht="15.75">
+      <c r="A246" s="1"/>
+    </row>
+    <row r="247" spans="1:1" ht="15.75">
+      <c r="A247" s="1"/>
+    </row>
+    <row r="248" spans="1:1" ht="15.75">
+      <c r="A248" s="1"/>
+    </row>
+    <row r="250" spans="1:1" ht="15.75">
+      <c r="A250" s="1"/>
+    </row>
+    <row r="479" spans="1:1">
+      <c r="A479" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -11063,23 +11473,8 @@
   <sortState ref="A3:A29">
     <sortCondition ref="A3"/>
   </sortState>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19">
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33">
-    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6 D8 D10 D13 D15 D17 D19 D23 D25 D27 D31 D33 D35 D37">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+  <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D31 D33 D39 D56 D35 D58:D60 D41:D53 D19:D27">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11093,7 +11488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I534"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
@@ -13099,32 +13494,32 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16562,67 +16957,67 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D17 D19 D21 D23 D25 D27 D14">
-    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D37 D41 D43 D45 D47 D50">
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D129 D131 D133 D136 D138 D140 D142 D144">
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
mark STDEVP as unsupported
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -1354,7 +1354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="416">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2777,1975 +2777,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="371">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="207">
     <dxf>
       <font>
         <condense val="0"/>
@@ -7608,12 +5640,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="370" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="369" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9046,37 +7078,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="344" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="343" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="342" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="341" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="340" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="339" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="338" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9442,87 +7474,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="46" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="45" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="43" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9614,32 +7646,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="337" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="336" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="335" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="334" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="333" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="332" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9729,12 +7761,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="368" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="367" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10632,7 +8664,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>1.6268346978346004</v>
+        <v>20.034945987855846</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -10650,7 +8682,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -11531,7 +9563,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="366" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11741,7 +9773,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="365" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11754,7 +9786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -12898,7 +10930,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D72">
-    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13858,17 +11890,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8:D10 D13 D16 D19 D21 D24 D27 D29">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D36 D39 D41">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14205,7 +12237,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41443.728476388889</v>
+        <v>41444.624134490739</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -14276,7 +12308,7 @@
       </c>
       <c r="B37" s="19">
         <f ca="1">TODAY()</f>
-        <v>41443</v>
+        <v>41444</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75">
@@ -15140,7 +13172,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D31 D33 D39 D56 D35 D58:D60 D41:D53 D19:D27">
-    <cfRule type="cellIs" dxfId="364" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17156,62 +15188,62 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="363" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="362" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="361" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="360" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="359" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="358" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="319" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="317" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="315" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="313" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D113">
-    <cfRule type="cellIs" dxfId="311" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D113">
-    <cfRule type="cellIs" dxfId="309" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17225,8 +15257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19532,9 +17564,8 @@
       <c r="C168" s="22">
         <v>26.054558142482477</v>
       </c>
-      <c r="D168" t="str">
-        <f>IF(B168=C168,"T","WARN")</f>
-        <v>T</v>
+      <c r="D168" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="15.75">
@@ -20615,726 +18646,746 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="357" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="356" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="355" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="354" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="353" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="352" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="351" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="350" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="349" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="348" priority="136" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D164 D166 D168 D170 D172">
-    <cfRule type="cellIs" dxfId="347" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="140" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D164 D166 D170 D172 D168">
+    <cfRule type="cellIs" dxfId="173" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="346" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="345" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="331" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="306" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="303" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="300" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="298" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="296" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="293" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="291" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="288" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="286" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="283" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="281" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="279" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="277" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="275" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="273" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="271" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="269" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="267" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="265" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="263" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="261" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="259" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="257" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="255" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="253" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="251" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="249" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="247" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="245" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="243" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="241" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="239" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="237" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="235" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="233" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="231" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="228" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="226" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="224" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="222" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="219" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="217" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="215" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="213" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="210" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="208" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="206" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="204" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="201" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="199" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="197" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="195" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="192" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="190" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="188" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="186" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="183" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="181" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="179" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="177" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="174" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="172" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="170" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="168" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="166" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="164" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="162" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="160" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="158" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="156" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="154" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="152" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="150" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="148" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="146" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="144" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="142" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="140" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="138" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="136" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="134" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="132" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="130" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="128" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="126" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="124" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="122" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="120" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="118" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="116" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="114" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="112" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="110" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="108" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="106" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="104" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="102" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="100" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="98" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="96" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="94" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="92" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="90" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="88" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="86" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="84" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="82" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="80" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="78" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="74" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="72" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="70" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="62" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D166">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D166">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D166">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D168">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D166">
+  <conditionalFormatting sqref="D168">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D166">
+  <conditionalFormatting sqref="D168">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D166">
+  <conditionalFormatting sqref="D168">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>

</xml_diff>

<commit_message>
ZSS-269 error evaluating some financial formulas change cell format setting to eliminate format difference of evaluation result, and financial test cases can pass.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -393,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A101" authorId="0">
+    <comment ref="A102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A113" authorId="0">
+    <comment ref="A114" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2608,14 +2608,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;NT$&quot;#,##0.00;[Red]\-&quot;NT$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="167" formatCode="0.00_ ;[Red]\-0.00\ "/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0_ ;[Red]\-0\ "/>
     <numFmt numFmtId="170" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12">
@@ -2728,7 +2725,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2754,12 +2751,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2777,55 +2771,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="207">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="203">
     <dxf>
       <font>
         <condense val="0"/>
@@ -5560,10 +5506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5571,6 +5517,12 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="15">
+        <f>NPV(0.08,8000,9200,10000,12000,14500)</f>
+        <v>41922.06155493237</v>
+      </c>
+    </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>124</v>
@@ -5640,12 +5592,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="206" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="205" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5819,7 +5771,7 @@
         <f>BIN2OCT(1001,3)</f>
         <v>011</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="29" t="s">
         <v>368</v>
       </c>
       <c r="D15" t="str">
@@ -5882,7 +5834,7 @@
         <f>DEC2HEX(100,4)</f>
         <v>0064</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="29" t="s">
         <v>371</v>
       </c>
       <c r="D21" t="str">
@@ -5903,7 +5855,7 @@
         <f>DEC2OCT(58,3)</f>
         <v>072</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="29" t="s">
         <v>372</v>
       </c>
       <c r="D23" t="str">
@@ -5941,7 +5893,7 @@
       <c r="A27" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="27">
         <f>ERF(0.745)</f>
         <v>0.70792869314881979</v>
       </c>
@@ -6008,7 +5960,7 @@
         <f>HEX2BIN("F",8)</f>
         <v>00001111</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="29" t="s">
         <v>373</v>
       </c>
       <c r="D33" t="str">
@@ -6050,7 +6002,7 @@
         <f>HEX2OCT("F",3)</f>
         <v>017</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="29" t="s">
         <v>374</v>
       </c>
       <c r="D37" t="str">
@@ -6425,7 +6377,7 @@
         <f>OCT2BIN(3, 3)</f>
         <v>011</v>
       </c>
-      <c r="C73" s="32" t="s">
+      <c r="C73" s="29" t="s">
         <v>368</v>
       </c>
       <c r="D73" t="str">
@@ -6467,7 +6419,7 @@
         <f>OCT2HEX(100, 4)</f>
         <v>0040</v>
       </c>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="29" t="s">
         <v>387</v>
       </c>
       <c r="D77" t="str">
@@ -7078,37 +7030,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7140,7 +7092,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>124</v>
       </c>
       <c r="B2" t="str">
@@ -7170,13 +7122,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="30" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>388</v>
       </c>
       <c r="B5" s="11"/>
@@ -7474,87 +7426,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7646,32 +7598,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7681,17 +7633,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="22"/>
+    </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>124</v>
@@ -7761,12 +7714,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7804,17 +7757,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -7860,7 +7813,7 @@
         <f>ACOS(-0.5)</f>
         <v>2.0943951023931957</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="31">
         <v>2.0943951023931957</v>
       </c>
       <c r="D7" t="str">
@@ -7914,7 +7867,7 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="27">
         <f>ASINH(-2.5)</f>
         <v>-1.6472311463710965</v>
       </c>
@@ -7933,7 +7886,7 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="27">
         <f>ATAN(1)</f>
         <v>0.78539816339744828</v>
       </c>
@@ -7952,11 +7905,11 @@
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="27">
         <f>ATAN2(1, 1)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="27">
         <v>0.78539816339744828</v>
       </c>
       <c r="D17" t="str">
@@ -7971,7 +7924,7 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="27">
         <f>ATANH(0.76159416)</f>
         <v>1.0000000096297197</v>
       </c>
@@ -8028,7 +7981,7 @@
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="27">
         <f>COS(1.047)</f>
         <v>0.50017107459707011</v>
       </c>
@@ -8047,7 +8000,7 @@
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="27">
         <f>COSH(4)</f>
         <v>27.308232836016487</v>
       </c>
@@ -8664,7 +8617,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>20.034945987855846</v>
+        <v>23.153652570547266</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8682,7 +8635,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9563,7 +9516,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="202" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9773,7 +9726,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10930,7 +10883,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D72">
-    <cfRule type="cellIs" dxfId="200" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11890,17 +11843,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8:D10 D13 D16 D19 D21 D24 D27 D29">
-    <cfRule type="cellIs" dxfId="199" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D36 D39 D41">
-    <cfRule type="cellIs" dxfId="198" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="197" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12059,7 +12012,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="1"/>
-      <c r="B14" s="35">
+      <c r="B14" s="32">
         <v>0.14618055555555556</v>
       </c>
     </row>
@@ -12081,7 +12034,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="1"/>
-      <c r="B16" s="35">
+      <c r="B16" s="32">
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -12237,7 +12190,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41444.624134490739</v>
+        <v>41446.401156018517</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -12261,7 +12214,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="1"/>
-      <c r="B32" s="35">
+      <c r="B32" s="32">
         <v>0.70020833333333332</v>
       </c>
     </row>
@@ -12308,7 +12261,7 @@
       </c>
       <c r="B37" s="19">
         <f ca="1">TODAY()</f>
-        <v>41444</v>
+        <v>41446</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75">
@@ -13172,7 +13125,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D31 D33 D39 D56 D35 D58:D60 D41:D53 D19:D27">
-    <cfRule type="cellIs" dxfId="196" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13184,10 +13137,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I534"/>
+  <dimension ref="A1:I536"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13693,7 +13646,7 @@
       <c r="A42" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B42" s="23">
+      <c r="B42" s="22">
         <f>DDB(B43,C43,D43*365,1)</f>
         <v>1.3150684931506849</v>
       </c>
@@ -13864,7 +13817,7 @@
       <c r="A57" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B57" s="24">
+      <c r="B57" s="22">
         <f>FV(B58/12,C58,D58,E58,F58)</f>
         <v>2581.4033740601185</v>
       </c>
@@ -13988,11 +13941,11 @@
       <c r="A67" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B67" s="26">
+      <c r="B67" s="24">
         <f>IRR(B68:F68)</f>
         <v>-2.1244848273020495E-2</v>
       </c>
-      <c r="C67" s="26">
+      <c r="C67" s="24">
         <v>-2.1244848273020495E-2</v>
       </c>
       <c r="D67" t="str">
@@ -14121,11 +14074,11 @@
       <c r="A78" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B78" s="25">
+      <c r="B78" s="23">
         <f>MIRR(B79:G79,H79,I79)</f>
         <v>0.12609413036590511</v>
       </c>
-      <c r="C78" s="25">
+      <c r="C78" s="23">
         <v>0.12609413036590511</v>
       </c>
       <c r="D78" t="s">
@@ -14228,7 +14181,7 @@
       <c r="A87" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B87" s="24">
+      <c r="B87" s="22">
         <f>NPV(0.08,8000,9200,10000,12000,14500)</f>
         <v>41922.06155493237</v>
       </c>
@@ -14247,7 +14200,7 @@
       <c r="A89" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B89" s="24">
+      <c r="B89" s="22">
         <f>PMT(0.08/12,10,10000)</f>
         <v>-1037.0320893591606</v>
       </c>
@@ -14266,7 +14219,7 @@
       <c r="A91" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B91" s="24">
+      <c r="B91" s="22">
         <f>PPMT(0.1/12,1,2*12,2000)</f>
         <v>-75.623186008366716</v>
       </c>
@@ -14346,257 +14299,260 @@
       <c r="A99" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B99" s="24">
+      <c r="B99" s="22">
+        <f>PV(0.08/12,20*12,500,0,0)</f>
+        <v>-59777.145851187823</v>
+      </c>
+      <c r="C99" s="22">
+        <v>-59777.145851187823</v>
+      </c>
+      <c r="D99" t="str">
+        <f>IF(B99=C99,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15.75">
+      <c r="A100" s="1"/>
+      <c r="B100" s="22">
         <f>PV(0.08/12,20*12,500,,0)</f>
         <v>-59777.145851187823</v>
       </c>
-      <c r="C99" s="22">
-        <v>-59777.145851187823</v>
-      </c>
-      <c r="D99" t="str">
-        <f>IF(B99=C99,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="15.75">
-      <c r="A100" s="1"/>
-      <c r="B100" s="5"/>
+      <c r="C100" s="22" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D100" t="e">
+        <f>IF(B100=C100,"T","WARN")</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="15.75">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="1"/>
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="1:4" ht="15.75">
+      <c r="A102" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B101" s="27">
+      <c r="B102" s="25">
         <f>RATE(4*12,-200,8000)</f>
         <v>7.7014724882013682E-3</v>
       </c>
-      <c r="C101" s="25">
+      <c r="C102" s="23">
         <v>7.7014724882013682E-3</v>
       </c>
-      <c r="D101" t="str">
-        <f>IF(B101=C101,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75">
-      <c r="A102" s="1"/>
-      <c r="B102" s="5"/>
+      <c r="D102" t="str">
+        <f>IF(B102=C102,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="103" spans="1:4" ht="15.75">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="1"/>
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="1:4" ht="15.75">
+      <c r="A104" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B103" s="22">
+      <c r="B104" s="22">
         <f>RECEIVED(DATE(2008,2,15),DATE(2008,5,15),1000000,0.0575,2)</f>
         <v>1014584.6544071021</v>
       </c>
-      <c r="C103" s="22">
+      <c r="C104" s="22">
         <v>1014584.6544071021</v>
       </c>
-      <c r="D103" t="str">
-        <f>IF(B103=C103,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75">
-      <c r="A104" s="1"/>
-      <c r="B104" s="8"/>
+      <c r="D104" t="str">
+        <f>IF(B104=C104,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="15.75">
-      <c r="A105" s="1" t="s">
+      <c r="A105" s="1"/>
+      <c r="B105" s="8"/>
+    </row>
+    <row r="106" spans="1:4" ht="15.75">
+      <c r="A106" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B105" s="28">
+      <c r="B106" s="12">
         <f>SLN(30000,7500,10)</f>
         <v>2250</v>
       </c>
-      <c r="C105">
+      <c r="C106">
         <v>2250</v>
       </c>
-      <c r="D105" t="str">
-        <f>IF(B105=C105,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75">
-      <c r="A106" s="1"/>
-      <c r="B106" s="5"/>
+      <c r="D106" t="str">
+        <f>IF(B106=C106,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="107" spans="1:4" ht="15.75">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="1"/>
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="1:4" ht="15.75">
+      <c r="A108" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B107" s="24">
+      <c r="B108" s="22">
         <f>SYD(30000,7500,10,1)</f>
         <v>4090.909090909091</v>
       </c>
-      <c r="C107" s="22">
+      <c r="C108" s="22">
         <v>4090.909090909091</v>
       </c>
-      <c r="D107" t="str">
-        <f>IF(B107=C107,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75">
-      <c r="A108" s="1"/>
+      <c r="D108" t="str">
+        <f>IF(B108=C108,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="15.75">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:4" ht="15.75">
+      <c r="A110" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B109" s="22">
+      <c r="B110" s="22">
         <f>TBILLEQ(DATE(2008,3,31), DATE(2008,6,1), 0.0914)</f>
         <v>9.4151493565943017E-2</v>
       </c>
-      <c r="C109" s="22">
+      <c r="C110" s="22">
         <v>9.4151493565943017E-2</v>
       </c>
-      <c r="D109" t="str">
-        <f>IF(B109=C109,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="15.75">
-      <c r="A110" s="1"/>
+      <c r="D110" t="str">
+        <f>IF(B110=C110,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="111" spans="1:4" ht="15.75">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" ht="15.75">
+      <c r="A112" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B111" s="22">
+      <c r="B112" s="22">
         <f>TBILLYIELD(DATE(2008,3,31),DATE(2008,6,1), 98.45)</f>
         <v>9.141696292534264E-2</v>
       </c>
-      <c r="C111" s="22">
+      <c r="C112" s="22">
         <v>9.141696292534264E-2</v>
       </c>
-      <c r="D111" t="str">
-        <f>IF(B111=C111,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15.75">
-      <c r="A112" s="1"/>
+      <c r="D112" t="str">
+        <f>IF(B112=C112,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="113" spans="1:7" ht="15.75">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:7" ht="15.75">
+      <c r="A114" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B113" s="24">
+      <c r="B114" s="22">
         <f>VDB(2400,400,10*365,0,1)</f>
         <v>1.3150684931506849</v>
       </c>
-      <c r="C113" s="22">
+      <c r="C114" s="22">
         <v>1.3150684931506849</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15.75">
-      <c r="A114" s="1"/>
-    </row>
     <row r="115" spans="1:7" ht="15.75">
-      <c r="A115" s="1" t="s">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:7" ht="15.75">
+      <c r="A116" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B115" s="22">
-        <f>XNPV(0.09,B116:F116,B117:F117)</f>
+      <c r="B116" s="22">
+        <f>XNPV(0.09,B117:F117,B118:F118)</f>
         <v>2086.6476020315349</v>
       </c>
-      <c r="C115" s="22">
+      <c r="C116" s="22">
         <v>2086.6476020315349</v>
       </c>
-      <c r="D115" t="str">
-        <f>IF(B115=C115,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="15.75">
-      <c r="A116" s="1"/>
-      <c r="B116">
-        <v>-10000</v>
-      </c>
-      <c r="C116">
-        <v>2750</v>
-      </c>
-      <c r="D116">
-        <v>4250</v>
-      </c>
-      <c r="E116">
-        <v>3250</v>
-      </c>
-      <c r="F116">
-        <v>2750</v>
+      <c r="D116" t="str">
+        <f>IF(B116=C116,"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15.75">
       <c r="A117" s="1"/>
-      <c r="B117" s="18">
+      <c r="B117">
+        <v>-10000</v>
+      </c>
+      <c r="C117">
+        <v>2750</v>
+      </c>
+      <c r="D117">
+        <v>4250</v>
+      </c>
+      <c r="E117">
+        <v>3250</v>
+      </c>
+      <c r="F117">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15.75">
+      <c r="A118" s="1"/>
+      <c r="B118" s="18">
         <v>39448</v>
       </c>
-      <c r="C117" s="18">
+      <c r="C118" s="18">
         <v>39508</v>
       </c>
-      <c r="D117" s="18">
+      <c r="D118" s="18">
         <v>39751</v>
       </c>
-      <c r="E117" s="18">
+      <c r="E118" s="18">
         <v>39859</v>
       </c>
-      <c r="F117" s="18">
+      <c r="F118" s="18">
         <v>39904</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15.75">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:7" ht="15.75">
+      <c r="A119" s="1"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
+    </row>
+    <row r="120" spans="1:7" ht="15.75">
+      <c r="A120" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B118" s="22">
+      <c r="B120" s="22">
         <f>YIELD(DATE(2008,2,14), DATE(2016,11,15), 0.0575, 95.04287, 100, 2,0)</f>
         <v>6.4998178600204778E-2</v>
       </c>
-      <c r="C118" s="22">
+      <c r="C120" s="22">
         <v>6.4998178600204778E-2</v>
       </c>
-      <c r="D118" t="str">
-        <f>IF(B118=C118,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="15.75">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:7" ht="15.75">
-      <c r="A120" s="1" t="s">
+      <c r="D120" t="str">
+        <f>IF(B120=C120,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:7" ht="15.75">
+      <c r="A122" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B120" s="22">
+      <c r="B122" s="22">
         <f>YIELDDISC(DATE(2008,2,16), DATE(2008,3,1), 99.795, 100, 2)</f>
         <v>5.2822571986858337E-2</v>
       </c>
-      <c r="C120" s="22">
+      <c r="C122" s="22">
         <v>5.2822571986858337E-2</v>
-      </c>
-      <c r="D120" t="str">
-        <f>IF(B120=C120,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="15.75">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" ht="15.75">
-      <c r="A122" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B122" s="22">
-        <f>YIELDMAT(B123,C123,D123,E123,F123,G123)</f>
-        <v>6.0954333691538673E-2</v>
-      </c>
-      <c r="C122" s="22">
-        <v>6.0954333691538673E-2</v>
       </c>
       <c r="D122" t="str">
         <f>IF(B122=C122,"T","WARN")</f>
@@ -14605,34 +14561,47 @@
     </row>
     <row r="123" spans="1:7" ht="15.75">
       <c r="A123" s="1"/>
-      <c r="B123" s="18">
+    </row>
+    <row r="124" spans="1:7" ht="15.75">
+      <c r="A124" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B124" s="22">
+        <f>YIELDMAT(B125,C125,D125,E125,F125,G125)</f>
+        <v>6.0954333691538673E-2</v>
+      </c>
+      <c r="C124" s="22">
+        <v>6.0954333691538673E-2</v>
+      </c>
+      <c r="D124" t="str">
+        <f>IF(B124=C124,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15.75">
+      <c r="A125" s="1"/>
+      <c r="B125" s="18">
         <v>39522</v>
       </c>
-      <c r="C123" s="18">
+      <c r="C125" s="18">
         <v>39755</v>
       </c>
-      <c r="D123" s="18">
+      <c r="D125" s="18">
         <v>39394</v>
       </c>
-      <c r="E123" s="21">
+      <c r="E125" s="21">
         <v>6.25E-2</v>
       </c>
-      <c r="F123" s="21">
+      <c r="F125" s="21">
         <v>100.0123</v>
       </c>
-      <c r="G123" s="21">
+      <c r="G125" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="15.75">
-      <c r="A124" s="1"/>
     </row>
     <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:7" ht="15.75">
-      <c r="A127" s="1"/>
-    </row>
     <row r="128" spans="1:7" ht="15.75">
       <c r="A128" s="1"/>
     </row>
@@ -14650,7 +14619,6 @@
     </row>
     <row r="133" spans="1:2" ht="15.75">
       <c r="A133" s="1"/>
-      <c r="B133" s="5"/>
     </row>
     <row r="134" spans="1:2" ht="15.75">
       <c r="A134" s="1"/>
@@ -14671,14 +14639,14 @@
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="1"/>
-      <c r="B139" s="8"/>
+      <c r="B139" s="5"/>
     </row>
     <row r="140" spans="1:2" ht="15.75">
       <c r="A140" s="1"/>
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="1"/>
-      <c r="B141" s="5"/>
+      <c r="B141" s="8"/>
     </row>
     <row r="142" spans="1:2" ht="15.75">
       <c r="A142" s="1"/>
@@ -14692,6 +14660,7 @@
     </row>
     <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="1"/>
+      <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="15.75">
       <c r="A146" s="1"/>
@@ -14701,34 +14670,33 @@
     </row>
     <row r="148" spans="1:2" ht="15.75">
       <c r="A148" s="1"/>
-      <c r="B148" s="5"/>
     </row>
     <row r="149" spans="1:2" ht="15.75">
       <c r="A149" s="1"/>
     </row>
     <row r="150" spans="1:2" ht="15.75">
       <c r="A150" s="1"/>
-      <c r="B150" s="11"/>
+      <c r="B150" s="5"/>
     </row>
     <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
-      <c r="B152" s="9"/>
+      <c r="B152" s="11"/>
     </row>
     <row r="153" spans="1:2" ht="15.75">
       <c r="A153" s="1"/>
     </row>
     <row r="154" spans="1:2" ht="15.75">
       <c r="A154" s="1"/>
+      <c r="B154" s="9"/>
     </row>
     <row r="155" spans="1:2" ht="15.75">
       <c r="A155" s="1"/>
     </row>
     <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="1"/>
-      <c r="B156" s="5"/>
     </row>
     <row r="157" spans="1:2" ht="15.75">
       <c r="A157" s="1"/>
@@ -14742,6 +14710,7 @@
     </row>
     <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="1"/>
+      <c r="B160" s="5"/>
     </row>
     <row r="161" spans="1:2" ht="15.75">
       <c r="A161" s="1"/>
@@ -14754,13 +14723,13 @@
     </row>
     <row r="164" spans="1:2" ht="15.75">
       <c r="A164" s="1"/>
-      <c r="B164" s="8"/>
     </row>
     <row r="165" spans="1:2" ht="15.75">
       <c r="A165" s="1"/>
     </row>
     <row r="166" spans="1:2" ht="15.75">
       <c r="A166" s="1"/>
+      <c r="B166" s="8"/>
     </row>
     <row r="167" spans="1:2" ht="15.75">
       <c r="A167" s="1"/>
@@ -14780,28 +14749,28 @@
     <row r="172" spans="1:2" ht="15.75">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:2">
-      <c r="B173" s="12"/>
+    <row r="173" spans="1:2" ht="15.75">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:2" ht="15.75">
+      <c r="A174" s="1"/>
     </row>
     <row r="175" spans="1:2">
-      <c r="B175" s="8"/>
-    </row>
-    <row r="177" spans="1:2" ht="15.75">
-      <c r="A177" s="1"/>
-      <c r="B177" s="5"/>
-    </row>
-    <row r="178" spans="1:2" ht="15.75">
-      <c r="A178" s="1"/>
+      <c r="B175" s="12"/>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="B177" s="8"/>
     </row>
     <row r="179" spans="1:2" ht="15.75">
       <c r="A179" s="1"/>
-      <c r="B179" s="11"/>
+      <c r="B179" s="5"/>
     </row>
     <row r="180" spans="1:2" ht="15.75">
       <c r="A180" s="1"/>
     </row>
     <row r="181" spans="1:2" ht="15.75">
       <c r="A181" s="1"/>
+      <c r="B181" s="11"/>
     </row>
     <row r="182" spans="1:2" ht="15.75">
       <c r="A182" s="1"/>
@@ -14889,23 +14858,23 @@
     </row>
     <row r="210" spans="1:2" ht="15.75">
       <c r="A210" s="1"/>
-      <c r="B210" s="5"/>
     </row>
     <row r="211" spans="1:2" ht="15.75">
       <c r="A211" s="1"/>
     </row>
     <row r="212" spans="1:2" ht="15.75">
       <c r="A212" s="1"/>
+      <c r="B212" s="5"/>
     </row>
     <row r="213" spans="1:2" ht="15.75">
       <c r="A213" s="1"/>
-      <c r="B213" s="5"/>
     </row>
     <row r="214" spans="1:2" ht="15.75">
       <c r="A214" s="1"/>
     </row>
     <row r="215" spans="1:2" ht="15.75">
       <c r="A215" s="1"/>
+      <c r="B215" s="5"/>
     </row>
     <row r="216" spans="1:2" ht="15.75">
       <c r="A216" s="1"/>
@@ -14934,54 +14903,53 @@
     <row r="224" spans="1:2" ht="15.75">
       <c r="A224" s="1"/>
     </row>
-    <row r="225" spans="1:2" ht="15.75">
+    <row r="225" spans="1:1" ht="15.75">
       <c r="A225" s="1"/>
     </row>
-    <row r="226" spans="1:2" ht="15.75">
+    <row r="226" spans="1:1" ht="15.75">
       <c r="A226" s="1"/>
     </row>
-    <row r="227" spans="1:2" ht="15.75">
+    <row r="227" spans="1:1" ht="15.75">
       <c r="A227" s="1"/>
     </row>
-    <row r="228" spans="1:2" ht="15.75">
+    <row r="228" spans="1:1" ht="15.75">
       <c r="A228" s="1"/>
     </row>
-    <row r="229" spans="1:2" ht="15.75">
+    <row r="229" spans="1:1" ht="15.75">
       <c r="A229" s="1"/>
     </row>
-    <row r="230" spans="1:2" ht="15.75">
+    <row r="230" spans="1:1" ht="15.75">
       <c r="A230" s="1"/>
     </row>
-    <row r="231" spans="1:2" ht="15.75">
+    <row r="231" spans="1:1" ht="15.75">
       <c r="A231" s="1"/>
     </row>
-    <row r="232" spans="1:2" ht="15.75">
+    <row r="232" spans="1:1" ht="15.75">
       <c r="A232" s="1"/>
     </row>
-    <row r="233" spans="1:2" ht="15.75">
+    <row r="233" spans="1:1" ht="15.75">
       <c r="A233" s="1"/>
     </row>
-    <row r="234" spans="1:2" ht="15.75">
+    <row r="234" spans="1:1" ht="15.75">
       <c r="A234" s="1"/>
     </row>
-    <row r="235" spans="1:2" ht="15.75">
+    <row r="235" spans="1:1" ht="15.75">
       <c r="A235" s="1"/>
     </row>
-    <row r="236" spans="1:2" ht="15.75">
+    <row r="236" spans="1:1" ht="15.75">
       <c r="A236" s="1"/>
     </row>
-    <row r="237" spans="1:2" ht="15.75">
+    <row r="237" spans="1:1" ht="15.75">
       <c r="A237" s="1"/>
     </row>
-    <row r="238" spans="1:2" ht="15.75">
+    <row r="238" spans="1:1" ht="15.75">
       <c r="A238" s="1"/>
     </row>
-    <row r="239" spans="1:2" ht="15.75">
+    <row r="239" spans="1:1" ht="15.75">
       <c r="A239" s="1"/>
     </row>
-    <row r="240" spans="1:2" ht="15.75">
+    <row r="240" spans="1:1" ht="15.75">
       <c r="A240" s="1"/>
-      <c r="B240" s="11"/>
     </row>
     <row r="241" spans="1:2" ht="15.75">
       <c r="A241" s="1"/>
@@ -14992,17 +14960,18 @@
     </row>
     <row r="243" spans="1:2" ht="15.75">
       <c r="A243" s="1"/>
-      <c r="B243" s="11"/>
     </row>
     <row r="244" spans="1:2" ht="15.75">
       <c r="A244" s="1"/>
-      <c r="B244" s="5"/>
+      <c r="B244" s="11"/>
     </row>
     <row r="245" spans="1:2" ht="15.75">
       <c r="A245" s="1"/>
+      <c r="B245" s="11"/>
     </row>
     <row r="246" spans="1:2" ht="15.75">
       <c r="A246" s="1"/>
+      <c r="B246" s="5"/>
     </row>
     <row r="247" spans="1:2" ht="15.75">
       <c r="A247" s="1"/>
@@ -15175,11 +15144,17 @@
     <row r="303" spans="1:1" ht="15.75">
       <c r="A303" s="1"/>
     </row>
+    <row r="304" spans="1:1" ht="15.75">
+      <c r="A304" s="1"/>
+    </row>
     <row r="305" spans="1:1" ht="15.75">
       <c r="A305" s="1"/>
     </row>
-    <row r="534" spans="1:1">
-      <c r="A534" s="3" t="s">
+    <row r="307" spans="1:1" ht="15.75">
+      <c r="A307" s="1"/>
+    </row>
+    <row r="536" spans="1:1">
+      <c r="A536" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15188,62 +15163,62 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="195" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="194" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="193" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="192" priority="9" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D99 D101 D103 D105 D107 D109">
-    <cfRule type="cellIs" dxfId="191" priority="8" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D111 D113 D115 D118 D120 D122">
-    <cfRule type="cellIs" dxfId="190" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112 D114 D116 D120 D122 D124">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="189" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="188" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="187" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="186" priority="3" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D113">
-    <cfRule type="cellIs" dxfId="185" priority="2" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D113">
-    <cfRule type="cellIs" dxfId="184" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D114">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D114">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15257,8 +15232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15277,7 +15252,7 @@
       <c r="A1" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="28" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -15566,11 +15541,11 @@
       <c r="A27" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="26">
         <f>CHITEST(B28:C30,B31:C33)</f>
         <v>3.081920170211661E-4</v>
       </c>
-      <c r="C27" s="29">
+      <c r="C27" s="26">
         <v>3.081920170211661E-4</v>
       </c>
       <c r="D27" t="s">
@@ -15638,7 +15613,7 @@
       <c r="A35" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="27">
         <f>CONFIDENCE(0.05,2.5,50)</f>
         <v>0.69295191217483887</v>
       </c>
@@ -16889,7 +16864,7 @@
       <c r="A125" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B125" s="30">
+      <c r="B125" s="27">
         <f>NORMDIST(42,40,1.5,TRUE)</f>
         <v>0.90878878027413212</v>
       </c>
@@ -17109,7 +17084,7 @@
       <c r="A142" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B142" s="30">
+      <c r="B142" s="27">
         <f>POISSON(2,5,TRUE)</f>
         <v>0.12465201948308466</v>
       </c>
@@ -17310,7 +17285,7 @@
       <c r="A154" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B154" s="30">
+      <c r="B154" s="27">
         <f>SKEW(B155:K155)</f>
         <v>0.35954307140679742</v>
       </c>
@@ -17359,7 +17334,7 @@
       <c r="A156" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B156" s="30">
+      <c r="B156" s="27">
         <f>SLOPE(B157:H157,B158:H158)</f>
         <v>0.30555555555555558</v>
       </c>
@@ -18646,747 +18621,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="183" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="182" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="181" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="180" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="179" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="178" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="177" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="176" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="175" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="174" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="173" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="172" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="171" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="170" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="169" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="168" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="167" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="166" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="165" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="164" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="163" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="162" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="161" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="160" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="159" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="158" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="157" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="156" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="155" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="154" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="153" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="152" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="151" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="150" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="149" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="148" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="147" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="146" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="145" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="144" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="143" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="142" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="141" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="140" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="139" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="138" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="137" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="136" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="135" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="134" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="133" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="132" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="131" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="130" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="129" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="128" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="127" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="126" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="125" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="124" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="123" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="122" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="121" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="120" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="119" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="118" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="117" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="116" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="115" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="114" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="113" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="112" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="111" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="110" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="109" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="108" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="107" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="106" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="105" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="104" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="103" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="102" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="101" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="100" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="99" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="98" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="97" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="96" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="95" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="94" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="93" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="92" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="91" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="90" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="89" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="88" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="87" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="86" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="85" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="84" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="83" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="82" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="81" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="80" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="79" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="78" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="77" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="76" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="74" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="73" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="72" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="71" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="70" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="69" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="68" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="67" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="66" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="65" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="64" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="63" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="62" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="61" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="60" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="59" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="58" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="57" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="56" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="55" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="54" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="53" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="52" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="51" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="49" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="48" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
* do not test some test cases for NETWORKDAYS, WORKDAY for now * remove test case in first sheet
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -167,6 +167,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="D20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hawk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+test in the future</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A41" authorId="0">
       <text>
         <r>
@@ -188,6 +212,30 @@
           </rPr>
           <t xml:space="preserve">
 not in document</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hawk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+test in the future</t>
         </r>
       </text>
     </comment>
@@ -1354,7 +1402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="416">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2608,11 +2656,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="8" formatCode="&quot;NT$&quot;#,##0.00;[Red]\-&quot;NT$&quot;#,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0_ ;[Red]\-0\ "/>
     <numFmt numFmtId="170" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12">
@@ -2725,7 +2775,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2754,6 +2804,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2766,6 +2817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5506,89 +5558,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="15">
-        <f>NPV(0.08,8000,9200,10000,12000,14500)</f>
-        <v>41922.06155493237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" t="str">
-        <f>ASC("EXCEL")</f>
-        <v>EXCEL</v>
-      </c>
-      <c r="C3" t="s">
-        <v>391</v>
-      </c>
-      <c r="D3" t="str">
-        <f>IF(B3=C3,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <f>CHAR(65)</f>
-        <v>A</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(B5=C5,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
-      <c r="A7" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B7" s="22">
-        <f>BETADIST(2,8,10,1,3)</f>
-        <v>0.68547058095349067</v>
-      </c>
-      <c r="C7">
-        <v>0.68547058095349067</v>
-      </c>
-      <c r="D7" t="str">
-        <f>IF(B7=C7,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
+    <row r="1" spans="1:2">
+      <c r="A1" s="26"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="22"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75">
-      <c r="A9" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B9" s="12">
-        <f>BETAINV(0.6854,8,10,1,3)</f>
-        <v>1.9999523162841797</v>
-      </c>
-      <c r="C9">
-        <v>1.9999523162841797</v>
-      </c>
-      <c r="D9" t="str">
-        <f>IF(B9=C9,"T","WARN")</f>
-        <v>T</v>
-      </c>
+    <row r="9" spans="1:2" ht="15.75">
+      <c r="A9" s="1"/>
+      <c r="B9" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
@@ -5610,8 +5608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5771,7 +5769,7 @@
         <f>BIN2OCT(1001,3)</f>
         <v>011</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="30" t="s">
         <v>368</v>
       </c>
       <c r="D15" t="str">
@@ -5788,11 +5786,11 @@
       <c r="A17" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B17" s="12" t="str">
+      <c r="B17" s="35" t="str">
         <f>COMPLEX(3,4)</f>
         <v>3+4i</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="35" t="s">
         <v>369</v>
       </c>
       <c r="D17" t="str">
@@ -5834,7 +5832,7 @@
         <f>DEC2HEX(100,4)</f>
         <v>0064</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="30" t="s">
         <v>371</v>
       </c>
       <c r="D21" t="str">
@@ -5855,7 +5853,7 @@
         <f>DEC2OCT(58,3)</f>
         <v>072</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="30" t="s">
         <v>372</v>
       </c>
       <c r="D23" t="str">
@@ -5893,7 +5891,7 @@
       <c r="A27" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="28">
         <f>ERF(0.745)</f>
         <v>0.70792869314881979</v>
       </c>
@@ -5960,7 +5958,7 @@
         <f>HEX2BIN("F",8)</f>
         <v>00001111</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>373</v>
       </c>
       <c r="D33" t="str">
@@ -6002,7 +6000,7 @@
         <f>HEX2OCT("F",3)</f>
         <v>017</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="30" t="s">
         <v>374</v>
       </c>
       <c r="D37" t="str">
@@ -6377,7 +6375,7 @@
         <f>OCT2BIN(3, 3)</f>
         <v>011</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="30" t="s">
         <v>368</v>
       </c>
       <c r="D73" t="str">
@@ -6419,7 +6417,7 @@
         <f>OCT2HEX(100, 4)</f>
         <v>0040</v>
       </c>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="30" t="s">
         <v>387</v>
       </c>
       <c r="D77" t="str">
@@ -7092,7 +7090,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="31" t="s">
         <v>124</v>
       </c>
       <c r="B2" t="str">
@@ -7122,13 +7120,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>125</v>
       </c>
       <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="31" t="s">
         <v>388</v>
       </c>
       <c r="B5" s="11"/>
@@ -7635,7 +7633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7757,17 +7757,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -7813,7 +7813,7 @@
         <f>ACOS(-0.5)</f>
         <v>2.0943951023931957</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="32">
         <v>2.0943951023931957</v>
       </c>
       <c r="D7" t="str">
@@ -7867,7 +7867,7 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="28">
         <f>ASINH(-2.5)</f>
         <v>-1.6472311463710965</v>
       </c>
@@ -7886,7 +7886,7 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="28">
         <f>ATAN(1)</f>
         <v>0.78539816339744828</v>
       </c>
@@ -7905,11 +7905,11 @@
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="28">
         <f>ATAN2(1, 1)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="28">
         <v>0.78539816339744828</v>
       </c>
       <c r="D17" t="str">
@@ -7924,7 +7924,7 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="28">
         <f>ATANH(0.76159416)</f>
         <v>1.0000000096297197</v>
       </c>
@@ -7981,7 +7981,7 @@
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="28">
         <f>COS(1.047)</f>
         <v>0.50017107459707011</v>
       </c>
@@ -8000,7 +8000,7 @@
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="28">
         <f>COSH(4)</f>
         <v>27.308232836016487</v>
       </c>
@@ -8617,7 +8617,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>23.153652570547266</v>
+        <v>7.927829281525467</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -11866,8 +11866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D479"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12012,7 +12012,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="1"/>
-      <c r="B14" s="32">
+      <c r="B14" s="33">
         <v>0.14618055555555556</v>
       </c>
     </row>
@@ -12034,7 +12034,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="1"/>
-      <c r="B16" s="32">
+      <c r="B16" s="33">
         <v>0.70000000000000007</v>
       </c>
     </row>
@@ -12082,10 +12082,6 @@
       <c r="C20">
         <v>108</v>
       </c>
-      <c r="D20" t="str">
-        <f t="shared" ref="D20:D25" si="0">IF(B20=C20,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="1" t="s">
@@ -12098,10 +12094,6 @@
       <c r="C21">
         <v>5</v>
       </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="1" t="s">
@@ -12113,10 +12105,6 @@
       </c>
       <c r="C22">
         <v>0</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75">
@@ -12128,10 +12116,6 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="1" t="s">
@@ -12143,10 +12127,6 @@
       </c>
       <c r="C24">
         <v>107</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75">
@@ -12158,10 +12138,6 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="1" t="s">
@@ -12174,9 +12150,6 @@
       <c r="C26" t="e">
         <v>#NAME?</v>
       </c>
-      <c r="D26" t="s">
-        <v>403</v>
-      </c>
     </row>
     <row r="27" spans="1:4" ht="15.75">
       <c r="A27" s="1"/>
@@ -12190,7 +12163,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41446.401156018517</v>
+        <v>41446.428749189814</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -12214,7 +12187,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="1"/>
-      <c r="B32" s="32">
+      <c r="B32" s="33">
         <v>0.70020833333333332</v>
       </c>
     </row>
@@ -12298,7 +12271,7 @@
         <v>41369</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D44" si="1">IF(B41=C41,"T","WARN")</f>
+        <f t="shared" ref="D41:D44" si="0">IF(B41=C41,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
@@ -12311,10 +12284,6 @@
       <c r="C42" s="18">
         <v>39933</v>
       </c>
-      <c r="D42" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="43" spans="1:4" ht="15.75">
       <c r="A43" s="1" t="s">
@@ -12326,10 +12295,6 @@
       </c>
       <c r="C43" s="18">
         <v>41428</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75">
@@ -12341,10 +12306,6 @@
       <c r="C44" s="18">
         <v>41425</v>
       </c>
-      <c r="D44" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="1" t="s">
@@ -12356,10 +12317,6 @@
       </c>
       <c r="C45" s="18">
         <v>41372</v>
-      </c>
-      <c r="D45" t="str">
-        <f>IF(B45=C45,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75">
@@ -12371,10 +12328,6 @@
       <c r="C46" s="18">
         <v>41372</v>
       </c>
-      <c r="D46" t="str">
-        <f t="shared" ref="D46:D53" si="2">IF(B46=C46,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="1" t="s">
@@ -12386,10 +12339,6 @@
       </c>
       <c r="C47" s="18">
         <v>41362</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75">
@@ -12401,10 +12350,6 @@
       <c r="C48" s="18">
         <v>41425</v>
       </c>
-      <c r="D48" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="1" t="s">
@@ -12416,10 +12361,6 @@
       </c>
       <c r="C49" s="18">
         <v>41365</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75">
@@ -12431,10 +12372,6 @@
       <c r="C50" s="18">
         <v>41426</v>
       </c>
-      <c r="D50" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="1" t="s">
@@ -12446,10 +12383,6 @@
       </c>
       <c r="C51" s="18">
         <v>41369</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75">
@@ -12461,10 +12394,6 @@
       <c r="C52" s="18">
         <v>41367</v>
       </c>
-      <c r="D52" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="53" spans="1:4" ht="15.75">
       <c r="A53" s="1"/>
@@ -12475,10 +12404,6 @@
       <c r="C53" s="18">
         <v>41365</v>
       </c>
-      <c r="D53" t="str">
-        <f t="shared" si="2"/>
-        <v>T</v>
-      </c>
     </row>
     <row r="54" spans="1:4" ht="15.75">
       <c r="A54" s="1"/>
@@ -12529,7 +12454,7 @@
         <v>413</v>
       </c>
       <c r="C60" s="21">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
         <v>414</v>
@@ -13139,8 +13064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I536"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15252,7 +15177,7 @@
       <c r="A1" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -15541,11 +15466,11 @@
       <c r="A27" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="27">
         <f>CHITEST(B28:C30,B31:C33)</f>
         <v>3.081920170211661E-4</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="27">
         <v>3.081920170211661E-4</v>
       </c>
       <c r="D27" t="s">
@@ -15613,7 +15538,7 @@
       <c r="A35" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="28">
         <f>CONFIDENCE(0.05,2.5,50)</f>
         <v>0.69295191217483887</v>
       </c>
@@ -16864,7 +16789,7 @@
       <c r="A125" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B125" s="27">
+      <c r="B125" s="28">
         <f>NORMDIST(42,40,1.5,TRUE)</f>
         <v>0.90878878027413212</v>
       </c>
@@ -17084,7 +17009,7 @@
       <c r="A142" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B142" s="27">
+      <c r="B142" s="28">
         <f>POISSON(2,5,TRUE)</f>
         <v>0.12465201948308466</v>
       </c>
@@ -17285,7 +17210,7 @@
       <c r="A154" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B154" s="27">
+      <c r="B154" s="28">
         <f>SKEW(B155:K155)</f>
         <v>0.35954307140679742</v>
       </c>
@@ -17334,7 +17259,7 @@
       <c r="A156" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B156" s="27">
+      <c r="B156" s="28">
         <f>SLOPE(B157:H157,B158:H158)</f>
         <v>0.30555555555555558</v>
       </c>

</xml_diff>

<commit_message>
* verify unsupported formula with #NAME? or #VALUE! * refactor
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -1402,7 +1402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="416">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2823,7 +2823,31 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="203">
+  <dxfs count="205">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -5590,12 +5614,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7028,37 +7052,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7424,87 +7448,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7596,32 +7620,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7714,12 +7738,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="200" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8617,7 +8641,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>7.927829281525467</v>
+        <v>77.118490576990254</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8635,7 +8659,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9516,7 +9540,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="198" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9726,7 +9750,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9739,8 +9763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10412,21 +10436,30 @@
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="21">
+        <f>VALUE("1,000")</f>
+        <v>1000</v>
+      </c>
+      <c r="C72">
+        <v>1000</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" ref="D70:D73" si="0">IF(B72=C72,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75">
+      <c r="A73" s="1"/>
+      <c r="B73">
         <f>VALUE("16:48:00")</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>0.7</v>
       </c>
-      <c r="D72" t="str">
-        <f>IF(B72=C72,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75">
-      <c r="A73" s="1"/>
-      <c r="C73" s="18"/>
+      <c r="D73" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
       <c r="B78" s="11"/>
@@ -10882,8 +10915,8 @@
   <sortState ref="A5:A26">
     <sortCondition ref="A5"/>
   </sortState>
-  <conditionalFormatting sqref="D3:D72">
-    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
+  <conditionalFormatting sqref="D3:D73">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11843,17 +11876,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8:D10 D13 D16 D19 D21 D24 D27 D29">
-    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D36 D39 D41">
-    <cfRule type="cellIs" dxfId="194" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="193" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11866,7 +11899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -12163,7 +12196,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41446.428749189814</v>
+        <v>41446.441274421297</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -13050,7 +13083,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D31 D33 D39 D56 D35 D58:D60 D41:D53 D19:D27">
-    <cfRule type="cellIs" dxfId="192" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15088,62 +15121,62 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112 D114 D116 D120 D122 D124">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18546,747 +18579,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="191" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="190" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="189" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="188" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="187" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="186" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="185" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="184" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="183" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="182" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="181" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="180" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="179" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="178" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="177" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="176" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="175" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="174" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="173" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="172" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="171" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="170" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="169" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="168" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="167" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="166" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="165" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="164" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="163" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="162" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="161" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="160" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="159" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="158" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="157" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="156" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="155" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="154" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="153" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="152" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="151" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="150" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="149" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="148" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="147" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="146" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="145" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="144" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="143" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="142" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="141" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="140" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="139" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="138" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="137" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="136" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="135" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="134" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="133" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="132" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="131" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="130" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="129" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="128" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="127" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="126" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="125" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="124" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="123" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="122" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="121" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="120" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="119" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="118" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="117" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="116" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="115" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="114" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="113" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="112" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="111" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="110" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="109" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="108" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="107" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="106" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="105" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="104" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="103" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="102" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="101" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="100" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="99" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="98" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="97" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="96" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="95" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="94" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="93" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="92" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="91" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="90" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="89" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="88" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="87" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="86" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="85" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="84" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="83" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="82" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="81" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="80" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="79" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="77" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="76" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="75" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="74" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="73" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="72" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="71" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="69" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="68" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="67" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="66" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="65" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="64" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="63" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="61" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="60" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="55" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="54" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="53" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="52" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="50" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="47" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix NETWORKDAYS & WORKDAY, so enable those test cases for them
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -2661,9 +2661,9 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0_ ;[Red]\-0\ "/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -2802,10 +2802,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2814,16 +2814,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="205">
+  <dxfs count="206">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -5614,12 +5626,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5810,11 +5822,11 @@
       <c r="A17" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B17" s="35" t="str">
+      <c r="B17" s="34" t="str">
         <f>COMPLEX(3,4)</f>
         <v>3+4i</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="34" t="s">
         <v>369</v>
       </c>
       <c r="D17" t="str">
@@ -7052,37 +7064,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7448,87 +7460,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="38" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="37" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="35" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7620,32 +7632,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7738,12 +7750,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7781,17 +7793,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -8641,7 +8653,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>77.118490576990254</v>
+        <v>27.55696701865018</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8659,7 +8671,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9540,7 +9552,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="200" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9750,7 +9762,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9763,8 +9775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10444,7 +10456,7 @@
         <v>1000</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" ref="D70:D73" si="0">IF(B72=C72,"T","WARN")</f>
+        <f t="shared" ref="D72:D73" si="0">IF(B72=C72,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
@@ -10457,8 +10469,9 @@
       <c r="C73">
         <v>0.7</v>
       </c>
-      <c r="D73" t="s">
-        <v>403</v>
+      <c r="D73" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -10916,7 +10929,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11899,8 +11912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D479"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12115,6 +12128,10 @@
       <c r="C20">
         <v>108</v>
       </c>
+      <c r="D20" t="str">
+        <f t="shared" ref="D20:D25" si="0">IF(B20=C20,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="1" t="s">
@@ -12127,6 +12144,10 @@
       <c r="C21">
         <v>5</v>
       </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="1" t="s">
@@ -12138,6 +12159,10 @@
       </c>
       <c r="C22">
         <v>0</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75">
@@ -12149,6 +12174,10 @@
       <c r="C23">
         <v>0</v>
       </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75">
       <c r="A24" s="1" t="s">
@@ -12160,6 +12189,10 @@
       </c>
       <c r="C24">
         <v>107</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75">
@@ -12171,6 +12204,10 @@
       <c r="C25">
         <v>1</v>
       </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="1" t="s">
@@ -12180,8 +12217,11 @@
         <f>NETWORKDAYS(DATE(2013,6,2), DATE(2013,6,1))</f>
         <v>0</v>
       </c>
-      <c r="C26" t="e">
-        <v>#NAME?</v>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75">
@@ -12196,7 +12236,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41446.441274421297</v>
+        <v>41446.592544791667</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -12304,7 +12344,7 @@
         <v>41369</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D44" si="0">IF(B41=C41,"T","WARN")</f>
+        <f t="shared" ref="D41:D53" si="1">IF(B41=C41,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
@@ -12317,6 +12357,10 @@
       <c r="C42" s="18">
         <v>39933</v>
       </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15.75">
       <c r="A43" s="1" t="s">
@@ -12328,6 +12372,10 @@
       </c>
       <c r="C43" s="18">
         <v>41428</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75">
@@ -12339,6 +12387,10 @@
       <c r="C44" s="18">
         <v>41425</v>
       </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="1" t="s">
@@ -12350,6 +12402,10 @@
       </c>
       <c r="C45" s="18">
         <v>41372</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75">
@@ -12361,6 +12417,10 @@
       <c r="C46" s="18">
         <v>41372</v>
       </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="1" t="s">
@@ -12372,6 +12432,10 @@
       </c>
       <c r="C47" s="18">
         <v>41362</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75">
@@ -12383,6 +12447,10 @@
       <c r="C48" s="18">
         <v>41425</v>
       </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="1" t="s">
@@ -12394,6 +12462,10 @@
       </c>
       <c r="C49" s="18">
         <v>41365</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75">
@@ -12405,6 +12477,10 @@
       <c r="C50" s="18">
         <v>41426</v>
       </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="1" t="s">
@@ -12416,6 +12492,10 @@
       </c>
       <c r="C51" s="18">
         <v>41369</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75">
@@ -12427,6 +12507,10 @@
       <c r="C52" s="18">
         <v>41367</v>
       </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15.75">
       <c r="A53" s="1"/>
@@ -12436,6 +12520,10 @@
       </c>
       <c r="C53" s="18">
         <v>41365</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75">
@@ -15121,62 +15209,62 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112 D114 D116 D120 D122 D124">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18579,747 +18667,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="194" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="193" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="192" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="191" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="190" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="189" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="188" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="187" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="186" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="185" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="184" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="183" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="182" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="181" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="180" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="179" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="178" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="177" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="176" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="175" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="174" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="173" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="172" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="171" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="170" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="169" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="168" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="167" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="166" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="165" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="164" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="163" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="162" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="161" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="160" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="159" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="158" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="157" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="156" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="155" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="154" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="153" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="152" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="151" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="150" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="149" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="148" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="147" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="146" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="145" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="144" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="143" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="142" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="141" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="140" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="139" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="138" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="137" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="136" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="135" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="134" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="133" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="132" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="131" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="130" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="129" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="128" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="127" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="126" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="125" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="124" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="123" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="122" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="121" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="120" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="119" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="118" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="117" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="116" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="115" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="114" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="113" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="112" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="111" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="110" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="109" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="108" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="107" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="106" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="105" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="104" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="103" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="102" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="101" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="100" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="99" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="98" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="97" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="96" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="95" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="94" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="93" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="92" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="91" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="90" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="89" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="88" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="86" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="85" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="84" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="83" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="82" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="81" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="80" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="79" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="78" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="77" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="76" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="74" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="73" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="72" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="71" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="70" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="69" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="68" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="66" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="65" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="64" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="63" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="62" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="61" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="60" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="59" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="58" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="57" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="56" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="53" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="52" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="51" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="50" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add test cases for ISERR()
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'formula-engineering'!$A$10:$C$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$8:$C$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$8:$C$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'formula-logical'!$A$8:$C$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'formula-math'!$A$9:$C$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'formula-statistical'!$A$11:$C$45</definedName>
@@ -2823,43 +2823,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="206">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="203">
     <dxf>
       <font>
         <condense val="0"/>
@@ -5626,12 +5590,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="205" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="204" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7750,12 +7714,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="203" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="202" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8653,7 +8617,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>27.55696701865018</v>
+        <v>55.438436526051049</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8671,7 +8635,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9552,7 +9516,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="201" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9762,7 +9726,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="200" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10929,7 +10893,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="199" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10941,10 +10905,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D449"/>
+  <dimension ref="A1:D451"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11060,85 +11024,87 @@
     </row>
     <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="b">
+        <f ca="1">ISERR(B13)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" ref="D11:D12" ca="1" si="0">IF(B12=C12,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.75">
-      <c r="A13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" t="b">
-        <f>ISERROR(B14)</f>
-        <v>1</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="str">
-        <f>IF(B13=C13,"T","WARN")</f>
-        <v>T</v>
+      <c r="A13" s="1"/>
+      <c r="B13" s="5" t="e">
+        <f ca="1">abc()</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="1"/>
-      <c r="B14" s="5" t="e">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="A15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" t="b">
+        <f>ISERROR(B16)</f>
+        <v>1</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f>IF(B15=C15,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5" t="e">
         <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75">
-      <c r="A16" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" t="b">
-        <f>ISEVEN(B17)</f>
-        <v>1</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="str">
-        <f>IF(B16=C16,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="A17" s="1"/>
-      <c r="B17">
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" t="b">
+        <f>ISEVEN(B19)</f>
+        <v>1</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(B18=C18,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
+      <c r="A19" s="1"/>
+      <c r="B19">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:4" ht="15.75">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
+      <c r="A21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B19" t="b">
+      <c r="B21" t="b">
         <f>ISLOGICAL("TRUE")</f>
         <v>0</v>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(B19=C19,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75">
-      <c r="A21" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" t="b">
-        <f>ISNA(B22)</f>
-        <v>0</v>
-      </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
@@ -11149,110 +11115,109 @@
     </row>
     <row r="22" spans="1:4" ht="15.75">
       <c r="A22" s="1"/>
-      <c r="B22" s="5" t="e">
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" t="b">
+        <f>ISNA(B24)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(B23=C23,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5" t="e">
         <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75">
-      <c r="A23" s="1"/>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75">
-      <c r="A24" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" t="b">
-        <f>ISNONTEXT(B25)</f>
-        <v>1</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="str">
-        <f>IF(B24=C24,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75">
       <c r="A25" s="1"/>
-      <c r="B25">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
+      <c r="A26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" t="b">
+        <f>ISNONTEXT(B27)</f>
+        <v>1</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f>IF(B26=C26,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75">
+      <c r="A27" s="1"/>
+      <c r="B27">
         <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75">
-      <c r="A27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" t="b">
-        <f>ISNUMBER(B28)</f>
-        <v>1</v>
-      </c>
-      <c r="C27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" t="str">
-        <f>IF(B27=C27,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75">
       <c r="A28" s="1"/>
-      <c r="B28">
-        <v>10</v>
-      </c>
     </row>
     <row r="29" spans="1:4" ht="15.75">
       <c r="A29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" t="b">
+        <f>ISNUMBER(B30)</f>
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="str">
+        <f>IF(B29=C29,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75">
+      <c r="A30" s="1"/>
+      <c r="B30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
+      <c r="A31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B29" t="b">
+      <c r="B31" t="b">
         <f>ISODD(10)</f>
         <v>0</v>
       </c>
-      <c r="C29" t="b">
+      <c r="C31" t="b">
         <v>0</v>
       </c>
-      <c r="D29" t="str">
-        <f>IF(B29=C29,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75">
-      <c r="A31" s="1" t="s">
+      <c r="D31" t="str">
+        <f>IF(B31=C31,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75">
+      <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B31" t="b">
+      <c r="B33" t="b">
         <f>ISREF(B3A2)</f>
         <v>0</v>
       </c>
-      <c r="C31" t="b">
+      <c r="C33" t="b">
         <v>0</v>
-      </c>
-      <c r="D31" t="str">
-        <f>IF(B31=C31,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75">
-      <c r="A32" s="1"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75">
-      <c r="A33" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B33" t="b">
-        <f>ISTEXT(B34)</f>
-        <v>1</v>
-      </c>
-      <c r="C33" t="b">
-        <v>1</v>
       </c>
       <c r="D33" t="str">
         <f>IF(B33=C33,"T","WARN")</f>
@@ -11261,87 +11226,101 @@
     </row>
     <row r="34" spans="1:4" ht="15.75">
       <c r="A34" s="1"/>
-      <c r="B34" t="s">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75">
+      <c r="A35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" t="b">
+        <f>ISTEXT(B36)</f>
+        <v>1</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(B35=C35,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
+      <c r="A36" s="1"/>
+      <c r="B36" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75">
-      <c r="A36" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B36">
-        <f>N(B37)</f>
-        <v>7</v>
-      </c>
-      <c r="C36">
-        <v>7</v>
-      </c>
-      <c r="D36" t="str">
-        <f>IF(B36=C36,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75">
       <c r="A37" s="1"/>
-      <c r="B37">
+    </row>
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38">
+        <f>N(B39)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75">
-      <c r="A38" s="1"/>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" t="str">
+        <f>IF(B38=C38,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15.75">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="1"/>
+      <c r="B39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
+      <c r="A41" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B39" t="e">
+      <c r="B41" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="C39" t="e">
+      <c r="C41" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D41" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75">
-      <c r="A41" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B41">
-        <f>TYPE(B42)</f>
-        <v>2</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41" t="str">
-        <f>IF(B41=C41,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75">
       <c r="A42" s="1"/>
-      <c r="B42" t="s">
+    </row>
+    <row r="43" spans="1:4" ht="15.75">
+      <c r="A43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43">
+        <f>TYPE(B44)</f>
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(B43=C43,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="1"/>
+      <c r="B44" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75">
-      <c r="A43" s="1"/>
     </row>
     <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75">
-      <c r="A46" s="1"/>
-    </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="1"/>
     </row>
@@ -11416,7 +11395,6 @@
     </row>
     <row r="71" spans="1:2" ht="15.75">
       <c r="A71" s="1"/>
-      <c r="B71" s="5"/>
     </row>
     <row r="72" spans="1:2" ht="15.75">
       <c r="A72" s="1"/>
@@ -11451,20 +11429,21 @@
     </row>
     <row r="81" spans="1:2" ht="15.75">
       <c r="A81" s="1"/>
-      <c r="B81" s="8"/>
+      <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:2" ht="15.75">
       <c r="A82" s="1"/>
     </row>
     <row r="83" spans="1:2" ht="15.75">
       <c r="A83" s="1"/>
-      <c r="B83" s="5"/>
+      <c r="B83" s="8"/>
     </row>
     <row r="84" spans="1:2" ht="15.75">
       <c r="A84" s="1"/>
     </row>
     <row r="85" spans="1:2" ht="15.75">
       <c r="A85" s="1"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" ht="15.75">
       <c r="A86" s="1"/>
@@ -11472,11 +11451,11 @@
     <row r="87" spans="1:2" ht="15.75">
       <c r="A87" s="1"/>
     </row>
-    <row r="92" spans="1:2" ht="15.75">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.75">
-      <c r="A93" s="1"/>
+    <row r="88" spans="1:2" ht="15.75">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.75">
+      <c r="A89" s="1"/>
     </row>
     <row r="94" spans="1:2" ht="15.75">
       <c r="A94" s="1"/>
@@ -11513,7 +11492,6 @@
     </row>
     <row r="105" spans="1:2" ht="15.75">
       <c r="A105" s="1"/>
-      <c r="B105" s="5"/>
     </row>
     <row r="106" spans="1:2" ht="15.75">
       <c r="A106" s="1"/>
@@ -11541,14 +11519,14 @@
     </row>
     <row r="113" spans="1:2" ht="15.75">
       <c r="A113" s="1"/>
-      <c r="B113" s="8"/>
+      <c r="B113" s="5"/>
     </row>
     <row r="114" spans="1:2" ht="15.75">
       <c r="A114" s="1"/>
     </row>
     <row r="115" spans="1:2" ht="15.75">
       <c r="A115" s="1"/>
-      <c r="B115" s="5"/>
+      <c r="B115" s="8"/>
     </row>
     <row r="116" spans="1:2" ht="15.75">
       <c r="A116" s="1"/>
@@ -11562,6 +11540,7 @@
     </row>
     <row r="119" spans="1:2" ht="15.75">
       <c r="A119" s="1"/>
+      <c r="B119" s="5"/>
     </row>
     <row r="120" spans="1:2" ht="15.75">
       <c r="A120" s="1"/>
@@ -11571,34 +11550,33 @@
     </row>
     <row r="122" spans="1:2" ht="15.75">
       <c r="A122" s="1"/>
-      <c r="B122" s="5"/>
     </row>
     <row r="123" spans="1:2" ht="15.75">
       <c r="A123" s="1"/>
     </row>
     <row r="124" spans="1:2" ht="15.75">
       <c r="A124" s="1"/>
-      <c r="B124" s="11"/>
+      <c r="B124" s="5"/>
     </row>
     <row r="125" spans="1:2" ht="15.75">
       <c r="A125" s="1"/>
     </row>
     <row r="126" spans="1:2" ht="15.75">
       <c r="A126" s="1"/>
-      <c r="B126" s="9"/>
+      <c r="B126" s="11"/>
     </row>
     <row r="127" spans="1:2" ht="15.75">
       <c r="A127" s="1"/>
     </row>
     <row r="128" spans="1:2" ht="15.75">
       <c r="A128" s="1"/>
+      <c r="B128" s="9"/>
     </row>
     <row r="129" spans="1:2" ht="15.75">
       <c r="A129" s="1"/>
     </row>
     <row r="130" spans="1:2" ht="15.75">
       <c r="A130" s="1"/>
-      <c r="B130" s="5"/>
     </row>
     <row r="131" spans="1:2" ht="15.75">
       <c r="A131" s="1"/>
@@ -11612,6 +11590,7 @@
     </row>
     <row r="134" spans="1:2" ht="15.75">
       <c r="A134" s="1"/>
+      <c r="B134" s="5"/>
     </row>
     <row r="135" spans="1:2" ht="15.75">
       <c r="A135" s="1"/>
@@ -11624,13 +11603,13 @@
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="1"/>
-      <c r="B138" s="8"/>
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="1"/>
     </row>
     <row r="140" spans="1:2" ht="15.75">
       <c r="A140" s="1"/>
+      <c r="B140" s="8"/>
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="1"/>
@@ -11652,34 +11631,34 @@
     </row>
     <row r="147" spans="1:2" ht="15.75">
       <c r="A147" s="1"/>
-      <c r="B147" s="12"/>
     </row>
     <row r="148" spans="1:2" ht="15.75">
       <c r="A148" s="1"/>
     </row>
     <row r="149" spans="1:2" ht="15.75">
       <c r="A149" s="1"/>
-      <c r="B149" s="8"/>
+      <c r="B149" s="12"/>
     </row>
     <row r="150" spans="1:2" ht="15.75">
       <c r="A150" s="1"/>
     </row>
     <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
-      <c r="B151" s="5"/>
+      <c r="B151" s="8"/>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
     </row>
     <row r="153" spans="1:2" ht="15.75">
       <c r="A153" s="1"/>
-      <c r="B153" s="11"/>
+      <c r="B153" s="5"/>
     </row>
     <row r="154" spans="1:2" ht="15.75">
       <c r="A154" s="1"/>
     </row>
     <row r="155" spans="1:2" ht="15.75">
       <c r="A155" s="1"/>
+      <c r="B155" s="11"/>
     </row>
     <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="1"/>
@@ -11767,23 +11746,23 @@
     </row>
     <row r="184" spans="1:2" ht="15.75">
       <c r="A184" s="1"/>
-      <c r="B184" s="5"/>
     </row>
     <row r="185" spans="1:2" ht="15.75">
       <c r="A185" s="1"/>
     </row>
     <row r="186" spans="1:2" ht="15.75">
       <c r="A186" s="1"/>
+      <c r="B186" s="5"/>
     </row>
     <row r="187" spans="1:2" ht="15.75">
       <c r="A187" s="1"/>
-      <c r="B187" s="5"/>
     </row>
     <row r="188" spans="1:2" ht="15.75">
       <c r="A188" s="1"/>
     </row>
     <row r="189" spans="1:2" ht="15.75">
       <c r="A189" s="1"/>
+      <c r="B189" s="5"/>
     </row>
     <row r="190" spans="1:2" ht="15.75">
       <c r="A190" s="1"/>
@@ -11859,7 +11838,6 @@
     </row>
     <row r="214" spans="1:2" ht="15.75">
       <c r="A214" s="1"/>
-      <c r="B214" s="11"/>
     </row>
     <row r="215" spans="1:2" ht="15.75">
       <c r="A215" s="1"/>
@@ -11870,17 +11848,24 @@
     </row>
     <row r="217" spans="1:2" ht="15.75">
       <c r="A217" s="1"/>
-      <c r="B217" s="11"/>
     </row>
     <row r="218" spans="1:2" ht="15.75">
       <c r="A218" s="1"/>
-      <c r="B218" s="5"/>
+      <c r="B218" s="11"/>
+    </row>
+    <row r="219" spans="1:2" ht="15.75">
+      <c r="A219" s="1"/>
+      <c r="B219" s="11"/>
     </row>
     <row r="220" spans="1:2" ht="15.75">
       <c r="A220" s="1"/>
-    </row>
-    <row r="449" spans="1:1">
-      <c r="A449" s="3" t="s">
+      <c r="B220" s="5"/>
+    </row>
+    <row r="222" spans="1:2" ht="15.75">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="451" spans="1:1">
+      <c r="A451" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -11888,18 +11873,18 @@
   <sortState ref="A3:A18">
     <sortCondition ref="A3"/>
   </sortState>
-  <conditionalFormatting sqref="D3 D6 D8:D10 D13 D16 D19 D21 D24 D27 D29">
-    <cfRule type="cellIs" dxfId="198" priority="5" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31 D33 D36 D39 D41">
-    <cfRule type="cellIs" dxfId="197" priority="4" operator="equal">
+  <conditionalFormatting sqref="D3 D6 D15 D18 D21 D23 D26 D29 D31 D8:D12">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33 D35 D38 D41 D43">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="196" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11912,8 +11897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12236,7 +12221,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41446.592544791667</v>
+        <v>41446.628422569447</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">

</xml_diff>

<commit_message>
mark =VALUE("16:48:00") as unsupported date string
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -1402,7 +1402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="416">
   <si>
     <t>name-range formula</t>
   </si>
@@ -7028,37 +7028,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7424,87 +7424,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7596,32 +7596,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8617,7 +8617,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>55.438436526051049</v>
+        <v>43.352118695573182</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9739,8 +9739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10433,9 +10433,8 @@
       <c r="C73">
         <v>0.7</v>
       </c>
-      <c r="D73" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
+      <c r="D73" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -10907,7 +10906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D451"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -11032,7 +11031,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" ref="D11:D12" ca="1" si="0">IF(B12=C12,"T","WARN")</f>
+        <f t="shared" ref="D12" ca="1" si="0">IF(B12=C12,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
@@ -11874,17 +11873,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D15 D18 D21 D23 D26 D29 D31 D8:D12">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12221,7 +12220,7 @@
       </c>
       <c r="B29" s="20">
         <f ca="1">NOW()</f>
-        <v>41446.628422569447</v>
+        <v>41446.675288773149</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
@@ -13156,7 +13155,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D31 D33 D39 D56 D35 D58:D60 D41:D53 D19:D27">
-    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15194,62 +15193,62 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="194" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="193" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="192" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="191" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
-    <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112 D114 D116 D120 D122 D124">
-    <cfRule type="cellIs" dxfId="189" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="188" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="187" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="186" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="185" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="184" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="183" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18652,747 +18651,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="182" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="181" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="180" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="179" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="178" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="177" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="176" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="175" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="174" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="173" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="172" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="171" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="170" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="169" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="168" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="167" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="166" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="165" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="164" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="163" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="162" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="161" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="160" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="159" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="158" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="157" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="156" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="155" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="154" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="153" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="152" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="151" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="150" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="149" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="148" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="147" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="146" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="145" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="144" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="143" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="142" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="141" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="140" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="139" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="138" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="137" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="136" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="135" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="134" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="133" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="132" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="131" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="130" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="129" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="128" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="127" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="126" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="125" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="124" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="123" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="122" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="121" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="120" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="119" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="118" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="117" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="116" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="115" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="114" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="113" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="112" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="111" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="110" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="109" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="108" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="107" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="106" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="105" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="104" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="103" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="102" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="101" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="100" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="99" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="98" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="97" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="96" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="95" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="94" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="93" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="92" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="91" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="90" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="89" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="88" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="87" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="86" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="85" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="84" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="83" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="82" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="81" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="80" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="79" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="78" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="77" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="76" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="75" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="73" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="72" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="71" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="69" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="68" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="65" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="64" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="63" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="62" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="60" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="58" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="57" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="56" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="55" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="51" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="46" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="44" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add more test cases for NETWORKDAYS for 1900/1/1 issue
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="7110" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="formula-custom" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'formula-engineering'!$A$10:$C$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$8:$C$49</definedName>
@@ -191,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="0">
+    <comment ref="A45" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D42" authorId="0">
+    <comment ref="D46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -239,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A58" authorId="0">
+    <comment ref="A62" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1402,7 +1402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="420">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2650,6 +2650,18 @@
   </si>
   <si>
     <t>invalid, different spec</t>
+  </si>
+  <si>
+    <t>empty date</t>
+  </si>
+  <si>
+    <t>start date empty</t>
+  </si>
+  <si>
+    <t>end date empty</t>
+  </si>
+  <si>
+    <t>1900/1/1 is not workday in Excel</t>
   </si>
 </sst>
 </file>
@@ -2823,19 +2835,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="203">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="202">
     <dxf>
       <font>
         <condense val="0"/>
@@ -5590,12 +5590,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7714,12 +7714,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="200" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8617,7 +8617,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>43.352118695573182</v>
+        <v>6.2854998038929466</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9516,7 +9516,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="198" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9726,7 +9726,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9739,7 +9739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
@@ -10420,7 +10420,7 @@
         <v>1000</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" ref="D72:D73" si="0">IF(B72=C72,"T","WARN")</f>
+        <f t="shared" ref="D72" si="0">IF(B72=C72,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
@@ -10892,7 +10892,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11873,17 +11873,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D15 D18 D21 D23 D26 D29 D31 D8:D12">
-    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="194" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="193" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11894,17 +11894,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D479"/>
+  <dimension ref="A1:D483"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
@@ -12209,197 +12209,188 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B27">
+        <f>NETWORKDAYS(E27,F27)</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15.75">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75">
-      <c r="A29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" s="20">
-        <f ca="1">NOW()</f>
-        <v>41446.675288773149</v>
+      <c r="A28" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B28">
+        <f>NETWORKDAYS(B29,C29)</f>
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" s="18"/>
+      <c r="C29" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B30">
+        <f>NETWORKDAYS(C29, B29)</f>
+        <v>-1</v>
+      </c>
+      <c r="C30" s="21">
+        <v>-1</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="1" t="s">
-        <v>173</v>
+        <v>419</v>
       </c>
       <c r="B31">
-        <f>SECOND(B32)</f>
-        <v>18</v>
-      </c>
-      <c r="C31">
-        <v>18</v>
-      </c>
-      <c r="D31" t="str">
-        <f>IF(B31=C31,"T","WARN")</f>
-        <v>T</v>
+        <f>NETWORKDAYS(DATE(1900,1,1),DATE(1900,1,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="21">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75">
       <c r="A32" s="1"/>
-      <c r="B32" s="33">
-        <v>0.70020833333333332</v>
-      </c>
     </row>
     <row r="33" spans="1:4" ht="15.75">
       <c r="A33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="20">
+        <f ca="1">NOW()</f>
+        <v>41452.423760300924</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75">
+      <c r="A35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35">
+        <f>SECOND(B36)</f>
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <v>18</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(B35=C35,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
+      <c r="A36" s="1"/>
+      <c r="B36" s="33">
+        <v>0.70020833333333332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B37" s="16">
         <f>TIME(12,0,0)</f>
         <v>0.5</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <v>0.5</v>
       </c>
-      <c r="D33" t="str">
-        <f>IF(B33=C33,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75">
-      <c r="A35" s="1" t="s">
+      <c r="D37" t="str">
+        <f>IF(B37=C37,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75">
+      <c r="A39" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B39" s="5">
         <f>TIMEVALUE("2:24 AM")</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="C35">
+      <c r="C39">
         <v>0.1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D39" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:4" ht="15.75">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
+      <c r="A41" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B41" s="19">
         <f ca="1">TODAY()</f>
-        <v>41446</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75">
-      <c r="A39" s="1" t="s">
+        <v>41452</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75">
+      <c r="A43" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B39">
+      <c r="B43">
         <f>WEEKDAY(DATE(2008,2,14))</f>
         <v>5</v>
       </c>
-      <c r="C39">
+      <c r="C43">
         <v>5</v>
       </c>
-      <c r="D39" t="str">
-        <f>IF(B39=C39,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75">
-      <c r="A41" s="1" t="s">
+      <c r="D43" t="str">
+        <f>IF(B43=C43,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75">
+      <c r="A45" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B45" s="18">
         <f>WORKDAY(DATE(2013,4,1),4)</f>
         <v>41369</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C45" s="18">
         <v>41369</v>
       </c>
-      <c r="D41" t="str">
-        <f t="shared" ref="D41:D53" si="1">IF(B41=C41,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75">
-      <c r="A42" s="1"/>
-      <c r="B42" s="18">
-        <f>WORKDAY(DATE(2008,10,1),151)</f>
-        <v>39933</v>
-      </c>
-      <c r="C42" s="18">
-        <v>39933</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75">
-      <c r="A43" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B43" s="18">
-        <f>WORKDAY(DATE(2013,6,1),1)</f>
-        <v>41428</v>
-      </c>
-      <c r="C43" s="18">
-        <v>41428</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75">
-      <c r="A44" s="1"/>
-      <c r="B44" s="18">
-        <f>WORKDAY(DATE(2013,6,1), -1)</f>
-        <v>41425</v>
-      </c>
-      <c r="C44" s="18">
-        <v>41425</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75">
-      <c r="A45" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B45" s="18">
-        <f>WORKDAY(DATE(2013,4,1),5)</f>
-        <v>41372</v>
-      </c>
-      <c r="C45" s="18">
-        <v>41372</v>
-      </c>
       <c r="D45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D45:D57" si="1">IF(B45=C45,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75">
       <c r="A46" s="1"/>
       <c r="B46" s="18">
-        <f>WORKDAY(DATE(2013,4,5),1)</f>
-        <v>41372</v>
+        <f>WORKDAY(DATE(2008,10,1),151)</f>
+        <v>39933</v>
       </c>
       <c r="C46" s="18">
-        <v>41372</v>
+        <v>39933</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
@@ -12408,14 +12399,14 @@
     </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B47" s="18">
-        <f>WORKDAY(DATE(2013,4,1),-1)</f>
-        <v>41362</v>
+        <f>WORKDAY(DATE(2013,6,1),1)</f>
+        <v>41428</v>
       </c>
       <c r="C47" s="18">
-        <v>41362</v>
+        <v>41428</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
@@ -12425,7 +12416,7 @@
     <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="1"/>
       <c r="B48" s="18">
-        <f>WORKDAY(DATE(2013,6,7),-5)</f>
+        <f>WORKDAY(DATE(2013,6,1), -1)</f>
         <v>41425</v>
       </c>
       <c r="C48" s="18">
@@ -12438,14 +12429,14 @@
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B49" s="18">
-        <f>WORKDAY(DATE(2013,4,1),0)</f>
-        <v>41365</v>
+        <f>WORKDAY(DATE(2013,4,1),5)</f>
+        <v>41372</v>
       </c>
       <c r="C49" s="18">
-        <v>41365</v>
+        <v>41372</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
@@ -12455,11 +12446,11 @@
     <row r="50" spans="1:4" ht="15.75">
       <c r="A50" s="1"/>
       <c r="B50" s="18">
-        <f>WORKDAY(DATE(2013,6,1),0)</f>
-        <v>41426</v>
+        <f>WORKDAY(DATE(2013,4,5),1)</f>
+        <v>41372</v>
       </c>
       <c r="C50" s="18">
-        <v>41426</v>
+        <v>41372</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
@@ -12468,14 +12459,14 @@
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B51" s="18">
-        <f>WORKDAY(DATE(2013,4,1),3, DATE(2013,4,2))</f>
-        <v>41369</v>
+        <f>WORKDAY(DATE(2013,4,1),-1)</f>
+        <v>41362</v>
       </c>
       <c r="C51" s="18">
-        <v>41369</v>
+        <v>41362</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
@@ -12485,144 +12476,190 @@
     <row r="52" spans="1:4" ht="15.75">
       <c r="A52" s="1"/>
       <c r="B52" s="18">
+        <f>WORKDAY(DATE(2013,6,7),-5)</f>
+        <v>41425</v>
+      </c>
+      <c r="C52" s="18">
+        <v>41425</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75">
+      <c r="A53" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B53" s="18">
+        <f>WORKDAY(DATE(2013,4,1),0)</f>
+        <v>41365</v>
+      </c>
+      <c r="C53" s="18">
+        <v>41365</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75">
+      <c r="A54" s="1"/>
+      <c r="B54" s="18">
+        <f>WORKDAY(DATE(2013,6,1),0)</f>
+        <v>41426</v>
+      </c>
+      <c r="C54" s="18">
+        <v>41426</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75">
+      <c r="A55" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B55" s="18">
+        <f>WORKDAY(DATE(2013,4,1),3, DATE(2013,4,2))</f>
+        <v>41369</v>
+      </c>
+      <c r="C55" s="18">
+        <v>41369</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="1"/>
+      <c r="B56" s="18">
         <f>WORKDAY(DATE(2013,4,7), -3,DATE(2013,4,2))</f>
         <v>41367</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C56" s="18">
         <v>41367</v>
       </c>
-      <c r="D52" t="str">
+      <c r="D56" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75">
-      <c r="A53" s="1"/>
-      <c r="B53" s="18">
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="1"/>
+      <c r="B57" s="18">
         <f>WORKDAY(DATE(2013,4,3), -1,DATE(2013,4,2))</f>
         <v>41365</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C57" s="18">
         <v>41365</v>
       </c>
-      <c r="D53" t="str">
+      <c r="D57" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75">
+      <c r="A60" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B56">
+      <c r="B60">
         <f>YEAR(DATE(2008,1,1))</f>
         <v>2008</v>
       </c>
-      <c r="C56">
+      <c r="C60">
         <v>2008</v>
       </c>
-      <c r="D56" t="str">
-        <f>IF(B56=C56,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="1" t="s">
+      <c r="D60" t="str">
+        <f>IF(B60=C60,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75">
+      <c r="A62" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B58" s="22">
+      <c r="B62" s="22">
         <f>YEARFRAC(DATE(2012,1,1),DATE(2012,7,30))</f>
         <v>0.5805555555555556</v>
       </c>
-      <c r="C58" s="22">
+      <c r="C62" s="22">
         <v>0.5805555555555556</v>
       </c>
-      <c r="D58" t="str">
-        <f>IF(B58=C58,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="3" t="s">
+      <c r="D62" t="str">
+        <f>IF(B62=C62,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C60" s="21">
+      <c r="C64" s="21">
         <v>15</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D64" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="D63" s="18"/>
-    </row>
-    <row r="64" spans="1:4" ht="15.75">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.75">
+    <row r="65" spans="1:4" ht="15.75">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:2" ht="15.75">
+    <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:2" ht="15.75">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" ht="15.75">
+    <row r="67" spans="1:4">
+      <c r="D67" s="18"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:2" ht="15.75">
+    <row r="69" spans="1:4" ht="15.75">
       <c r="A69" s="1"/>
     </row>
-    <row r="73" spans="1:2" ht="15.75">
+    <row r="70" spans="1:4" ht="15.75">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" ht="15.75">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:2" ht="15.75">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:2" ht="15.75">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:2" ht="15.75">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.75">
+    <row r="77" spans="1:4" ht="15.75">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:2" ht="15.75">
+    <row r="78" spans="1:4" ht="15.75">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:2" ht="15.75">
+    <row r="79" spans="1:4" ht="15.75">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:2" ht="15.75">
+    <row r="80" spans="1:4" ht="15.75">
       <c r="A80" s="1"/>
-      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" ht="15.75">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:2" ht="15.75">
       <c r="A82" s="1"/>
-      <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:2" ht="15.75">
       <c r="A83" s="1"/>
@@ -12650,7 +12687,7 @@
     </row>
     <row r="90" spans="1:2" ht="15.75">
       <c r="A90" s="1"/>
-      <c r="B90" s="8"/>
+      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" ht="15.75">
       <c r="A91" s="1"/>
@@ -12664,12 +12701,14 @@
     </row>
     <row r="94" spans="1:2" ht="15.75">
       <c r="A94" s="1"/>
+      <c r="B94" s="8"/>
     </row>
     <row r="95" spans="1:2" ht="15.75">
       <c r="A95" s="1"/>
     </row>
     <row r="96" spans="1:2" ht="15.75">
       <c r="A96" s="1"/>
+      <c r="B96" s="5"/>
     </row>
     <row r="97" spans="1:1" ht="15.75">
       <c r="A97" s="1"/>
@@ -12724,110 +12763,109 @@
     </row>
     <row r="114" spans="1:2" ht="15.75">
       <c r="A114" s="1"/>
-      <c r="B114" s="5"/>
     </row>
     <row r="115" spans="1:2" ht="15.75">
       <c r="A115" s="1"/>
     </row>
     <row r="116" spans="1:2" ht="15.75">
       <c r="A116" s="1"/>
-      <c r="B116" s="5"/>
     </row>
     <row r="117" spans="1:2" ht="15.75">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" ht="15.75">
+      <c r="A118" s="1"/>
       <c r="B118" s="5"/>
     </row>
-    <row r="120" spans="1:2">
+    <row r="119" spans="1:2" ht="15.75">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.75">
+      <c r="A120" s="1"/>
       <c r="B120" s="5"/>
     </row>
-    <row r="122" spans="1:2" ht="15.75">
-      <c r="A122" s="1"/>
-      <c r="B122" s="8"/>
-    </row>
-    <row r="123" spans="1:2" ht="15.75">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.75">
-      <c r="A124" s="1"/>
+    <row r="121" spans="1:2" ht="15.75">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="B122" s="5"/>
+    </row>
+    <row r="124" spans="1:2">
       <c r="B124" s="5"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.75">
-      <c r="A125" s="1"/>
     </row>
     <row r="126" spans="1:2" ht="15.75">
       <c r="A126" s="1"/>
-      <c r="B126" s="5"/>
+      <c r="B126" s="8"/>
     </row>
     <row r="127" spans="1:2" ht="15.75">
       <c r="A127" s="1"/>
     </row>
     <row r="128" spans="1:2" ht="15.75">
       <c r="A128" s="1"/>
+      <c r="B128" s="5"/>
     </row>
     <row r="129" spans="1:2" ht="15.75">
       <c r="A129" s="1"/>
     </row>
     <row r="130" spans="1:2" ht="15.75">
       <c r="A130" s="1"/>
+      <c r="B130" s="5"/>
     </row>
     <row r="131" spans="1:2" ht="15.75">
       <c r="A131" s="1"/>
-      <c r="B131" s="5"/>
     </row>
     <row r="132" spans="1:2" ht="15.75">
       <c r="A132" s="1"/>
     </row>
     <row r="133" spans="1:2" ht="15.75">
       <c r="A133" s="1"/>
-      <c r="B133" s="11"/>
     </row>
     <row r="134" spans="1:2" ht="15.75">
       <c r="A134" s="1"/>
     </row>
     <row r="135" spans="1:2" ht="15.75">
       <c r="A135" s="1"/>
-      <c r="B135" s="9"/>
+      <c r="B135" s="5"/>
     </row>
     <row r="136" spans="1:2" ht="15.75">
       <c r="A136" s="1"/>
     </row>
     <row r="137" spans="1:2" ht="15.75">
       <c r="A137" s="1"/>
+      <c r="B137" s="11"/>
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="1"/>
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="1"/>
-      <c r="B139" s="5"/>
+      <c r="B139" s="9"/>
     </row>
     <row r="140" spans="1:2" ht="15.75">
       <c r="A140" s="1"/>
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="1"/>
-      <c r="B141" s="5"/>
     </row>
     <row r="142" spans="1:2" ht="15.75">
       <c r="A142" s="1"/>
     </row>
     <row r="143" spans="1:2" ht="15.75">
       <c r="A143" s="1"/>
+      <c r="B143" s="5"/>
     </row>
     <row r="144" spans="1:2" ht="15.75">
       <c r="A144" s="1"/>
     </row>
     <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="1"/>
+      <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="15.75">
       <c r="A146" s="1"/>
     </row>
     <row r="147" spans="1:2" ht="15.75">
       <c r="A147" s="1"/>
-      <c r="B147" s="8"/>
     </row>
     <row r="148" spans="1:2" ht="15.75">
       <c r="A148" s="1"/>
@@ -12840,6 +12878,7 @@
     </row>
     <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
+      <c r="B151" s="8"/>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
@@ -12855,40 +12894,40 @@
     </row>
     <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="1"/>
-      <c r="B156" s="12"/>
     </row>
     <row r="157" spans="1:2" ht="15.75">
       <c r="A157" s="1"/>
     </row>
     <row r="158" spans="1:2" ht="15.75">
       <c r="A158" s="1"/>
-      <c r="B158" s="8"/>
     </row>
     <row r="159" spans="1:2" ht="15.75">
       <c r="A159" s="1"/>
     </row>
     <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="1"/>
-      <c r="B160" s="5"/>
+      <c r="B160" s="12"/>
     </row>
     <row r="161" spans="1:2" ht="15.75">
       <c r="A161" s="1"/>
     </row>
     <row r="162" spans="1:2" ht="15.75">
       <c r="A162" s="1"/>
-      <c r="B162" s="11"/>
+      <c r="B162" s="8"/>
     </row>
     <row r="163" spans="1:2" ht="15.75">
       <c r="A163" s="1"/>
     </row>
     <row r="164" spans="1:2" ht="15.75">
       <c r="A164" s="1"/>
+      <c r="B164" s="5"/>
     </row>
     <row r="165" spans="1:2" ht="15.75">
       <c r="A165" s="1"/>
     </row>
     <row r="166" spans="1:2" ht="15.75">
       <c r="A166" s="1"/>
+      <c r="B166" s="11"/>
     </row>
     <row r="167" spans="1:2" ht="15.75">
       <c r="A167" s="1"/>
@@ -12970,7 +13009,6 @@
     </row>
     <row r="193" spans="1:2" ht="15.75">
       <c r="A193" s="1"/>
-      <c r="B193" s="5"/>
     </row>
     <row r="194" spans="1:2" ht="15.75">
       <c r="A194" s="1"/>
@@ -12980,10 +13018,10 @@
     </row>
     <row r="196" spans="1:2" ht="15.75">
       <c r="A196" s="1"/>
-      <c r="B196" s="5"/>
     </row>
     <row r="197" spans="1:2" ht="15.75">
       <c r="A197" s="1"/>
+      <c r="B197" s="5"/>
     </row>
     <row r="198" spans="1:2" ht="15.75">
       <c r="A198" s="1"/>
@@ -12993,6 +13031,7 @@
     </row>
     <row r="200" spans="1:2" ht="15.75">
       <c r="A200" s="1"/>
+      <c r="B200" s="5"/>
     </row>
     <row r="201" spans="1:2" ht="15.75">
       <c r="A201" s="1"/>
@@ -13018,78 +13057,78 @@
     <row r="208" spans="1:2" ht="15.75">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" spans="1:2" ht="15.75">
+    <row r="209" spans="1:1" ht="15.75">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" spans="1:2" ht="15.75">
+    <row r="210" spans="1:1" ht="15.75">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" spans="1:2" ht="15.75">
+    <row r="211" spans="1:1" ht="15.75">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" spans="1:2" ht="15.75">
+    <row r="212" spans="1:1" ht="15.75">
       <c r="A212" s="1"/>
     </row>
-    <row r="213" spans="1:2" ht="15.75">
+    <row r="213" spans="1:1" ht="15.75">
       <c r="A213" s="1"/>
     </row>
-    <row r="214" spans="1:2" ht="15.75">
+    <row r="214" spans="1:1" ht="15.75">
       <c r="A214" s="1"/>
     </row>
-    <row r="215" spans="1:2" ht="15.75">
+    <row r="215" spans="1:1" ht="15.75">
       <c r="A215" s="1"/>
     </row>
-    <row r="216" spans="1:2" ht="15.75">
+    <row r="216" spans="1:1" ht="15.75">
       <c r="A216" s="1"/>
     </row>
-    <row r="217" spans="1:2" ht="15.75">
+    <row r="217" spans="1:1" ht="15.75">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" spans="1:2" ht="15.75">
+    <row r="218" spans="1:1" ht="15.75">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" spans="1:2" ht="15.75">
+    <row r="219" spans="1:1" ht="15.75">
       <c r="A219" s="1"/>
     </row>
-    <row r="220" spans="1:2" ht="15.75">
+    <row r="220" spans="1:1" ht="15.75">
       <c r="A220" s="1"/>
     </row>
-    <row r="221" spans="1:2" ht="15.75">
+    <row r="221" spans="1:1" ht="15.75">
       <c r="A221" s="1"/>
     </row>
-    <row r="222" spans="1:2" ht="15.75">
+    <row r="222" spans="1:1" ht="15.75">
       <c r="A222" s="1"/>
     </row>
-    <row r="223" spans="1:2" ht="15.75">
+    <row r="223" spans="1:1" ht="15.75">
       <c r="A223" s="1"/>
-      <c r="B223" s="11"/>
-    </row>
-    <row r="224" spans="1:2" ht="15.75">
+    </row>
+    <row r="224" spans="1:1" ht="15.75">
       <c r="A224" s="1"/>
     </row>
     <row r="225" spans="1:2" ht="15.75">
       <c r="A225" s="1"/>
-      <c r="B225" s="11"/>
     </row>
     <row r="226" spans="1:2" ht="15.75">
       <c r="A226" s="1"/>
-      <c r="B226" s="11"/>
     </row>
     <row r="227" spans="1:2" ht="15.75">
       <c r="A227" s="1"/>
-      <c r="B227" s="5"/>
+      <c r="B227" s="11"/>
     </row>
     <row r="228" spans="1:2" ht="15.75">
       <c r="A228" s="1"/>
     </row>
     <row r="229" spans="1:2" ht="15.75">
       <c r="A229" s="1"/>
+      <c r="B229" s="11"/>
     </row>
     <row r="230" spans="1:2" ht="15.75">
       <c r="A230" s="1"/>
+      <c r="B230" s="11"/>
     </row>
     <row r="231" spans="1:2" ht="15.75">
       <c r="A231" s="1"/>
+      <c r="B231" s="5"/>
     </row>
     <row r="232" spans="1:2" ht="15.75">
       <c r="A232" s="1"/>
@@ -13142,11 +13181,23 @@
     <row r="248" spans="1:1" ht="15.75">
       <c r="A248" s="1"/>
     </row>
+    <row r="249" spans="1:1" ht="15.75">
+      <c r="A249" s="1"/>
+    </row>
     <row r="250" spans="1:1" ht="15.75">
       <c r="A250" s="1"/>
     </row>
-    <row r="479" spans="1:1">
-      <c r="A479" s="3" t="s">
+    <row r="251" spans="1:1" ht="15.75">
+      <c r="A251" s="1"/>
+    </row>
+    <row r="252" spans="1:1" ht="15.75">
+      <c r="A252" s="1"/>
+    </row>
+    <row r="254" spans="1:1" ht="15.75">
+      <c r="A254" s="1"/>
+    </row>
+    <row r="483" spans="1:1">
+      <c r="A483" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -13154,8 +13205,8 @@
   <sortState ref="A3:A29">
     <sortCondition ref="A3"/>
   </sortState>
-  <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D31 D33 D39 D56 D35 D58:D60 D41:D53 D19:D27">
-    <cfRule type="cellIs" dxfId="192" priority="5" operator="equal">
+  <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D35 D37 D43 D60 D39 D62:D64 D45:D57 D19:D31">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
* add more test cases for NETWORKDAYS(). * change test file format, add "invalid" for verification
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="formula-custom" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'formula-engineering'!$A$10:$C$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$8:$C$49</definedName>
@@ -191,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A45" authorId="0">
+    <comment ref="A46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D46" authorId="0">
+    <comment ref="D47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -239,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A62" authorId="0">
+    <comment ref="A63" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1402,7 +1402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="422">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2649,19 +2649,25 @@
     <t>count</t>
   </si>
   <si>
-    <t>invalid, different spec</t>
-  </si>
-  <si>
     <t>empty date</t>
   </si>
   <si>
-    <t>start date empty</t>
-  </si>
-  <si>
     <t>end date empty</t>
   </si>
   <si>
     <t>1900/1/1 is not workday in Excel</t>
+  </si>
+  <si>
+    <t>start later than end</t>
+  </si>
+  <si>
+    <t>start equals end</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>start date empty (different spce)</t>
   </si>
 </sst>
 </file>
@@ -7028,37 +7034,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7424,87 +7430,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7596,32 +7602,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8617,7 +8623,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>6.2854998038929466</v>
+        <v>43.953146225312281</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8635,7 +8641,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9739,8 +9745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10434,7 +10440,7 @@
         <v>0.7</v>
       </c>
       <c r="D73" t="s">
-        <v>403</v>
+        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -11894,10 +11900,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D483"/>
+  <dimension ref="A1:D484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12113,7 +12119,7 @@
         <v>108</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" ref="D20:D25" si="0">IF(B20=C20,"T","WARN")</f>
+        <f t="shared" ref="D20:D29" si="0">IF(B20=C20,"T","WARN")</f>
         <v>T</v>
       </c>
     </row>
@@ -12195,352 +12201,362 @@
     </row>
     <row r="26" spans="1:4" ht="15.75">
       <c r="A26" s="1" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B26">
+        <f>NETWORKDAYS(DATE(2013,6,28), DATE(2013,6,28))</f>
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75">
+      <c r="A27" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B27">
         <f>NETWORKDAYS(DATE(2013,6,2), DATE(2013,6,1))</f>
         <v>0</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75">
-      <c r="A27" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B27">
-        <f>NETWORKDAYS(E27,F27)</f>
-        <v>0</v>
-      </c>
       <c r="C27">
         <v>0</v>
       </c>
+      <c r="D27" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15.75">
       <c r="A28" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B28">
-        <f>NETWORKDAYS(B29,C29)</f>
+        <f>NETWORKDAYS(E28,F28)</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B29">
+        <f>NETWORKDAYS(B30,C30)</f>
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="B29" s="18"/>
-      <c r="C29" s="18">
+      <c r="C29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B30">
-        <f>NETWORKDAYS(C29, B29)</f>
-        <v>-1</v>
-      </c>
-      <c r="C30" s="21">
-        <v>-1</v>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>WARN</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75">
       <c r="A31" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B31">
+        <f>NETWORKDAYS(C30, B30)</f>
+        <v>-1</v>
+      </c>
+      <c r="C31" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B32">
         <f>NETWORKDAYS(DATE(1900,1,1),DATE(1900,1,1))</f>
         <v>0</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C32" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75">
-      <c r="A32" s="1"/>
-    </row>
     <row r="33" spans="1:4" ht="15.75">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B34" s="20">
         <f ca="1">NOW()</f>
-        <v>41452.423760300924</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75">
-      <c r="A34" s="1"/>
+        <v>41453.447021180553</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15.75">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
+      <c r="A36" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B35">
-        <f>SECOND(B36)</f>
+      <c r="B36">
+        <f>SECOND(B37)</f>
         <v>18</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>18</v>
       </c>
-      <c r="D35" t="str">
-        <f>IF(B35=C35,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75">
-      <c r="A36" s="1"/>
-      <c r="B36" s="33">
+      <c r="D36" t="str">
+        <f>IF(B36=C36,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" s="1"/>
+      <c r="B37" s="33">
         <v>0.70020833333333332</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B38" s="16">
         <f>TIME(12,0,0)</f>
         <v>0.5</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>0.5</v>
       </c>
-      <c r="D37" t="str">
-        <f>IF(B37=C37,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75">
-      <c r="A38" s="1"/>
+      <c r="D38" t="str">
+        <f>IF(B38=C38,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15.75">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75">
+      <c r="A40" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B40" s="5">
         <f>TIMEVALUE("2:24 AM")</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>0.1</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75">
-      <c r="A40" s="1"/>
-    </row>
     <row r="41" spans="1:4" ht="15.75">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B41" s="19">
+      <c r="B42" s="19">
         <f ca="1">TODAY()</f>
-        <v>41452</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75">
-      <c r="A42" s="1"/>
+        <v>41453</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15.75">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <f>WEEKDAY(DATE(2008,2,14))</f>
         <v>5</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>5</v>
       </c>
-      <c r="D43" t="str">
-        <f>IF(B43=C43,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75">
-      <c r="A44" s="1"/>
+      <c r="D44" t="str">
+        <f>IF(B44=C44,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15.75">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75">
+      <c r="A46" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B46" s="18">
         <f>WORKDAY(DATE(2013,4,1),4)</f>
         <v>41369</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C46" s="18">
         <v>41369</v>
       </c>
-      <c r="D45" t="str">
-        <f t="shared" ref="D45:D57" si="1">IF(B45=C45,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75">
-      <c r="A46" s="1"/>
-      <c r="B46" s="18">
+      <c r="D46" t="str">
+        <f t="shared" ref="D46:D58" si="1">IF(B46=C46,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75">
+      <c r="A47" s="1"/>
+      <c r="B47" s="18">
         <f>WORKDAY(DATE(2008,10,1),151)</f>
         <v>39933</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C47" s="18">
         <v>39933</v>
       </c>
-      <c r="D46" t="str">
+      <c r="D47" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:4" ht="15.75">
+      <c r="A48" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B48" s="18">
         <f>WORKDAY(DATE(2013,6,1),1)</f>
         <v>41428</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C48" s="18">
         <v>41428</v>
       </c>
-      <c r="D47" t="str">
+      <c r="D48" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75">
-      <c r="A48" s="1"/>
-      <c r="B48" s="18">
+    <row r="49" spans="1:4" ht="15.75">
+      <c r="A49" s="1"/>
+      <c r="B49" s="18">
         <f>WORKDAY(DATE(2013,6,1), -1)</f>
         <v>41425</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C49" s="18">
         <v>41425</v>
       </c>
-      <c r="D48" t="str">
+      <c r="D49" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:4" ht="15.75">
+      <c r="A50" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B49" s="18">
+      <c r="B50" s="18">
         <f>WORKDAY(DATE(2013,4,1),5)</f>
         <v>41372</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C50" s="18">
         <v>41372</v>
       </c>
-      <c r="D49" t="str">
+      <c r="D50" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75">
-      <c r="A50" s="1"/>
-      <c r="B50" s="18">
+    <row r="51" spans="1:4" ht="15.75">
+      <c r="A51" s="1"/>
+      <c r="B51" s="18">
         <f>WORKDAY(DATE(2013,4,5),1)</f>
         <v>41372</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C51" s="18">
         <v>41372</v>
       </c>
-      <c r="D50" t="str">
+      <c r="D51" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:4" ht="15.75">
+      <c r="A52" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="B51" s="18">
+      <c r="B52" s="18">
         <f>WORKDAY(DATE(2013,4,1),-1)</f>
         <v>41362</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C52" s="18">
         <v>41362</v>
       </c>
-      <c r="D51" t="str">
+      <c r="D52" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75">
-      <c r="A52" s="1"/>
-      <c r="B52" s="18">
+    <row r="53" spans="1:4" ht="15.75">
+      <c r="A53" s="1"/>
+      <c r="B53" s="18">
         <f>WORKDAY(DATE(2013,6,7),-5)</f>
         <v>41425</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C53" s="18">
         <v>41425</v>
       </c>
-      <c r="D52" t="str">
+      <c r="D53" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:4" ht="15.75">
+      <c r="A54" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B54" s="18">
         <f>WORKDAY(DATE(2013,4,1),0)</f>
         <v>41365</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C54" s="18">
         <v>41365</v>
       </c>
-      <c r="D53" t="str">
+      <c r="D54" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75">
-      <c r="A54" s="1"/>
-      <c r="B54" s="18">
+    <row r="55" spans="1:4" ht="15.75">
+      <c r="A55" s="1"/>
+      <c r="B55" s="18">
         <f>WORKDAY(DATE(2013,6,1),0)</f>
         <v>41426</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C55" s="18">
         <v>41426</v>
       </c>
-      <c r="D54" t="str">
+      <c r="D55" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B55" s="18">
+      <c r="B56" s="18">
         <f>WORKDAY(DATE(2013,4,1),3, DATE(2013,4,2))</f>
         <v>41369</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C56" s="18">
         <v>41369</v>
-      </c>
-      <c r="D55" t="str">
-        <f t="shared" si="1"/>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="1"/>
-      <c r="B56" s="18">
-        <f>WORKDAY(DATE(2013,4,7), -3,DATE(2013,4,2))</f>
-        <v>41367</v>
-      </c>
-      <c r="C56" s="18">
-        <v>41367</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="1"/>
@@ -12550,83 +12566,94 @@
     <row r="57" spans="1:4" ht="15.75">
       <c r="A57" s="1"/>
       <c r="B57" s="18">
+        <f>WORKDAY(DATE(2013,4,7), -3,DATE(2013,4,2))</f>
+        <v>41367</v>
+      </c>
+      <c r="C57" s="18">
+        <v>41367</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75">
+      <c r="A58" s="1"/>
+      <c r="B58" s="18">
         <f>WORKDAY(DATE(2013,4,3), -1,DATE(2013,4,2))</f>
         <v>41365</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C58" s="18">
         <v>41365</v>
       </c>
-      <c r="D57" t="str">
+      <c r="D58" t="str">
         <f t="shared" si="1"/>
         <v>T</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:4" ht="15.75">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:4" ht="15.75">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75">
+      <c r="A61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B60">
+      <c r="B61">
         <f>YEAR(DATE(2008,1,1))</f>
         <v>2008</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>2008</v>
       </c>
-      <c r="D60" t="str">
-        <f>IF(B60=C60,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75">
-      <c r="A61" s="1"/>
+      <c r="D61" t="str">
+        <f>IF(B61=C61,"T","WARN")</f>
+        <v>T</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="15.75">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75">
+      <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B62" s="22">
+      <c r="B63" s="22">
         <f>YEARFRAC(DATE(2012,1,1),DATE(2012,7,30))</f>
         <v>0.5805555555555556</v>
       </c>
-      <c r="C62" s="22">
+      <c r="C63" s="22">
         <v>0.5805555555555556</v>
       </c>
-      <c r="D62" t="str">
-        <f>IF(B62=C62,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="15.75">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="3" t="s">
+      <c r="D63" t="str">
+        <f>IF(B63=C63,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C64" s="21">
-        <v>15</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C65" s="21">
+        <v>36</v>
+      </c>
+      <c r="D65" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15.75">
-      <c r="A65" s="1"/>
     </row>
     <row r="66" spans="1:4" ht="15.75">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:4">
-      <c r="D67" s="18"/>
-    </row>
-    <row r="68" spans="1:4" ht="15.75">
-      <c r="A68" s="1"/>
+    <row r="67" spans="1:4" ht="15.75">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="D68" s="18"/>
     </row>
     <row r="69" spans="1:4" ht="15.75">
       <c r="A69" s="1"/>
@@ -12643,8 +12670,8 @@
     <row r="73" spans="1:4" ht="15.75">
       <c r="A73" s="1"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75">
-      <c r="A77" s="1"/>
+    <row r="74" spans="1:4" ht="15.75">
+      <c r="A74" s="1"/>
     </row>
     <row r="78" spans="1:4" ht="15.75">
       <c r="A78" s="1"/>
@@ -12666,96 +12693,96 @@
     </row>
     <row r="84" spans="1:2" ht="15.75">
       <c r="A84" s="1"/>
-      <c r="B84" s="5"/>
     </row>
     <row r="85" spans="1:2" ht="15.75">
       <c r="A85" s="1"/>
+      <c r="B85" s="5"/>
     </row>
     <row r="86" spans="1:2" ht="15.75">
       <c r="A86" s="1"/>
-      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="1:2" ht="15.75">
       <c r="A87" s="1"/>
+      <c r="B87" s="5"/>
     </row>
     <row r="88" spans="1:2" ht="15.75">
       <c r="A88" s="1"/>
-      <c r="B88" s="5"/>
     </row>
     <row r="89" spans="1:2" ht="15.75">
       <c r="A89" s="1"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="1:2" ht="15.75">
       <c r="A90" s="1"/>
-      <c r="B90" s="5"/>
     </row>
     <row r="91" spans="1:2" ht="15.75">
       <c r="A91" s="1"/>
+      <c r="B91" s="5"/>
     </row>
     <row r="92" spans="1:2" ht="15.75">
       <c r="A92" s="1"/>
-      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:2" ht="15.75">
       <c r="A93" s="1"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="1:2" ht="15.75">
       <c r="A94" s="1"/>
-      <c r="B94" s="8"/>
     </row>
     <row r="95" spans="1:2" ht="15.75">
       <c r="A95" s="1"/>
+      <c r="B95" s="8"/>
     </row>
     <row r="96" spans="1:2" ht="15.75">
       <c r="A96" s="1"/>
-      <c r="B96" s="5"/>
-    </row>
-    <row r="97" spans="1:1" ht="15.75">
+    </row>
+    <row r="97" spans="1:2" ht="15.75">
       <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:1" ht="15.75">
+      <c r="B97" s="5"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.75">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" ht="15.75">
+    <row r="99" spans="1:2" ht="15.75">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" ht="15.75">
+    <row r="100" spans="1:2" ht="15.75">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" ht="15.75">
+    <row r="101" spans="1:2" ht="15.75">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" ht="15.75">
+    <row r="102" spans="1:2" ht="15.75">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" ht="15.75">
+    <row r="103" spans="1:2" ht="15.75">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" ht="15.75">
+    <row r="104" spans="1:2" ht="15.75">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" ht="15.75">
+    <row r="105" spans="1:2" ht="15.75">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" ht="15.75">
+    <row r="106" spans="1:2" ht="15.75">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" ht="15.75">
+    <row r="107" spans="1:2" ht="15.75">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" ht="15.75">
+    <row r="108" spans="1:2" ht="15.75">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" ht="15.75">
+    <row r="109" spans="1:2" ht="15.75">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" ht="15.75">
+    <row r="110" spans="1:2" ht="15.75">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" ht="15.75">
+    <row r="111" spans="1:2" ht="15.75">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" ht="15.75">
+    <row r="112" spans="1:2" ht="15.75">
       <c r="A112" s="1"/>
     </row>
     <row r="113" spans="1:2" ht="15.75">
@@ -12775,44 +12802,44 @@
     </row>
     <row r="118" spans="1:2" ht="15.75">
       <c r="A118" s="1"/>
-      <c r="B118" s="5"/>
     </row>
     <row r="119" spans="1:2" ht="15.75">
       <c r="A119" s="1"/>
+      <c r="B119" s="5"/>
     </row>
     <row r="120" spans="1:2" ht="15.75">
       <c r="A120" s="1"/>
-      <c r="B120" s="5"/>
     </row>
     <row r="121" spans="1:2" ht="15.75">
       <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="B122" s="5"/>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="B124" s="5"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.75">
-      <c r="A126" s="1"/>
-      <c r="B126" s="8"/>
+      <c r="B121" s="5"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.75">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="B123" s="5"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="B125" s="5"/>
     </row>
     <row r="127" spans="1:2" ht="15.75">
       <c r="A127" s="1"/>
+      <c r="B127" s="8"/>
     </row>
     <row r="128" spans="1:2" ht="15.75">
       <c r="A128" s="1"/>
-      <c r="B128" s="5"/>
     </row>
     <row r="129" spans="1:2" ht="15.75">
       <c r="A129" s="1"/>
+      <c r="B129" s="5"/>
     </row>
     <row r="130" spans="1:2" ht="15.75">
       <c r="A130" s="1"/>
-      <c r="B130" s="5"/>
     </row>
     <row r="131" spans="1:2" ht="15.75">
       <c r="A131" s="1"/>
+      <c r="B131" s="5"/>
     </row>
     <row r="132" spans="1:2" ht="15.75">
       <c r="A132" s="1"/>
@@ -12825,24 +12852,24 @@
     </row>
     <row r="135" spans="1:2" ht="15.75">
       <c r="A135" s="1"/>
-      <c r="B135" s="5"/>
     </row>
     <row r="136" spans="1:2" ht="15.75">
       <c r="A136" s="1"/>
+      <c r="B136" s="5"/>
     </row>
     <row r="137" spans="1:2" ht="15.75">
       <c r="A137" s="1"/>
-      <c r="B137" s="11"/>
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="1"/>
+      <c r="B138" s="11"/>
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="1"/>
-      <c r="B139" s="9"/>
     </row>
     <row r="140" spans="1:2" ht="15.75">
       <c r="A140" s="1"/>
+      <c r="B140" s="9"/>
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="1"/>
@@ -12852,17 +12879,17 @@
     </row>
     <row r="143" spans="1:2" ht="15.75">
       <c r="A143" s="1"/>
-      <c r="B143" s="5"/>
     </row>
     <row r="144" spans="1:2" ht="15.75">
       <c r="A144" s="1"/>
+      <c r="B144" s="5"/>
     </row>
     <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="1"/>
-      <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="15.75">
       <c r="A146" s="1"/>
+      <c r="B146" s="5"/>
     </row>
     <row r="147" spans="1:2" ht="15.75">
       <c r="A147" s="1"/>
@@ -12878,10 +12905,10 @@
     </row>
     <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
-      <c r="B151" s="8"/>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
+      <c r="B152" s="8"/>
     </row>
     <row r="153" spans="1:2" ht="15.75">
       <c r="A153" s="1"/>
@@ -12906,31 +12933,31 @@
     </row>
     <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="1"/>
-      <c r="B160" s="12"/>
     </row>
     <row r="161" spans="1:2" ht="15.75">
       <c r="A161" s="1"/>
+      <c r="B161" s="12"/>
     </row>
     <row r="162" spans="1:2" ht="15.75">
       <c r="A162" s="1"/>
-      <c r="B162" s="8"/>
     </row>
     <row r="163" spans="1:2" ht="15.75">
       <c r="A163" s="1"/>
+      <c r="B163" s="8"/>
     </row>
     <row r="164" spans="1:2" ht="15.75">
       <c r="A164" s="1"/>
-      <c r="B164" s="5"/>
     </row>
     <row r="165" spans="1:2" ht="15.75">
       <c r="A165" s="1"/>
+      <c r="B165" s="5"/>
     </row>
     <row r="166" spans="1:2" ht="15.75">
       <c r="A166" s="1"/>
-      <c r="B166" s="11"/>
     </row>
     <row r="167" spans="1:2" ht="15.75">
       <c r="A167" s="1"/>
+      <c r="B167" s="11"/>
     </row>
     <row r="168" spans="1:2" ht="15.75">
       <c r="A168" s="1"/>
@@ -13021,20 +13048,20 @@
     </row>
     <row r="197" spans="1:2" ht="15.75">
       <c r="A197" s="1"/>
-      <c r="B197" s="5"/>
     </row>
     <row r="198" spans="1:2" ht="15.75">
       <c r="A198" s="1"/>
+      <c r="B198" s="5"/>
     </row>
     <row r="199" spans="1:2" ht="15.75">
       <c r="A199" s="1"/>
     </row>
     <row r="200" spans="1:2" ht="15.75">
       <c r="A200" s="1"/>
-      <c r="B200" s="5"/>
     </row>
     <row r="201" spans="1:2" ht="15.75">
       <c r="A201" s="1"/>
+      <c r="B201" s="5"/>
     </row>
     <row r="202" spans="1:2" ht="15.75">
       <c r="A202" s="1"/>
@@ -13113,14 +13140,13 @@
     </row>
     <row r="227" spans="1:2" ht="15.75">
       <c r="A227" s="1"/>
-      <c r="B227" s="11"/>
     </row>
     <row r="228" spans="1:2" ht="15.75">
       <c r="A228" s="1"/>
+      <c r="B228" s="11"/>
     </row>
     <row r="229" spans="1:2" ht="15.75">
       <c r="A229" s="1"/>
-      <c r="B229" s="11"/>
     </row>
     <row r="230" spans="1:2" ht="15.75">
       <c r="A230" s="1"/>
@@ -13128,10 +13154,11 @@
     </row>
     <row r="231" spans="1:2" ht="15.75">
       <c r="A231" s="1"/>
-      <c r="B231" s="5"/>
+      <c r="B231" s="11"/>
     </row>
     <row r="232" spans="1:2" ht="15.75">
       <c r="A232" s="1"/>
+      <c r="B232" s="5"/>
     </row>
     <row r="233" spans="1:2" ht="15.75">
       <c r="A233" s="1"/>
@@ -13193,11 +13220,14 @@
     <row r="252" spans="1:1" ht="15.75">
       <c r="A252" s="1"/>
     </row>
-    <row r="254" spans="1:1" ht="15.75">
-      <c r="A254" s="1"/>
-    </row>
-    <row r="483" spans="1:1">
-      <c r="A483" s="3" t="s">
+    <row r="253" spans="1:1" ht="15.75">
+      <c r="A253" s="1"/>
+    </row>
+    <row r="255" spans="1:1" ht="15.75">
+      <c r="A255" s="1"/>
+    </row>
+    <row r="484" spans="1:1">
+      <c r="A484" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -13205,8 +13235,8 @@
   <sortState ref="A3:A29">
     <sortCondition ref="A3"/>
   </sortState>
-  <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D35 D37 D43 D60 D39 D62:D64 D45:D57 D19:D31">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+  <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D36 D38 D44 D61 D40 D63:D65 D46:D58 D19:D32">
+    <cfRule type="cellIs" dxfId="191" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15244,62 +15274,62 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="191" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="190" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="189" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="188" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
-    <cfRule type="cellIs" dxfId="187" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112 D114 D116 D120 D122 D124">
-    <cfRule type="cellIs" dxfId="186" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="185" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="184" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="183" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="182" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="181" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18702,747 +18732,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="179" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="178" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="177" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="176" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="175" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="174" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="173" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="172" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="171" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="170" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="169" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="168" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="167" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="166" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="165" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="164" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="163" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="162" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="161" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="160" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="159" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="158" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="157" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="156" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="155" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="154" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="153" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="152" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="151" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="150" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="149" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="148" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="147" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="146" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="145" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="144" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="143" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="142" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="141" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="140" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="139" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="138" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="137" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="136" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="135" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="134" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="133" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="132" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="131" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="130" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="129" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="128" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="127" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="126" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="125" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="124" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="123" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="122" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="121" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="120" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="119" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="118" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="117" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="116" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="115" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="114" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="113" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="112" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="111" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="110" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="109" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="108" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="107" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="106" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="105" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="104" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="103" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="102" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="101" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="100" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="99" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="98" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="97" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="96" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="95" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="94" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="93" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="92" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="91" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="90" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="89" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="88" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="87" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="86" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="85" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="84" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="83" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="82" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="81" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="80" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="79" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="78" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="77" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="76" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="75" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="74" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="73" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="72" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="71" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="69" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="68" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="67" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="66" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="65" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="64" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="63" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="62" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="61" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="60" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="59" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="58" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="57" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="55" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="53" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="50" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="49" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="48" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="47" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="46" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="45" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a formula - TBILLPRICE in test file
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -465,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A114" authorId="0">
+    <comment ref="A117" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1402,7 +1402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="422">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2841,7 +2841,19 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="202">
+  <dxfs count="203">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -5269,6 +5281,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FF0000FF"/>
       <color rgb="FF3333FF"/>
@@ -5287,7 +5365,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5596,12 +5674,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="201" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="200" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7034,37 +7112,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7430,87 +7508,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7602,32 +7680,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7720,12 +7798,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="199" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="198" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8623,7 +8701,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>43.953146225312281</v>
+        <v>28.290524368504009</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8641,7 +8719,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9522,7 +9600,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="197" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9732,7 +9810,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="196" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9745,7 +9823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -10898,7 +10976,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="195" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11879,17 +11957,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D15 D18 D21 D23 D26 D29 D31 D8:D12">
-    <cfRule type="cellIs" dxfId="194" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="193" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="192" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12301,7 +12379,7 @@
       </c>
       <c r="B34" s="20">
         <f ca="1">NOW()</f>
-        <v>41453.447021180553</v>
+        <v>41499.618067129632</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75">
@@ -12372,7 +12450,7 @@
       </c>
       <c r="B42" s="19">
         <f ca="1">TODAY()</f>
-        <v>41453</v>
+        <v>41499</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75">
@@ -13236,7 +13314,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D36 D38 D44 D61 D40 D63:D65 D46:D58 D19:D32">
-    <cfRule type="cellIs" dxfId="191" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13248,10 +13326,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I536"/>
+  <dimension ref="A1:I539"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14540,188 +14618,210 @@
     </row>
     <row r="112" spans="1:4" ht="15.75">
       <c r="A112" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B112">
+        <f>TBILLPRICE(B113,C113,D113)</f>
+        <v>98.45</v>
+      </c>
+      <c r="C112">
+        <v>98.45</v>
+      </c>
+      <c r="D112" t="str">
+        <f>IF(B112=C112,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75">
+      <c r="A113" s="1"/>
+      <c r="B113" s="18">
+        <v>39538</v>
+      </c>
+      <c r="C113" s="18">
+        <v>39600</v>
+      </c>
+      <c r="D113">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15.75">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:7" ht="15.75">
+      <c r="A115" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B112" s="22">
+      <c r="B115" s="22">
         <f>TBILLYIELD(DATE(2008,3,31),DATE(2008,6,1), 98.45)</f>
         <v>9.141696292534264E-2</v>
       </c>
-      <c r="C112" s="22">
+      <c r="C115" s="22">
         <v>9.141696292534264E-2</v>
       </c>
-      <c r="D112" t="str">
-        <f>IF(B112=C112,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="15.75">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:7" ht="15.75">
-      <c r="A114" s="1" t="s">
+      <c r="D115" t="str">
+        <f>IF(B115=C115,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:7" ht="15.75">
+      <c r="A117" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B114" s="22">
+      <c r="B117" s="22">
         <f>VDB(2400,400,10*365,0,1)</f>
         <v>1.3150684931506849</v>
       </c>
-      <c r="C114" s="22">
+      <c r="C117" s="22">
         <v>1.3150684931506849</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D117" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="15.75">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:7" ht="15.75">
-      <c r="A116" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B116" s="22">
-        <f>XNPV(0.09,B117:F117,B118:F118)</f>
-        <v>2086.6476020315349</v>
-      </c>
-      <c r="C116" s="22">
-        <v>2086.6476020315349</v>
-      </c>
-      <c r="D116" t="str">
-        <f>IF(B116=C116,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="15.75">
-      <c r="A117" s="1"/>
-      <c r="B117">
-        <v>-10000</v>
-      </c>
-      <c r="C117">
-        <v>2750</v>
-      </c>
-      <c r="D117">
-        <v>4250</v>
-      </c>
-      <c r="E117">
-        <v>3250</v>
-      </c>
-      <c r="F117">
-        <v>2750</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75">
       <c r="A118" s="1"/>
-      <c r="B118" s="18">
+    </row>
+    <row r="119" spans="1:7" ht="15.75">
+      <c r="A119" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B119" s="22">
+        <f>XNPV(0.09,B120:F120,B121:F121)</f>
+        <v>2086.6476020315349</v>
+      </c>
+      <c r="C119" s="22">
+        <v>2086.6476020315349</v>
+      </c>
+      <c r="D119" t="str">
+        <f>IF(B119=C119,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15.75">
+      <c r="A120" s="1"/>
+      <c r="B120">
+        <v>-10000</v>
+      </c>
+      <c r="C120">
+        <v>2750</v>
+      </c>
+      <c r="D120">
+        <v>4250</v>
+      </c>
+      <c r="E120">
+        <v>3250</v>
+      </c>
+      <c r="F120">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75">
+      <c r="A121" s="1"/>
+      <c r="B121" s="18">
         <v>39448</v>
       </c>
-      <c r="C118" s="18">
+      <c r="C121" s="18">
         <v>39508</v>
       </c>
-      <c r="D118" s="18">
+      <c r="D121" s="18">
         <v>39751</v>
       </c>
-      <c r="E118" s="18">
+      <c r="E121" s="18">
         <v>39859</v>
       </c>
-      <c r="F118" s="18">
+      <c r="F121" s="18">
         <v>39904</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15.75">
-      <c r="A119" s="1"/>
-      <c r="B119" s="18"/>
-      <c r="C119" s="18"/>
-      <c r="D119" s="18"/>
-      <c r="E119" s="18"/>
-      <c r="F119" s="18"/>
-    </row>
-    <row r="120" spans="1:7" ht="15.75">
-      <c r="A120" s="1" t="s">
+    <row r="122" spans="1:7" ht="15.75">
+      <c r="A122" s="1"/>
+      <c r="B122" s="18"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="18"/>
+    </row>
+    <row r="123" spans="1:7" ht="15.75">
+      <c r="A123" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B120" s="22">
+      <c r="B123" s="22">
         <f>YIELD(DATE(2008,2,14), DATE(2016,11,15), 0.0575, 95.04287, 100, 2,0)</f>
         <v>6.4998178600204778E-2</v>
       </c>
-      <c r="C120" s="22">
+      <c r="C123" s="22">
         <v>6.4998178600204778E-2</v>
       </c>
-      <c r="D120" t="str">
-        <f>IF(B120=C120,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="15.75">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" ht="15.75">
-      <c r="A122" s="1" t="s">
+      <c r="D123" t="str">
+        <f>IF(B123=C123,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15.75">
+      <c r="A124" s="1"/>
+    </row>
+    <row r="125" spans="1:7" ht="15.75">
+      <c r="A125" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B122" s="22">
+      <c r="B125" s="22">
         <f>YIELDDISC(DATE(2008,2,16), DATE(2008,3,1), 99.795, 100, 2)</f>
         <v>5.2822571986858337E-2</v>
       </c>
-      <c r="C122" s="22">
+      <c r="C125" s="22">
         <v>5.2822571986858337E-2</v>
       </c>
-      <c r="D122" t="str">
-        <f>IF(B122=C122,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="15.75">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:7" ht="15.75">
-      <c r="A124" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B124" s="22">
-        <f>YIELDMAT(B125,C125,D125,E125,F125,G125)</f>
-        <v>6.0954333691538673E-2</v>
-      </c>
-      <c r="C124" s="22">
-        <v>6.0954333691538673E-2</v>
-      </c>
-      <c r="D124" t="str">
-        <f>IF(B124=C124,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="15.75">
-      <c r="A125" s="1"/>
-      <c r="B125" s="18">
-        <v>39522</v>
-      </c>
-      <c r="C125" s="18">
-        <v>39755</v>
-      </c>
-      <c r="D125" s="18">
-        <v>39394</v>
-      </c>
-      <c r="E125" s="21">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F125" s="21">
-        <v>100.0123</v>
-      </c>
-      <c r="G125" s="21">
-        <v>0</v>
+      <c r="D125" t="str">
+        <f>IF(B125=C125,"T","WARN")</f>
+        <v>T</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="1"/>
     </row>
+    <row r="127" spans="1:7" ht="15.75">
+      <c r="A127" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B127" s="22">
+        <f>YIELDMAT(B128,C128,D128,E128,F128,G128)</f>
+        <v>6.0954333691538673E-2</v>
+      </c>
+      <c r="C127" s="22">
+        <v>6.0954333691538673E-2</v>
+      </c>
+      <c r="D127" t="str">
+        <f>IF(B127=C127,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
     <row r="128" spans="1:7" ht="15.75">
       <c r="A128" s="1"/>
+      <c r="B128" s="18">
+        <v>39522</v>
+      </c>
+      <c r="C128" s="18">
+        <v>39755</v>
+      </c>
+      <c r="D128" s="18">
+        <v>39394</v>
+      </c>
+      <c r="E128" s="21">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F128" s="21">
+        <v>100.0123</v>
+      </c>
+      <c r="G128" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:2" ht="15.75">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:2" ht="15.75">
-      <c r="A130" s="1"/>
-    </row>
     <row r="131" spans="1:2" ht="15.75">
       <c r="A131" s="1"/>
     </row>
@@ -14736,101 +14836,101 @@
     </row>
     <row r="135" spans="1:2" ht="15.75">
       <c r="A135" s="1"/>
-      <c r="B135" s="5"/>
     </row>
     <row r="136" spans="1:2" ht="15.75">
       <c r="A136" s="1"/>
     </row>
     <row r="137" spans="1:2" ht="15.75">
       <c r="A137" s="1"/>
-      <c r="B137" s="5"/>
     </row>
     <row r="138" spans="1:2" ht="15.75">
       <c r="A138" s="1"/>
+      <c r="B138" s="5"/>
     </row>
     <row r="139" spans="1:2" ht="15.75">
       <c r="A139" s="1"/>
-      <c r="B139" s="5"/>
     </row>
     <row r="140" spans="1:2" ht="15.75">
       <c r="A140" s="1"/>
+      <c r="B140" s="5"/>
     </row>
     <row r="141" spans="1:2" ht="15.75">
       <c r="A141" s="1"/>
-      <c r="B141" s="8"/>
     </row>
     <row r="142" spans="1:2" ht="15.75">
       <c r="A142" s="1"/>
+      <c r="B142" s="5"/>
     </row>
     <row r="143" spans="1:2" ht="15.75">
       <c r="A143" s="1"/>
-      <c r="B143" s="5"/>
     </row>
     <row r="144" spans="1:2" ht="15.75">
       <c r="A144" s="1"/>
+      <c r="B144" s="8"/>
     </row>
     <row r="145" spans="1:2" ht="15.75">
       <c r="A145" s="1"/>
-      <c r="B145" s="5"/>
     </row>
     <row r="146" spans="1:2" ht="15.75">
       <c r="A146" s="1"/>
+      <c r="B146" s="5"/>
     </row>
     <row r="147" spans="1:2" ht="15.75">
       <c r="A147" s="1"/>
     </row>
     <row r="148" spans="1:2" ht="15.75">
       <c r="A148" s="1"/>
+      <c r="B148" s="5"/>
     </row>
     <row r="149" spans="1:2" ht="15.75">
       <c r="A149" s="1"/>
     </row>
     <row r="150" spans="1:2" ht="15.75">
       <c r="A150" s="1"/>
-      <c r="B150" s="5"/>
     </row>
     <row r="151" spans="1:2" ht="15.75">
       <c r="A151" s="1"/>
     </row>
     <row r="152" spans="1:2" ht="15.75">
       <c r="A152" s="1"/>
-      <c r="B152" s="11"/>
     </row>
     <row r="153" spans="1:2" ht="15.75">
       <c r="A153" s="1"/>
+      <c r="B153" s="5"/>
     </row>
     <row r="154" spans="1:2" ht="15.75">
       <c r="A154" s="1"/>
-      <c r="B154" s="9"/>
     </row>
     <row r="155" spans="1:2" ht="15.75">
       <c r="A155" s="1"/>
+      <c r="B155" s="11"/>
     </row>
     <row r="156" spans="1:2" ht="15.75">
       <c r="A156" s="1"/>
     </row>
     <row r="157" spans="1:2" ht="15.75">
       <c r="A157" s="1"/>
+      <c r="B157" s="9"/>
     </row>
     <row r="158" spans="1:2" ht="15.75">
       <c r="A158" s="1"/>
-      <c r="B158" s="5"/>
     </row>
     <row r="159" spans="1:2" ht="15.75">
       <c r="A159" s="1"/>
     </row>
     <row r="160" spans="1:2" ht="15.75">
       <c r="A160" s="1"/>
-      <c r="B160" s="5"/>
     </row>
     <row r="161" spans="1:2" ht="15.75">
       <c r="A161" s="1"/>
+      <c r="B161" s="5"/>
     </row>
     <row r="162" spans="1:2" ht="15.75">
       <c r="A162" s="1"/>
     </row>
     <row r="163" spans="1:2" ht="15.75">
       <c r="A163" s="1"/>
+      <c r="B163" s="5"/>
     </row>
     <row r="164" spans="1:2" ht="15.75">
       <c r="A164" s="1"/>
@@ -14840,7 +14940,6 @@
     </row>
     <row r="166" spans="1:2" ht="15.75">
       <c r="A166" s="1"/>
-      <c r="B166" s="8"/>
     </row>
     <row r="167" spans="1:2" ht="15.75">
       <c r="A167" s="1"/>
@@ -14850,6 +14949,7 @@
     </row>
     <row r="169" spans="1:2" ht="15.75">
       <c r="A169" s="1"/>
+      <c r="B169" s="8"/>
     </row>
     <row r="170" spans="1:2" ht="15.75">
       <c r="A170" s="1"/>
@@ -14866,31 +14966,31 @@
     <row r="174" spans="1:2" ht="15.75">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:2">
-      <c r="B175" s="12"/>
-    </row>
-    <row r="177" spans="1:2">
-      <c r="B177" s="8"/>
-    </row>
-    <row r="179" spans="1:2" ht="15.75">
-      <c r="A179" s="1"/>
-      <c r="B179" s="5"/>
-    </row>
-    <row r="180" spans="1:2" ht="15.75">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:2" ht="15.75">
-      <c r="A181" s="1"/>
-      <c r="B181" s="11"/>
+    <row r="175" spans="1:2" ht="15.75">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:2" ht="15.75">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:2" ht="15.75">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="B178" s="12"/>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="B180" s="8"/>
     </row>
     <row r="182" spans="1:2" ht="15.75">
       <c r="A182" s="1"/>
+      <c r="B182" s="5"/>
     </row>
     <row r="183" spans="1:2" ht="15.75">
       <c r="A183" s="1"/>
     </row>
     <row r="184" spans="1:2" ht="15.75">
       <c r="A184" s="1"/>
+      <c r="B184" s="11"/>
     </row>
     <row r="185" spans="1:2" ht="15.75">
       <c r="A185" s="1"/>
@@ -14975,7 +15075,6 @@
     </row>
     <row r="212" spans="1:2" ht="15.75">
       <c r="A212" s="1"/>
-      <c r="B212" s="5"/>
     </row>
     <row r="213" spans="1:2" ht="15.75">
       <c r="A213" s="1"/>
@@ -14995,6 +15094,7 @@
     </row>
     <row r="218" spans="1:2" ht="15.75">
       <c r="A218" s="1"/>
+      <c r="B218" s="5"/>
     </row>
     <row r="219" spans="1:2" ht="15.75">
       <c r="A219" s="1"/>
@@ -15067,14 +15167,12 @@
     </row>
     <row r="242" spans="1:2" ht="15.75">
       <c r="A242" s="1"/>
-      <c r="B242" s="11"/>
     </row>
     <row r="243" spans="1:2" ht="15.75">
       <c r="A243" s="1"/>
     </row>
     <row r="244" spans="1:2" ht="15.75">
       <c r="A244" s="1"/>
-      <c r="B244" s="11"/>
     </row>
     <row r="245" spans="1:2" ht="15.75">
       <c r="A245" s="1"/>
@@ -15082,16 +15180,18 @@
     </row>
     <row r="246" spans="1:2" ht="15.75">
       <c r="A246" s="1"/>
-      <c r="B246" s="5"/>
     </row>
     <row r="247" spans="1:2" ht="15.75">
       <c r="A247" s="1"/>
+      <c r="B247" s="11"/>
     </row>
     <row r="248" spans="1:2" ht="15.75">
       <c r="A248" s="1"/>
+      <c r="B248" s="11"/>
     </row>
     <row r="249" spans="1:2" ht="15.75">
       <c r="A249" s="1"/>
+      <c r="B249" s="5"/>
     </row>
     <row r="250" spans="1:2" ht="15.75">
       <c r="A250" s="1"/>
@@ -15261,11 +15361,20 @@
     <row r="305" spans="1:1" ht="15.75">
       <c r="A305" s="1"/>
     </row>
+    <row r="306" spans="1:1" ht="15.75">
+      <c r="A306" s="1"/>
+    </row>
     <row r="307" spans="1:1" ht="15.75">
       <c r="A307" s="1"/>
     </row>
-    <row r="536" spans="1:1">
-      <c r="A536" s="3" t="s">
+    <row r="308" spans="1:1" ht="15.75">
+      <c r="A308" s="1"/>
+    </row>
+    <row r="310" spans="1:1" ht="15.75">
+      <c r="A310" s="1"/>
+    </row>
+    <row r="539" spans="1:1">
+      <c r="A539" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15274,62 +15383,67 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="190" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="189" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="188" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="187" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
-    <cfRule type="cellIs" dxfId="186" priority="8" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D112 D114 D116 D120 D122 D124">
-    <cfRule type="cellIs" dxfId="185" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D115 D117 D119 D123 D125 D127">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="184" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="183" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="182" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="181" priority="3" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="180" priority="2" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D114">
-    <cfRule type="cellIs" dxfId="179" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D117">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D117">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18732,747 +18846,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="178" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="177" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="176" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="175" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="174" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="173" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="172" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="171" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="170" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="169" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="168" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="167" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="166" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="165" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="164" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="163" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="162" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="161" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="160" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="159" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="158" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="157" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="156" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="155" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="154" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="153" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="152" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="151" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="150" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="149" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="148" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="147" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="146" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="145" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="144" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="143" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="142" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="141" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="140" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="139" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="138" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="137" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="136" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="135" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="134" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="133" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="132" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="131" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="130" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="129" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="128" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="127" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="126" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="125" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="124" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="123" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="122" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="121" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="120" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="119" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="118" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="117" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="116" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="115" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="114" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="113" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="112" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="111" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="110" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="109" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="108" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="107" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="106" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="105" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="104" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="103" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="102" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="101" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="100" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="99" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="98" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="97" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="96" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="95" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="94" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="93" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="92" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="91" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="90" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="89" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="88" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="87" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="86" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="85" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="84" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="82" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="81" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="79" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="78" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="77" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="76" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="75" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="74" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="73" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="72" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="71" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="70" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="69" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="67" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="66" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="65" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="64" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="63" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="62" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="61" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="60" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="58" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="57" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="56" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="55" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="54" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="53" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="52" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="51" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="50" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="49" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="47" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="46" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="45" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="43" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add more formulas supported by POI in test excel file, category: Lookup & Reference
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
+++ b/zss.test/src/main/webapp/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -17,8 +17,9 @@
     <sheet name="formula-financial" sheetId="8" r:id="rId8"/>
     <sheet name="formula-statistical" sheetId="9" r:id="rId9"/>
     <sheet name="formula-engineering" sheetId="10" r:id="rId10"/>
-    <sheet name="formula-notsupported" sheetId="11" r:id="rId11"/>
-    <sheet name="formula-custom" sheetId="13" r:id="rId12"/>
+    <sheet name="formula-custom" sheetId="13" r:id="rId11"/>
+    <sheet name="formula-notsupported" sheetId="11" r:id="rId12"/>
+    <sheet name="formula-lookup" sheetId="16" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'formula-datetime'!$A$10:$C$61</definedName>
@@ -26,6 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'formula-financial'!$A$13:$C$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'formula-info'!$A$8:$C$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'formula-logical'!$A$8:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'formula-lookup'!$A$11:$C$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'formula-math'!$A$9:$C$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'formula-statistical'!$A$11:$C$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'formula-text'!$A$4:$C$34</definedName>
@@ -1402,7 +1404,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="457">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2668,6 +2670,111 @@
   </si>
   <si>
     <t>start date empty (different spce)</t>
+  </si>
+  <si>
+    <t>Lookup</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>AREAS</t>
+  </si>
+  <si>
+    <t>CHOOSE</t>
+  </si>
+  <si>
+    <t>COLUMN</t>
+  </si>
+  <si>
+    <t>COLUMNS</t>
+  </si>
+  <si>
+    <t>HLOOKUP</t>
+  </si>
+  <si>
+    <t>HYPERLINK</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>INDIRECT</t>
+  </si>
+  <si>
+    <t>LOOKUP</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>OFFSET</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>ROWS</t>
+  </si>
+  <si>
+    <t>RTD</t>
+  </si>
+  <si>
+    <t>TRANSPOSE</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>Axles</t>
+  </si>
+  <si>
+    <t>Bearings</t>
+  </si>
+  <si>
+    <t>Bolts</t>
+  </si>
+  <si>
+    <t>bananas</t>
+  </si>
+  <si>
+    <t>lemons</t>
+  </si>
+  <si>
+    <t>pears</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>$C$2</t>
+  </si>
+  <si>
+    <t>offset input</t>
   </si>
 </sst>
 </file>
@@ -2793,7 +2900,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2836,12 +2943,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="203">
+  <dxfs count="204">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -5674,12 +5794,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5692,7 +5812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -7112,37 +7232,37 @@
     <sortCondition ref="D3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D5 D7 D9 D11">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 D15 D17 D19 D21 D23 D25 D27 D29">
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D33 D35 D37 D39 D41 D43">
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47 D51 D49 D53 D55 D57 D59 D61 D63 D65 D67 D69 D71 D73 D75 D77">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7152,6 +7272,121 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="e">
+        <f ca="1">toTWD(B4,C4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3" t="e">
+        <f ca="1">IF(B3=C3,"T","WARN")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B6" t="e">
+        <f ca="1">USD2NTD(B7,C7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6" t="e">
+        <f ca="1">IF(B6=C6,"T","WARN")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -7508,87 +7743,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="34" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D22 E21:F22">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25 E25">
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7598,25 +7833,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D522"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="4" t="s">
-        <v>400</v>
+        <v>422</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -7625,91 +7864,1169 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
+    <row r="2" spans="1:4" ht="25.5" customHeight="1"/>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B3" t="e">
-        <f ca="1">toTWD(B4,C4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C3">
+        <v>423</v>
+      </c>
+      <c r="B3" s="22" t="str">
+        <f>ADDRESS(2,3)</f>
+        <v>$C$2</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(B3=C3,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="1"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="1"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" s="22" t="str">
+        <f>CHOOSE(2,B8,C8,D8)</f>
+        <v>2nd</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(B7=C7,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="D8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75">
+      <c r="A9" s="1"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75">
+      <c r="A10" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B10" s="21">
+        <f>COLUMN()</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2</v>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(B10=C10,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75">
+      <c r="A11" s="1"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
+      <c r="A12" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B12" s="7">
+        <f>COLUMNS(C1:E4)</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(B12=C12,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75">
+      <c r="A13" s="1"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75">
+      <c r="A14" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B14" s="21">
+        <f>HLOOKUP("Axles",B15:D18,2,TRUE)</f>
+        <v>4</v>
+      </c>
+      <c r="C14" s="21">
+        <v>4</v>
+      </c>
+      <c r="D14" t="str">
+        <f>IF(B14=C14,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="A15" s="1"/>
+      <c r="B15" s="21" t="s">
+        <v>443</v>
+      </c>
+      <c r="C15" t="s">
+        <v>444</v>
+      </c>
+      <c r="D15" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75">
+      <c r="A16" s="1"/>
+      <c r="B16" s="21">
+        <v>4</v>
+      </c>
+      <c r="C16" s="21">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
+      <c r="A17" s="1"/>
+      <c r="B17" s="21">
+        <v>5</v>
+      </c>
+      <c r="C17" s="21">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="1"/>
+      <c r="B18" s="21">
+        <v>6</v>
+      </c>
+      <c r="C18" s="21">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
+      <c r="A19" s="1"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
+      <c r="A20" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B20" s="36" t="str">
+        <f>HYPERLINK("http://www.zkoss.org", "ZK")</f>
+        <v>ZK</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="str">
+        <f>IF(B20=C20,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
+      <c r="A21" s="1"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
+      <c r="A22" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B22" s="34" t="str">
+        <f>INDEX(B23:C24,2,2)</f>
+        <v>pears</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>448</v>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(B22=C22,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" s="1"/>
+      <c r="B23" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75">
+      <c r="A24" s="1"/>
+      <c r="B24" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
+      <c r="A25" s="1"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
+      <c r="A26" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B26" s="21">
+        <f ca="1">INDIRECT($B$27)</f>
+        <v>1.333</v>
+      </c>
+      <c r="C26" s="21">
+        <v>1.333</v>
+      </c>
+      <c r="D26" t="str">
+        <f ca="1">IF(B26=C26,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75">
+      <c r="A27" s="1"/>
+      <c r="B27" t="s">
+        <v>449</v>
+      </c>
+      <c r="C27" s="21">
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75">
+      <c r="A28" s="1"/>
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B29" s="21" t="str">
+        <f>LOOKUP(4.19,B30:B34,C30:C34)</f>
+        <v>orange</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="D29" t="str">
+        <f>IF(B29=C29,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75">
+      <c r="A30" s="1"/>
+      <c r="B30" s="21">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
+      <c r="A31" s="1"/>
+      <c r="B31" s="21">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="1"/>
+      <c r="B32" s="21">
+        <v>5.17</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75">
+      <c r="A33" s="1"/>
+      <c r="B33" s="21">
+        <v>5.77</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75">
+      <c r="A34" s="1"/>
+      <c r="B34" s="21">
+        <v>6.39</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75">
+      <c r="A35" s="1"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75">
+      <c r="A36" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B36" s="21">
+        <f>MATCH(39,C37:C40,1)</f>
+        <v>2</v>
+      </c>
+      <c r="C36" s="21">
+        <v>2</v>
+      </c>
+      <c r="D36" t="str">
+        <f>IF(B36=C36,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" s="1"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" s="1"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75">
+      <c r="A39" s="1"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75">
+      <c r="A40" s="1"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
+      <c r="A41" s="1"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B42" s="7" t="str">
+        <f ca="1">OFFSET(B42,1,0,1,1)</f>
+        <v>offset input</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="D42" t="str">
+        <f ca="1">IF(B42=C42,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75">
+      <c r="A43" s="1"/>
+      <c r="B43" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75">
+      <c r="A44" s="1"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75">
+      <c r="A45" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B45" s="9">
+        <f>ROW()</f>
+        <v>45</v>
+      </c>
+      <c r="C45" s="12">
+        <v>45</v>
+      </c>
+      <c r="D45" t="str">
+        <f>IF(B45=C45,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75">
+      <c r="A46" s="1"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75">
+      <c r="A47" s="1"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75">
+      <c r="A48" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B48" s="12">
+        <f>ROWS(C1:E4)</f>
+        <v>4</v>
+      </c>
+      <c r="C48" s="12">
+        <v>4</v>
+      </c>
+      <c r="D48" t="str">
+        <f>IF(B48=C48,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75">
+      <c r="A49" s="1"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75">
+      <c r="A50" s="1"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75">
+      <c r="A51" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75">
+      <c r="A52" s="1"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75">
+      <c r="A53" s="1"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75">
+      <c r="A54" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B54" s="21"/>
+      <c r="C54" s="30"/>
+      <c r="D54" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75">
+      <c r="A55" s="1"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75">
+      <c r="A56" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B56" s="21">
+        <f>VLOOKUP(1,B57:D59,2)</f>
+        <v>2.93</v>
+      </c>
+      <c r="C56" s="21">
+        <v>2.93</v>
+      </c>
+      <c r="D56" t="str">
+        <f>IF(B56=C56,"T","WARN")</f>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75">
+      <c r="A57" s="1"/>
+      <c r="B57" s="21">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="C57" s="21">
+        <v>3.55</v>
+      </c>
+      <c r="D57">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="B58">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="C58">
+        <v>3.25</v>
+      </c>
+      <c r="D58">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="C59">
+        <v>2.93</v>
+      </c>
+      <c r="D59">
         <v>300</v>
       </c>
-      <c r="D3" t="e">
-        <f ca="1">IF(B3=C3,"T","WARN")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B6" t="e">
-        <f ca="1">USD2NTD(B7,C7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C6">
-        <v>150</v>
-      </c>
-      <c r="D6" t="e">
-        <f ca="1">IF(B6=C6,"T","WARN")</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>414</v>
+      </c>
+      <c r="D61">
+        <f ca="1">COUNTIF(D3:D56,"T")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="B100" s="21"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.75">
+      <c r="A101" s="1"/>
+      <c r="B101" s="21"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.75">
+      <c r="A102" s="1"/>
+      <c r="B102" s="21"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.75">
+      <c r="A103" s="1"/>
+      <c r="B103" s="21"/>
+    </row>
+    <row r="104" spans="1:2" ht="15.75">
+      <c r="A104" s="1"/>
+      <c r="B104" s="21"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.75">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" ht="15.75">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.75">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" ht="15.75">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.75">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.75">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.75">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.75">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.75">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.75">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.75">
+      <c r="A118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.75">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.75">
+      <c r="A120" s="1"/>
+      <c r="B120" s="5"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.75">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.75">
+      <c r="A122" s="1"/>
+      <c r="B122" s="5"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.75">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.75">
+      <c r="A124" s="1"/>
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.75">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.75">
+      <c r="A126" s="1"/>
+      <c r="B126" s="5"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.75">
+      <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.75">
+      <c r="A128" s="1"/>
+      <c r="B128" s="8"/>
+    </row>
+    <row r="129" spans="1:2" ht="15.75">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.75">
+      <c r="A130" s="1"/>
+      <c r="B130" s="5"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.75">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.75">
+      <c r="A132" s="1"/>
+      <c r="B132" s="5"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.75">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.75">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:2" ht="15.75">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:2" ht="15.75">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:2" ht="15.75">
+      <c r="A137" s="1"/>
+      <c r="B137" s="5"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.75">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:2" ht="15.75">
+      <c r="A139" s="1"/>
+      <c r="B139" s="11"/>
+    </row>
+    <row r="140" spans="1:2" ht="15.75">
+      <c r="A140" s="1"/>
+    </row>
+    <row r="141" spans="1:2" ht="15.75">
+      <c r="A141" s="1"/>
+      <c r="B141" s="9"/>
+    </row>
+    <row r="142" spans="1:2" ht="15.75">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:2" ht="15.75">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.75">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:2" ht="15.75">
+      <c r="A145" s="1"/>
+      <c r="B145" s="5"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.75">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.75">
+      <c r="A147" s="1"/>
+      <c r="B147" s="5"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.75">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.75">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:2" ht="15.75">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:2" ht="15.75">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:2" ht="15.75">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.75">
+      <c r="A153" s="1"/>
+      <c r="B153" s="8"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.75">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.75">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:2" ht="15.75">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.75">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:2" ht="15.75">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.75">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.75">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="B162" s="12"/>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="B164" s="8"/>
+    </row>
+    <row r="165" spans="1:2" ht="15.75">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:2" ht="15.75">
+      <c r="A166" s="1"/>
+      <c r="B166" s="5"/>
+    </row>
+    <row r="167" spans="1:2" ht="15.75">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:2" ht="15.75">
+      <c r="A168" s="1"/>
+      <c r="B168" s="11"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.75">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:2" ht="15.75">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:2" ht="15.75">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" spans="1:2" ht="15.75">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" spans="1:2" ht="15.75">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" spans="1:2" ht="15.75">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" spans="1:2" ht="15.75">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" spans="1:2" ht="15.75">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" spans="1:1" ht="15.75">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" spans="1:1" ht="15.75">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" spans="1:1" ht="15.75">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" ht="15.75">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" spans="1:1" ht="15.75">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="182" spans="1:1" ht="15.75">
+      <c r="A182" s="1"/>
+    </row>
+    <row r="183" spans="1:1" ht="15.75">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" spans="1:1" ht="15.75">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" spans="1:1" ht="15.75">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" spans="1:1" ht="15.75">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" spans="1:1" ht="15.75">
+      <c r="A187" s="1"/>
+    </row>
+    <row r="188" spans="1:1" ht="15.75">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" spans="1:1" ht="15.75">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" spans="1:1" ht="15.75">
+      <c r="A190" s="1"/>
+    </row>
+    <row r="191" spans="1:1" ht="15.75">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" spans="1:1" ht="15.75">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" spans="1:2" ht="15.75">
+      <c r="A193" s="1"/>
+    </row>
+    <row r="194" spans="1:2" ht="15.75">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" spans="1:2" ht="15.75">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" spans="1:2" ht="15.75">
+      <c r="A196" s="1"/>
+    </row>
+    <row r="197" spans="1:2" ht="15.75">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" spans="1:2" ht="15.75">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" spans="1:2" ht="15.75">
+      <c r="A199" s="1"/>
+      <c r="B199" s="5"/>
+    </row>
+    <row r="200" spans="1:2" ht="15.75">
+      <c r="A200" s="1"/>
+    </row>
+    <row r="201" spans="1:2" ht="15.75">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" spans="1:2" ht="15.75">
+      <c r="A202" s="1"/>
+      <c r="B202" s="5"/>
+    </row>
+    <row r="203" spans="1:2" ht="15.75">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" spans="1:2" ht="15.75">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:2" ht="15.75">
+      <c r="A205" s="1"/>
+    </row>
+    <row r="206" spans="1:2" ht="15.75">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207" spans="1:2" ht="15.75">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:2" ht="15.75">
+      <c r="A208" s="1"/>
+    </row>
+    <row r="209" spans="1:1" ht="15.75">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210" spans="1:1" ht="15.75">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211" spans="1:1" ht="15.75">
+      <c r="A211" s="1"/>
+    </row>
+    <row r="212" spans="1:1" ht="15.75">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:1" ht="15.75">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:1" ht="15.75">
+      <c r="A214" s="1"/>
+    </row>
+    <row r="215" spans="1:1" ht="15.75">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:1" ht="15.75">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:1" ht="15.75">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:1" ht="15.75">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="219" spans="1:1" ht="15.75">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="220" spans="1:1" ht="15.75">
+      <c r="A220" s="1"/>
+    </row>
+    <row r="221" spans="1:1" ht="15.75">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:1" ht="15.75">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="223" spans="1:1" ht="15.75">
+      <c r="A223" s="1"/>
+    </row>
+    <row r="224" spans="1:1" ht="15.75">
+      <c r="A224" s="1"/>
+    </row>
+    <row r="225" spans="1:2" ht="15.75">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:2" ht="15.75">
+      <c r="A226" s="1"/>
+    </row>
+    <row r="227" spans="1:2" ht="15.75">
+      <c r="A227" s="1"/>
+    </row>
+    <row r="228" spans="1:2" ht="15.75">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:2" ht="15.75">
+      <c r="A229" s="1"/>
+      <c r="B229" s="11"/>
+    </row>
+    <row r="230" spans="1:2" ht="15.75">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:2" ht="15.75">
+      <c r="A231" s="1"/>
+      <c r="B231" s="11"/>
+    </row>
+    <row r="232" spans="1:2" ht="15.75">
+      <c r="A232" s="1"/>
+      <c r="B232" s="11"/>
+    </row>
+    <row r="233" spans="1:2" ht="15.75">
+      <c r="A233" s="1"/>
+      <c r="B233" s="5"/>
+    </row>
+    <row r="234" spans="1:2" ht="15.75">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:2" ht="15.75">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:2" ht="15.75">
+      <c r="A236" s="1"/>
+    </row>
+    <row r="237" spans="1:2" ht="15.75">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:2" ht="15.75">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="239" spans="1:2" ht="15.75">
+      <c r="A239" s="1"/>
+    </row>
+    <row r="240" spans="1:2" ht="15.75">
+      <c r="A240" s="1"/>
+    </row>
+    <row r="241" spans="1:1" ht="15.75">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" ht="15.75">
+      <c r="A242" s="1"/>
+    </row>
+    <row r="243" spans="1:1" ht="15.75">
+      <c r="A243" s="1"/>
+    </row>
+    <row r="244" spans="1:1" ht="15.75">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="245" spans="1:1" ht="15.75">
+      <c r="A245" s="1"/>
+    </row>
+    <row r="246" spans="1:1" ht="15.75">
+      <c r="A246" s="1"/>
+    </row>
+    <row r="247" spans="1:1" ht="15.75">
+      <c r="A247" s="1"/>
+    </row>
+    <row r="248" spans="1:1" ht="15.75">
+      <c r="A248" s="1"/>
+    </row>
+    <row r="249" spans="1:1" ht="15.75">
+      <c r="A249" s="1"/>
+    </row>
+    <row r="250" spans="1:1" ht="15.75">
+      <c r="A250" s="1"/>
+    </row>
+    <row r="251" spans="1:1" ht="15.75">
+      <c r="A251" s="1"/>
+    </row>
+    <row r="252" spans="1:1" ht="15.75">
+      <c r="A252" s="1"/>
+    </row>
+    <row r="253" spans="1:1" ht="15.75">
+      <c r="A253" s="1"/>
+    </row>
+    <row r="254" spans="1:1" ht="15.75">
+      <c r="A254" s="1"/>
+    </row>
+    <row r="255" spans="1:1" ht="15.75">
+      <c r="A255" s="1"/>
+    </row>
+    <row r="256" spans="1:1" ht="15.75">
+      <c r="A256" s="1"/>
+    </row>
+    <row r="257" spans="1:1" ht="15.75">
+      <c r="A257" s="1"/>
+    </row>
+    <row r="258" spans="1:1" ht="15.75">
+      <c r="A258" s="1"/>
+    </row>
+    <row r="259" spans="1:1" ht="15.75">
+      <c r="A259" s="1"/>
+    </row>
+    <row r="260" spans="1:1" ht="15.75">
+      <c r="A260" s="1"/>
+    </row>
+    <row r="261" spans="1:1" ht="15.75">
+      <c r="A261" s="1"/>
+    </row>
+    <row r="262" spans="1:1" ht="15.75">
+      <c r="A262" s="1"/>
+    </row>
+    <row r="263" spans="1:1" ht="15.75">
+      <c r="A263" s="1"/>
+    </row>
+    <row r="264" spans="1:1" ht="15.75">
+      <c r="A264" s="1"/>
+    </row>
+    <row r="265" spans="1:1" ht="15.75">
+      <c r="A265" s="1"/>
+    </row>
+    <row r="266" spans="1:1" ht="15.75">
+      <c r="A266" s="1"/>
+    </row>
+    <row r="267" spans="1:1" ht="15.75">
+      <c r="A267" s="1"/>
+    </row>
+    <row r="268" spans="1:1" ht="15.75">
+      <c r="A268" s="1"/>
+    </row>
+    <row r="269" spans="1:1" ht="15.75">
+      <c r="A269" s="1"/>
+    </row>
+    <row r="270" spans="1:1" ht="15.75">
+      <c r="A270" s="1"/>
+    </row>
+    <row r="271" spans="1:1" ht="15.75">
+      <c r="A271" s="1"/>
+    </row>
+    <row r="272" spans="1:1" ht="15.75">
+      <c r="A272" s="1"/>
+    </row>
+    <row r="273" spans="1:1" ht="15.75">
+      <c r="A273" s="1"/>
+    </row>
+    <row r="274" spans="1:1" ht="15.75">
+      <c r="A274" s="1"/>
+    </row>
+    <row r="275" spans="1:1" ht="15.75">
+      <c r="A275" s="1"/>
+    </row>
+    <row r="276" spans="1:1" ht="15.75">
+      <c r="A276" s="1"/>
+    </row>
+    <row r="277" spans="1:1" ht="15.75">
+      <c r="A277" s="1"/>
+    </row>
+    <row r="278" spans="1:1" ht="15.75">
+      <c r="A278" s="1"/>
+    </row>
+    <row r="279" spans="1:1" ht="15.75">
+      <c r="A279" s="1"/>
+    </row>
+    <row r="280" spans="1:1" ht="15.75">
+      <c r="A280" s="1"/>
+    </row>
+    <row r="281" spans="1:1" ht="15.75">
+      <c r="A281" s="1"/>
+    </row>
+    <row r="282" spans="1:1" ht="15.75">
+      <c r="A282" s="1"/>
+    </row>
+    <row r="283" spans="1:1" ht="15.75">
+      <c r="A283" s="1"/>
+    </row>
+    <row r="284" spans="1:1" ht="15.75">
+      <c r="A284" s="1"/>
+    </row>
+    <row r="285" spans="1:1" ht="15.75">
+      <c r="A285" s="1"/>
+    </row>
+    <row r="286" spans="1:1" ht="15.75">
+      <c r="A286" s="1"/>
+    </row>
+    <row r="287" spans="1:1" ht="15.75">
+      <c r="A287" s="1"/>
+    </row>
+    <row r="288" spans="1:1" ht="15.75">
+      <c r="A288" s="1"/>
+    </row>
+    <row r="289" spans="1:1" ht="15.75">
+      <c r="A289" s="1"/>
+    </row>
+    <row r="290" spans="1:1" ht="15.75">
+      <c r="A290" s="1"/>
+    </row>
+    <row r="291" spans="1:1" ht="15.75">
+      <c r="A291" s="1"/>
+    </row>
+    <row r="293" spans="1:1" ht="15.75">
+      <c r="A293" s="1"/>
+    </row>
+    <row r="522" spans="1:1">
+      <c r="A522" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
-      <formula>"WARN"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="D3 D7:D8 D10 D12 D14 D20 D22:D24 D26 D29:D34 D36:D40 D42:D43 D45:D46 D48:D49 D56 D5 D51:D52 D54">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B36" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -7798,12 +9115,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="200" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8701,7 +10018,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>28.290524368504009</v>
+        <v>91.367089526201411</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -8719,7 +10036,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -9600,7 +10917,7 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="198" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9810,7 +11127,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10976,7 +12293,7 @@
     <sortCondition ref="A5"/>
   </sortState>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11957,17 +13274,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D15 D18 D21 D23 D26 D29 D31 D8:D12">
-    <cfRule type="cellIs" dxfId="195" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33 D35 D38 D41 D43">
-    <cfRule type="cellIs" dxfId="194" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="193" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12379,7 +13696,7 @@
       </c>
       <c r="B34" s="20">
         <f ca="1">NOW()</f>
-        <v>41499.618067129632</v>
+        <v>41500.485210995372</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75">
@@ -12450,7 +13767,7 @@
       </c>
       <c r="B42" s="19">
         <f ca="1">TODAY()</f>
-        <v>41499</v>
+        <v>41500</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75">
@@ -13314,7 +14631,7 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D10 D13 D15 D17 D36 D38 D44 D61 D40 D63:D65 D46:D58 D19:D32">
-    <cfRule type="cellIs" dxfId="192" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13328,7 +14645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
@@ -15383,67 +16700,67 @@
     <sortCondition ref="A40"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D9 D12">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15 D18 D21 D24 D27 D30 D33">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 D39 D42 D45 D47 D49 D51">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54 D57 D59 D62 D64 D67 D70 D73">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78 D81 D84 D87 D89 D91 D93 D95 D97 D102 D104 D106 D108 D110 D99:D100">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D115 D117 D119 D123 D125 D127">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15457,8 +16774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18846,747 +20163,747 @@
     <sortCondition ref="D50"/>
   </sortState>
   <conditionalFormatting sqref="D3 D6 D8 D11 D21 D23 D25 D14 D17 D19 D27">
-    <cfRule type="cellIs" dxfId="191" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="149" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35 D41 D43 D45 D47 D37 D50">
-    <cfRule type="cellIs" dxfId="190" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="148" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53 D55 D57 D59 D61 D63 D65 D67">
-    <cfRule type="cellIs" dxfId="189" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="147" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70 D73 D76 D78 D80 D82">
-    <cfRule type="cellIs" dxfId="188" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="146" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85 D89 D92 D94 D100 D106 D108">
-    <cfRule type="cellIs" dxfId="187" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="145" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110 D112 D114 D116 D118">
-    <cfRule type="cellIs" dxfId="186" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="144" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D121 D123 D125 D127 D142 D129 D131 D133 D136 D138 D140 D144">
-    <cfRule type="cellIs" dxfId="185" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="143" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147 D149 D151">
-    <cfRule type="cellIs" dxfId="184" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="142" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D154 D156 D162">
-    <cfRule type="cellIs" dxfId="183" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="141" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D159">
-    <cfRule type="cellIs" dxfId="182" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="140" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D164 D166 D170 D172 D168">
-    <cfRule type="cellIs" dxfId="181" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="139" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D175 D177 D179 D183 D186">
-    <cfRule type="cellIs" dxfId="180" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="138" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D189 D191 D193 D195 D197 D199">
-    <cfRule type="cellIs" dxfId="179" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="137" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="178" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="136" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="177" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="135" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="176" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="134" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="175" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="133" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="174" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="132" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="173" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="131" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="172" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="130" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="171" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="129" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="170" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="128" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="169" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="127" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="168" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="126" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="cellIs" dxfId="167" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="125" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="166" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="124" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="165" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="123" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70">
-    <cfRule type="cellIs" dxfId="164" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="122" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="163" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="121" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="162" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="120" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="cellIs" dxfId="161" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="119" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="160" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="118" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="159" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="117" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="cellIs" dxfId="158" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="116" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="157" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="115" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="156" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="114" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="155" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="113" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106">
-    <cfRule type="cellIs" dxfId="154" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="112" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="153" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="111" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="152" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="110" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="151" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="109" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108">
-    <cfRule type="cellIs" dxfId="150" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="108" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="149" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="107" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="148" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="106" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="147" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="105" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="146" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="104" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="145" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="103" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="144" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="102" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="143" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="101" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D127">
-    <cfRule type="cellIs" dxfId="142" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="100" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="141" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="99" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="140" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="98" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="139" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="97" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D129">
-    <cfRule type="cellIs" dxfId="138" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="96" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="137" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="95" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="136" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="94" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="135" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="93" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D131">
-    <cfRule type="cellIs" dxfId="134" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="92" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="133" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="91" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="132" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="90" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="131" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="89" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D133">
-    <cfRule type="cellIs" dxfId="130" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="88" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="129" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="87" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="128" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="86" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="127" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="85" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136">
-    <cfRule type="cellIs" dxfId="126" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="84" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="125" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="83" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="124" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="82" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="123" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="81" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="cellIs" dxfId="122" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="80" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="121" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="79" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="120" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="78" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="119" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="77" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D140">
-    <cfRule type="cellIs" dxfId="118" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="76" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="117" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="75" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="116" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="74" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="115" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="73" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="cellIs" dxfId="114" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="72" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="113" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="71" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="112" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="70" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="111" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="69" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="110" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="68" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D147">
-    <cfRule type="cellIs" dxfId="109" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="67" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="108" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="66" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="107" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="65" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="106" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="64" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="105" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="63" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D151">
-    <cfRule type="cellIs" dxfId="104" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="62" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="103" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="61" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="102" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="60" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="101" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="59" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="100" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="58" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162">
-    <cfRule type="cellIs" dxfId="99" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="57" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="98" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="56" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="97" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="55" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="96" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="54" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="95" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="53" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D170">
-    <cfRule type="cellIs" dxfId="94" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="52" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="93" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="51" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="92" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="50" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="91" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="49" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="90" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="48" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D172">
-    <cfRule type="cellIs" dxfId="89" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="47" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="88" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="46" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="87" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="45" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="86" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="44" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="85" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="43" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D179">
-    <cfRule type="cellIs" dxfId="84" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="42" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="83" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="41" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="82" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="81" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="39" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="80" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="38" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D183">
-    <cfRule type="cellIs" dxfId="79" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="37" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="78" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="36" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="77" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="35" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="76" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="34" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="75" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="33" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D186">
-    <cfRule type="cellIs" dxfId="74" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="32" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="73" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="31" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="72" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="30" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="71" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="29" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="70" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="28" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191">
-    <cfRule type="cellIs" dxfId="69" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="27" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="68" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="26" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="67" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="25" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="66" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="65" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="23" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="cellIs" dxfId="64" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="63" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="20" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="61" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="19" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="60" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="18" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="17" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="16" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="15" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="cellIs" dxfId="55" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="54" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="53" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="52" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D94">
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="50" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D166">
-    <cfRule type="cellIs" dxfId="47" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D168">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>